<commit_message>
Implemented the ability to save new Individual report.
</commit_message>
<xml_diff>
--- a/PaymentsBudgetSystem/wwwroot/Report.xlsx
+++ b/PaymentsBudgetSystem/wwwroot/Report.xlsx
@@ -817,7 +817,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1512">
   <si>
     <t>Временни безлихвени заеми от/за държавни предприятия и други сметки, включени в консолидираната фискална програма (нето)</t>
   </si>
@@ -8100,6 +8100,39 @@
   </si>
   <si>
     <t>Наименование разпоредителя с бюджет</t>
+  </si>
+  <si>
+    <t>здравно-осигурителни вноски</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">вноски за </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman Cyr"/>
+        <family val="1"/>
+      </rPr>
+      <t>допълнително задължително осигуряване</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">осигурителни вноски за </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman Cyr"/>
+        <family val="1"/>
+      </rPr>
+      <t>Държавното обществено осигуряване (ДОО)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -12986,261 +13019,10 @@
     <xf numFmtId="3" fontId="13" fillId="12" borderId="102" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -13263,9 +13045,290 @@
     <xf numFmtId="0" fontId="45" fillId="5" borderId="114" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="16" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="16" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="20" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -13273,48 +13336,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="16" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="151" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="151" fillId="16" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="152" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="152" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="152" fillId="20" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -13340,6 +13364,9 @@
     </xf>
     <xf numFmtId="0" fontId="149" fillId="20" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -13355,9 +13382,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -13374,7 +13407,7 @@
     <cellStyle name="Normal_MAKET" xfId="9"/>
     <cellStyle name="Normal_Sheet2" xfId="10"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="41">
     <dxf>
       <font>
         <color rgb="FF660066"/>
@@ -13559,18 +13592,6 @@
           <bgColor rgb="FFF0FDCF"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="0000&quot; &quot;0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0000&quot; &quot;0000&quot; &quot;0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="0000&quot; &quot;0000&quot; &quot;0000&quot; &quot;0000"/>
     </dxf>
     <dxf>
       <font>
@@ -14422,12 +14443,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="42" customHeight="1">
-      <c r="B7" s="776" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="777"/>
-      <c r="D7" s="777"/>
+      <c r="B7" s="691" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C7" s="692"/>
+      <c r="D7" s="692"/>
       <c r="F7" s="38"/>
       <c r="K7" s="167">
         <v>1</v>
@@ -14447,12 +14468,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="36.75" customHeight="1" thickBot="1">
-      <c r="B9" s="778" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="779"/>
-      <c r="D9" s="779"/>
+      <c r="B9" s="693" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="694"/>
+      <c r="D9" s="694"/>
       <c r="E9" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14487,12 +14508,12 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="39" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B12" s="778" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C12" s="779"/>
-      <c r="D12" s="779"/>
+      <c r="B12" s="693" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C12" s="694"/>
+      <c r="D12" s="694"/>
       <c r="E12" s="38" t="s">
         <v>505</v>
       </c>
@@ -14567,10 +14588,10 @@
     <row r="19" spans="1:11" ht="21.75" thickBot="1">
       <c r="A19" s="46"/>
       <c r="B19" s="47"/>
-      <c r="C19" s="782" t="s">
+      <c r="C19" s="699" t="s">
         <v>508</v>
       </c>
-      <c r="D19" s="698"/>
+      <c r="D19" s="700"/>
       <c r="E19" s="48" t="s">
         <v>509</v>
       </c>
@@ -14589,10 +14610,10 @@
       <c r="B20" s="49" t="s">
         <v>474</v>
       </c>
-      <c r="C20" s="697" t="s">
+      <c r="C20" s="701" t="s">
         <v>705</v>
       </c>
-      <c r="D20" s="696"/>
+      <c r="D20" s="702"/>
       <c r="E20" s="50">
         <v>2017</v>
       </c>
@@ -14617,10 +14638,10 @@
     </row>
     <row r="21" spans="1:11" ht="21.75" thickBot="1">
       <c r="B21" s="51"/>
-      <c r="C21" s="693" t="s">
+      <c r="C21" s="779" t="s">
         <v>512</v>
       </c>
-      <c r="D21" s="694"/>
+      <c r="D21" s="749"/>
       <c r="E21" s="10" t="s">
         <v>263</v>
       </c>
@@ -14650,10 +14671,10 @@
       <c r="B22" s="54">
         <v>100</v>
       </c>
-      <c r="C22" s="780" t="s">
+      <c r="C22" s="695" t="s">
         <v>513</v>
       </c>
-      <c r="D22" s="781"/>
+      <c r="D22" s="696"/>
       <c r="E22" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14690,10 +14711,10 @@
       <c r="B23" s="57">
         <v>200</v>
       </c>
-      <c r="C23" s="729" t="s">
+      <c r="C23" s="689" t="s">
         <v>514</v>
       </c>
-      <c r="D23" s="730"/>
+      <c r="D23" s="690"/>
       <c r="E23" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14730,10 +14751,10 @@
       <c r="B24" s="57">
         <v>400</v>
       </c>
-      <c r="C24" s="709" t="s">
+      <c r="C24" s="697" t="s">
         <v>515</v>
       </c>
-      <c r="D24" s="744"/>
+      <c r="D24" s="698"/>
       <c r="E24" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14770,10 +14791,10 @@
       <c r="B25" s="57">
         <v>800</v>
       </c>
-      <c r="C25" s="729" t="s">
+      <c r="C25" s="689" t="s">
         <v>924</v>
       </c>
-      <c r="D25" s="730"/>
+      <c r="D25" s="690"/>
       <c r="E25" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14810,10 +14831,10 @@
       <c r="B26" s="57">
         <v>1000</v>
       </c>
-      <c r="C26" s="729" t="s">
+      <c r="C26" s="689" t="s">
         <v>516</v>
       </c>
-      <c r="D26" s="730"/>
+      <c r="D26" s="690"/>
       <c r="E26" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14850,10 +14871,10 @@
       <c r="B27" s="57">
         <v>1300</v>
       </c>
-      <c r="C27" s="729" t="s">
+      <c r="C27" s="689" t="s">
         <v>706</v>
       </c>
-      <c r="D27" s="730"/>
+      <c r="D27" s="690"/>
       <c r="E27" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14890,10 +14911,10 @@
       <c r="B28" s="57">
         <v>1400</v>
       </c>
-      <c r="C28" s="729" t="s">
+      <c r="C28" s="689" t="s">
         <v>517</v>
       </c>
-      <c r="D28" s="730"/>
+      <c r="D28" s="690"/>
       <c r="E28" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14930,10 +14951,10 @@
       <c r="B29" s="57">
         <v>1500</v>
       </c>
-      <c r="C29" s="729" t="s">
+      <c r="C29" s="689" t="s">
         <v>518</v>
       </c>
-      <c r="D29" s="730"/>
+      <c r="D29" s="690"/>
       <c r="E29" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14967,10 +14988,10 @@
       <c r="B30" s="57">
         <v>1600</v>
       </c>
-      <c r="C30" s="729" t="s">
+      <c r="C30" s="689" t="s">
         <v>519</v>
       </c>
-      <c r="D30" s="730"/>
+      <c r="D30" s="690"/>
       <c r="E30" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15007,10 +15028,10 @@
       <c r="B31" s="57">
         <v>1700</v>
       </c>
-      <c r="C31" s="729" t="s">
+      <c r="C31" s="689" t="s">
         <v>520</v>
       </c>
-      <c r="D31" s="730"/>
+      <c r="D31" s="690"/>
       <c r="E31" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15047,10 +15068,10 @@
       <c r="B32" s="57">
         <v>1800</v>
       </c>
-      <c r="C32" s="729" t="s">
+      <c r="C32" s="689" t="s">
         <v>521</v>
       </c>
-      <c r="D32" s="730"/>
+      <c r="D32" s="690"/>
       <c r="E32" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15087,10 +15108,10 @@
       <c r="B33" s="57">
         <v>1900</v>
       </c>
-      <c r="C33" s="729" t="s">
+      <c r="C33" s="689" t="s">
         <v>522</v>
       </c>
-      <c r="D33" s="730"/>
+      <c r="D33" s="690"/>
       <c r="E33" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15127,10 +15148,10 @@
       <c r="B34" s="57">
         <v>2000</v>
       </c>
-      <c r="C34" s="729" t="s">
+      <c r="C34" s="689" t="s">
         <v>523</v>
       </c>
-      <c r="D34" s="730"/>
+      <c r="D34" s="690"/>
       <c r="E34" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15167,10 +15188,10 @@
       <c r="B35" s="57">
         <v>2400</v>
       </c>
-      <c r="C35" s="729" t="s">
+      <c r="C35" s="689" t="s">
         <v>524</v>
       </c>
-      <c r="D35" s="730"/>
+      <c r="D35" s="690"/>
       <c r="E35" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15207,10 +15228,10 @@
       <c r="B36" s="62">
         <v>2500</v>
       </c>
-      <c r="C36" s="723" t="s">
+      <c r="C36" s="707" t="s">
         <v>525</v>
       </c>
-      <c r="D36" s="724"/>
+      <c r="D36" s="708"/>
       <c r="E36" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15247,10 +15268,10 @@
       <c r="B37" s="57">
         <v>2600</v>
       </c>
-      <c r="C37" s="723" t="s">
+      <c r="C37" s="707" t="s">
         <v>300</v>
       </c>
-      <c r="D37" s="724"/>
+      <c r="D37" s="708"/>
       <c r="E37" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15287,10 +15308,10 @@
       <c r="B38" s="57">
         <v>2700</v>
       </c>
-      <c r="C38" s="729" t="s">
+      <c r="C38" s="689" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="730"/>
+      <c r="D38" s="690"/>
       <c r="E38" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15327,10 +15348,10 @@
       <c r="B39" s="57">
         <v>2800</v>
       </c>
-      <c r="C39" s="729" t="s">
+      <c r="C39" s="689" t="s">
         <v>529</v>
       </c>
-      <c r="D39" s="730"/>
+      <c r="D39" s="690"/>
       <c r="E39" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15367,10 +15388,10 @@
       <c r="B40" s="57">
         <v>3600</v>
       </c>
-      <c r="C40" s="729" t="s">
+      <c r="C40" s="689" t="s">
         <v>530</v>
       </c>
-      <c r="D40" s="730"/>
+      <c r="D40" s="690"/>
       <c r="E40" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15407,10 +15428,10 @@
       <c r="B41" s="57">
         <v>3700</v>
       </c>
-      <c r="C41" s="729" t="s">
+      <c r="C41" s="689" t="s">
         <v>531</v>
       </c>
-      <c r="D41" s="730"/>
+      <c r="D41" s="690"/>
       <c r="E41" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15501,10 +15522,10 @@
       <c r="B43" s="57">
         <v>4100</v>
       </c>
-      <c r="C43" s="729" t="s">
+      <c r="C43" s="689" t="s">
         <v>381</v>
       </c>
-      <c r="D43" s="730"/>
+      <c r="D43" s="690"/>
       <c r="E43" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15542,10 +15563,10 @@
       <c r="B44" s="57">
         <v>4200</v>
       </c>
-      <c r="C44" s="729" t="s">
+      <c r="C44" s="689" t="s">
         <v>382</v>
       </c>
-      <c r="D44" s="730"/>
+      <c r="D44" s="690"/>
       <c r="E44" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15583,10 +15604,10 @@
       <c r="B45" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="C45" s="729" t="s">
+      <c r="C45" s="689" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="730"/>
+      <c r="D45" s="690"/>
       <c r="E45" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15624,10 +15645,10 @@
       <c r="B46" s="57">
         <v>4600</v>
       </c>
-      <c r="C46" s="729" t="s">
+      <c r="C46" s="689" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="730"/>
+      <c r="D46" s="690"/>
       <c r="E46" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15664,10 +15685,10 @@
       <c r="B47" s="57">
         <v>4700</v>
       </c>
-      <c r="C47" s="729" t="s">
+      <c r="C47" s="689" t="s">
         <v>1410</v>
       </c>
-      <c r="D47" s="730"/>
+      <c r="D47" s="690"/>
       <c r="E47" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15704,10 +15725,10 @@
       <c r="B48" s="57">
         <v>4800</v>
       </c>
-      <c r="C48" s="774" t="s">
+      <c r="C48" s="703" t="s">
         <v>455</v>
       </c>
-      <c r="D48" s="775"/>
+      <c r="D48" s="704"/>
       <c r="E48" s="202" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15836,12 +15857,12 @@
       <c r="L53" s="74"/>
     </row>
     <row r="54" spans="1:15" s="46" customFormat="1" ht="44.25" customHeight="1">
-      <c r="B54" s="689" t="e">
+      <c r="B54" s="705" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C54" s="690"/>
-      <c r="D54" s="690"/>
+      <c r="C54" s="706"/>
+      <c r="D54" s="706"/>
       <c r="E54" s="79"/>
       <c r="F54" s="79"/>
       <c r="G54" s="30"/>
@@ -15873,12 +15894,12 @@
       <c r="L55" s="74"/>
     </row>
     <row r="56" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickBot="1">
-      <c r="B56" s="691" t="e">
+      <c r="B56" s="721" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C56" s="692"/>
-      <c r="D56" s="692"/>
+      <c r="C56" s="722"/>
+      <c r="D56" s="722"/>
       <c r="E56" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -15933,12 +15954,12 @@
       <c r="L58" s="74"/>
     </row>
     <row r="59" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B59" s="691" t="e">
+      <c r="B59" s="721" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C59" s="692"/>
-      <c r="D59" s="692"/>
+      <c r="C59" s="722"/>
+      <c r="D59" s="722"/>
       <c r="E59" s="79" t="s">
         <v>505</v>
       </c>
@@ -16009,10 +16030,10 @@
     </row>
     <row r="63" spans="1:15" s="46" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="B63" s="87"/>
-      <c r="C63" s="770" t="s">
+      <c r="C63" s="717" t="s">
         <v>473</v>
       </c>
-      <c r="D63" s="771"/>
+      <c r="D63" s="718"/>
       <c r="E63" s="48" t="s">
         <v>509</v>
       </c>
@@ -16026,16 +16047,16 @@
       <c r="K63" s="169">
         <v>1</v>
       </c>
-      <c r="L63" s="764" t="s">
+      <c r="L63" s="709" t="s">
         <v>1429</v>
       </c>
-      <c r="M63" s="764" t="s">
+      <c r="M63" s="709" t="s">
         <v>1430</v>
       </c>
-      <c r="N63" s="764" t="s">
+      <c r="N63" s="709" t="s">
         <v>1431</v>
       </c>
-      <c r="O63" s="764" t="s">
+      <c r="O63" s="709" t="s">
         <v>1432</v>
       </c>
     </row>
@@ -16043,10 +16064,10 @@
       <c r="B64" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="C64" s="697" t="s">
+      <c r="C64" s="701" t="s">
         <v>707</v>
       </c>
-      <c r="D64" s="767"/>
+      <c r="D64" s="714"/>
       <c r="E64" s="50">
         <v>2017</v>
       </c>
@@ -16068,17 +16089,17 @@
       <c r="K64" s="169">
         <v>1</v>
       </c>
-      <c r="L64" s="772"/>
-      <c r="M64" s="772"/>
-      <c r="N64" s="765"/>
-      <c r="O64" s="765"/>
+      <c r="L64" s="723"/>
+      <c r="M64" s="723"/>
+      <c r="N64" s="710"/>
+      <c r="O64" s="710"/>
     </row>
     <row r="65" spans="1:15" s="46" customFormat="1" ht="21.75" thickBot="1">
       <c r="B65" s="88"/>
-      <c r="C65" s="768" t="s">
+      <c r="C65" s="715" t="s">
         <v>387</v>
       </c>
-      <c r="D65" s="769"/>
+      <c r="D65" s="716"/>
       <c r="E65" s="10" t="s">
         <v>263</v>
       </c>
@@ -16100,10 +16121,10 @@
       <c r="K65" s="169">
         <v>1</v>
       </c>
-      <c r="L65" s="773"/>
-      <c r="M65" s="773"/>
-      <c r="N65" s="766"/>
-      <c r="O65" s="766"/>
+      <c r="L65" s="724"/>
+      <c r="M65" s="724"/>
+      <c r="N65" s="711"/>
+      <c r="O65" s="711"/>
     </row>
     <row r="66" spans="1:15" s="56" customFormat="1" ht="34.5" customHeight="1">
       <c r="A66" s="63">
@@ -16112,10 +16133,10 @@
       <c r="B66" s="54">
         <v>100</v>
       </c>
-      <c r="C66" s="752" t="s">
+      <c r="C66" s="725" t="s">
         <v>388</v>
       </c>
-      <c r="D66" s="737"/>
+      <c r="D66" s="726"/>
       <c r="E66" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16156,10 +16177,10 @@
       <c r="B67" s="57">
         <v>200</v>
       </c>
-      <c r="C67" s="723" t="s">
+      <c r="C67" s="707" t="s">
         <v>391</v>
       </c>
-      <c r="D67" s="724"/>
+      <c r="D67" s="708"/>
       <c r="E67" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16200,10 +16221,10 @@
       <c r="B68" s="57">
         <v>500</v>
       </c>
-      <c r="C68" s="729" t="s">
+      <c r="C68" s="689" t="s">
         <v>579</v>
       </c>
-      <c r="D68" s="730"/>
+      <c r="D68" s="690"/>
       <c r="E68" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16244,10 +16265,10 @@
       <c r="B69" s="57">
         <v>800</v>
       </c>
-      <c r="C69" s="709" t="s">
+      <c r="C69" s="697" t="s">
         <v>585</v>
       </c>
-      <c r="D69" s="700"/>
+      <c r="D69" s="727"/>
       <c r="E69" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16288,10 +16309,10 @@
       <c r="B70" s="57">
         <v>1000</v>
       </c>
-      <c r="C70" s="723" t="s">
+      <c r="C70" s="707" t="s">
         <v>586</v>
       </c>
-      <c r="D70" s="724"/>
+      <c r="D70" s="708"/>
       <c r="E70" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16332,10 +16353,10 @@
       <c r="B71" s="57">
         <v>1900</v>
       </c>
-      <c r="C71" s="703" t="s">
+      <c r="C71" s="719" t="s">
         <v>456</v>
       </c>
-      <c r="D71" s="704"/>
+      <c r="D71" s="720"/>
       <c r="E71" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16376,10 +16397,10 @@
       <c r="B72" s="57">
         <v>2100</v>
       </c>
-      <c r="C72" s="703" t="s">
+      <c r="C72" s="719" t="s">
         <v>741</v>
       </c>
-      <c r="D72" s="704"/>
+      <c r="D72" s="720"/>
       <c r="E72" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16420,10 +16441,10 @@
       <c r="B73" s="57">
         <v>2200</v>
       </c>
-      <c r="C73" s="703" t="s">
+      <c r="C73" s="719" t="s">
         <v>604</v>
       </c>
-      <c r="D73" s="704"/>
+      <c r="D73" s="720"/>
       <c r="E73" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16464,10 +16485,10 @@
       <c r="B74" s="57">
         <v>2500</v>
       </c>
-      <c r="C74" s="703" t="s">
+      <c r="C74" s="719" t="s">
         <v>606</v>
       </c>
-      <c r="D74" s="704"/>
+      <c r="D74" s="720"/>
       <c r="E74" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16508,10 +16529,10 @@
       <c r="B75" s="57">
         <v>2600</v>
       </c>
-      <c r="C75" s="731" t="s">
+      <c r="C75" s="712" t="s">
         <v>607</v>
       </c>
-      <c r="D75" s="726"/>
+      <c r="D75" s="713"/>
       <c r="E75" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16552,10 +16573,10 @@
       <c r="B76" s="57">
         <v>2700</v>
       </c>
-      <c r="C76" s="731" t="s">
+      <c r="C76" s="712" t="s">
         <v>608</v>
       </c>
-      <c r="D76" s="726"/>
+      <c r="D76" s="713"/>
       <c r="E76" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16596,10 +16617,10 @@
       <c r="B77" s="57">
         <v>2800</v>
       </c>
-      <c r="C77" s="731" t="s">
+      <c r="C77" s="712" t="s">
         <v>1408</v>
       </c>
-      <c r="D77" s="726"/>
+      <c r="D77" s="713"/>
       <c r="E77" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16640,10 +16661,10 @@
       <c r="B78" s="57">
         <v>2900</v>
       </c>
-      <c r="C78" s="703" t="s">
+      <c r="C78" s="719" t="s">
         <v>609</v>
       </c>
-      <c r="D78" s="704"/>
+      <c r="D78" s="720"/>
       <c r="E78" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16728,10 +16749,10 @@
       <c r="B80" s="57">
         <v>3900</v>
       </c>
-      <c r="C80" s="703" t="s">
+      <c r="C80" s="719" t="s">
         <v>618</v>
       </c>
-      <c r="D80" s="704"/>
+      <c r="D80" s="720"/>
       <c r="E80" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16772,10 +16793,10 @@
       <c r="B81" s="57">
         <v>4000</v>
       </c>
-      <c r="C81" s="703" t="s">
+      <c r="C81" s="719" t="s">
         <v>619</v>
       </c>
-      <c r="D81" s="704"/>
+      <c r="D81" s="720"/>
       <c r="E81" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16816,10 +16837,10 @@
       <c r="B82" s="57">
         <v>4100</v>
       </c>
-      <c r="C82" s="703" t="s">
+      <c r="C82" s="719" t="s">
         <v>620</v>
       </c>
-      <c r="D82" s="704"/>
+      <c r="D82" s="720"/>
       <c r="E82" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16860,10 +16881,10 @@
       <c r="B83" s="57">
         <v>4200</v>
       </c>
-      <c r="C83" s="703" t="s">
+      <c r="C83" s="719" t="s">
         <v>621</v>
       </c>
-      <c r="D83" s="704"/>
+      <c r="D83" s="720"/>
       <c r="E83" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16904,10 +16925,10 @@
       <c r="B84" s="57">
         <v>4300</v>
       </c>
-      <c r="C84" s="703" t="s">
+      <c r="C84" s="719" t="s">
         <v>1015</v>
       </c>
-      <c r="D84" s="704"/>
+      <c r="D84" s="720"/>
       <c r="E84" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16948,10 +16969,10 @@
       <c r="B85" s="57">
         <v>4400</v>
       </c>
-      <c r="C85" s="703" t="s">
+      <c r="C85" s="719" t="s">
         <v>1012</v>
       </c>
-      <c r="D85" s="704"/>
+      <c r="D85" s="720"/>
       <c r="E85" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16992,10 +17013,10 @@
       <c r="B86" s="57">
         <v>4500</v>
       </c>
-      <c r="C86" s="703" t="s">
+      <c r="C86" s="719" t="s">
         <v>1409</v>
       </c>
-      <c r="D86" s="704"/>
+      <c r="D86" s="720"/>
       <c r="E86" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17036,10 +17057,10 @@
       <c r="B87" s="57">
         <v>4600</v>
       </c>
-      <c r="C87" s="731" t="s">
+      <c r="C87" s="712" t="s">
         <v>630</v>
       </c>
-      <c r="D87" s="726"/>
+      <c r="D87" s="713"/>
       <c r="E87" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17080,10 +17101,10 @@
       <c r="B88" s="57">
         <v>4900</v>
       </c>
-      <c r="C88" s="703" t="s">
+      <c r="C88" s="719" t="s">
         <v>460</v>
       </c>
-      <c r="D88" s="704"/>
+      <c r="D88" s="720"/>
       <c r="E88" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17124,10 +17145,10 @@
       <c r="B89" s="96">
         <v>5100</v>
       </c>
-      <c r="C89" s="757" t="s">
+      <c r="C89" s="728" t="s">
         <v>631</v>
       </c>
-      <c r="D89" s="758"/>
+      <c r="D89" s="729"/>
       <c r="E89" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17168,10 +17189,10 @@
       <c r="B90" s="96">
         <v>5200</v>
       </c>
-      <c r="C90" s="757" t="s">
+      <c r="C90" s="728" t="s">
         <v>632</v>
       </c>
-      <c r="D90" s="758"/>
+      <c r="D90" s="729"/>
       <c r="E90" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17212,10 +17233,10 @@
       <c r="B91" s="96">
         <v>5300</v>
       </c>
-      <c r="C91" s="757" t="s">
+      <c r="C91" s="728" t="s">
         <v>191</v>
       </c>
-      <c r="D91" s="758"/>
+      <c r="D91" s="729"/>
       <c r="E91" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17256,10 +17277,10 @@
       <c r="B92" s="96">
         <v>5400</v>
       </c>
-      <c r="C92" s="757" t="s">
+      <c r="C92" s="728" t="s">
         <v>643</v>
       </c>
-      <c r="D92" s="758"/>
+      <c r="D92" s="729"/>
       <c r="E92" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17300,10 +17321,10 @@
       <c r="B93" s="57">
         <v>5500</v>
       </c>
-      <c r="C93" s="703" t="s">
+      <c r="C93" s="719" t="s">
         <v>644</v>
       </c>
-      <c r="D93" s="704"/>
+      <c r="D93" s="720"/>
       <c r="E93" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17344,10 +17365,10 @@
       <c r="B94" s="96">
         <v>5700</v>
       </c>
-      <c r="C94" s="759" t="s">
+      <c r="C94" s="730" t="s">
         <v>649</v>
       </c>
-      <c r="D94" s="760"/>
+      <c r="D94" s="731"/>
       <c r="E94" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17388,10 +17409,10 @@
       <c r="B95" s="98" t="s">
         <v>708</v>
       </c>
-      <c r="C95" s="761" t="s">
+      <c r="C95" s="732" t="s">
         <v>653</v>
       </c>
-      <c r="D95" s="762"/>
+      <c r="D95" s="733"/>
       <c r="E95" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17430,10 +17451,10 @@
         <v>825</v>
       </c>
       <c r="B96" s="104"/>
-      <c r="C96" s="763" t="s">
+      <c r="C96" s="734" t="s">
         <v>654</v>
       </c>
-      <c r="D96" s="763"/>
+      <c r="D96" s="734"/>
       <c r="E96" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17499,12 +17520,12 @@
     </row>
     <row r="99" spans="1:11" ht="40.5" customHeight="1">
       <c r="A99" s="70"/>
-      <c r="B99" s="689" t="e">
+      <c r="B99" s="705" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C99" s="690"/>
-      <c r="D99" s="690"/>
+      <c r="C99" s="706"/>
+      <c r="D99" s="706"/>
       <c r="E99" s="79"/>
       <c r="F99" s="79"/>
       <c r="K99" s="167">
@@ -17527,12 +17548,12 @@
     </row>
     <row r="101" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A101" s="70"/>
-      <c r="B101" s="691" t="e">
+      <c r="B101" s="721" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C101" s="692"/>
-      <c r="D101" s="692"/>
+      <c r="C101" s="722"/>
+      <c r="D101" s="722"/>
       <c r="E101" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -17571,12 +17592,12 @@
     </row>
     <row r="104" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A104" s="70"/>
-      <c r="B104" s="691" t="e">
+      <c r="B104" s="721" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C104" s="692"/>
-      <c r="D104" s="692"/>
+      <c r="C104" s="722"/>
+      <c r="D104" s="722"/>
       <c r="E104" s="79" t="s">
         <v>505</v>
       </c>
@@ -17626,10 +17647,10 @@
     <row r="108" spans="1:11" ht="21.75" thickBot="1">
       <c r="A108" s="70"/>
       <c r="B108" s="138"/>
-      <c r="C108" s="695" t="s">
+      <c r="C108" s="744" t="s">
         <v>908</v>
       </c>
-      <c r="D108" s="753"/>
+      <c r="D108" s="745"/>
       <c r="E108" s="48" t="s">
         <v>509</v>
       </c>
@@ -17649,10 +17670,10 @@
       <c r="B109" s="107" t="s">
         <v>474</v>
       </c>
-      <c r="C109" s="754" t="s">
+      <c r="C109" s="746" t="s">
         <v>707</v>
       </c>
-      <c r="D109" s="755"/>
+      <c r="D109" s="747"/>
       <c r="E109" s="50">
         <v>2017</v>
       </c>
@@ -17680,10 +17701,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="743" t="s">
+      <c r="C110" s="748" t="s">
         <v>251</v>
       </c>
-      <c r="D110" s="694"/>
+      <c r="D110" s="749"/>
       <c r="E110" s="10" t="s">
         <v>263</v>
       </c>
@@ -17711,10 +17732,10 @@
         <v>2</v>
       </c>
       <c r="B111" s="14"/>
-      <c r="C111" s="756" t="s">
+      <c r="C111" s="750" t="s">
         <v>463</v>
       </c>
-      <c r="D111" s="694"/>
+      <c r="D111" s="749"/>
       <c r="E111" s="12"/>
       <c r="F111" s="29"/>
       <c r="G111" s="29"/>
@@ -17732,10 +17753,10 @@
       <c r="B112" s="54">
         <v>3000</v>
       </c>
-      <c r="C112" s="741" t="s">
+      <c r="C112" s="751" t="s">
         <v>909</v>
       </c>
-      <c r="D112" s="742"/>
+      <c r="D112" s="752"/>
       <c r="E112" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17772,10 +17793,10 @@
       <c r="B113" s="57">
         <v>3100</v>
       </c>
-      <c r="C113" s="729" t="s">
+      <c r="C113" s="689" t="s">
         <v>464</v>
       </c>
-      <c r="D113" s="730"/>
+      <c r="D113" s="690"/>
       <c r="E113" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17812,10 +17833,10 @@
       <c r="B114" s="110">
         <v>3200</v>
       </c>
-      <c r="C114" s="745" t="s">
+      <c r="C114" s="735" t="s">
         <v>758</v>
       </c>
-      <c r="D114" s="702"/>
+      <c r="D114" s="736"/>
       <c r="E114" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17852,10 +17873,10 @@
       <c r="B115" s="57">
         <v>6000</v>
       </c>
-      <c r="C115" s="752" t="s">
+      <c r="C115" s="725" t="s">
         <v>635</v>
       </c>
-      <c r="D115" s="737"/>
+      <c r="D115" s="726"/>
       <c r="E115" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17892,10 +17913,10 @@
       <c r="B116" s="57">
         <v>6100</v>
       </c>
-      <c r="C116" s="723" t="s">
+      <c r="C116" s="707" t="s">
         <v>636</v>
       </c>
-      <c r="D116" s="724"/>
+      <c r="D116" s="708"/>
       <c r="E116" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17932,10 +17953,10 @@
       <c r="B117" s="57">
         <v>6200</v>
       </c>
-      <c r="C117" s="728" t="s">
+      <c r="C117" s="754" t="s">
         <v>637</v>
       </c>
-      <c r="D117" s="738"/>
+      <c r="D117" s="755"/>
       <c r="E117" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17972,10 +17993,10 @@
       <c r="B118" s="57">
         <v>6300</v>
       </c>
-      <c r="C118" s="725" t="s">
+      <c r="C118" s="741" t="s">
         <v>638</v>
       </c>
-      <c r="D118" s="726"/>
+      <c r="D118" s="713"/>
       <c r="E118" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18012,10 +18033,10 @@
       <c r="B119" s="57">
         <v>6400</v>
       </c>
-      <c r="C119" s="748" t="s">
+      <c r="C119" s="739" t="s">
         <v>639</v>
       </c>
-      <c r="D119" s="749"/>
+      <c r="D119" s="740"/>
       <c r="E119" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18110,10 +18131,10 @@
       <c r="B121" s="57">
         <v>6600</v>
       </c>
-      <c r="C121" s="725" t="s">
+      <c r="C121" s="741" t="s">
         <v>254</v>
       </c>
-      <c r="D121" s="726"/>
+      <c r="D121" s="713"/>
       <c r="E121" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18150,10 +18171,10 @@
       <c r="B122" s="57">
         <v>6700</v>
       </c>
-      <c r="C122" s="725" t="s">
+      <c r="C122" s="741" t="s">
         <v>687</v>
       </c>
-      <c r="D122" s="726"/>
+      <c r="D122" s="713"/>
       <c r="E122" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18190,10 +18211,10 @@
       <c r="B123" s="57">
         <v>6900</v>
       </c>
-      <c r="C123" s="750" t="s">
+      <c r="C123" s="742" t="s">
         <v>640</v>
       </c>
-      <c r="D123" s="751"/>
+      <c r="D123" s="743"/>
       <c r="E123" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18228,10 +18249,10 @@
         <v>260</v>
       </c>
       <c r="B124" s="71"/>
-      <c r="C124" s="734" t="s">
+      <c r="C124" s="758" t="s">
         <v>252</v>
       </c>
-      <c r="D124" s="735"/>
+      <c r="D124" s="759"/>
       <c r="E124" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18265,10 +18286,10 @@
         <v>261</v>
       </c>
       <c r="B125" s="112"/>
-      <c r="C125" s="743" t="s">
+      <c r="C125" s="748" t="s">
         <v>253</v>
       </c>
-      <c r="D125" s="694"/>
+      <c r="D125" s="749"/>
       <c r="E125" s="113"/>
       <c r="F125" s="170"/>
       <c r="G125" s="170"/>
@@ -18286,10 +18307,10 @@
       <c r="B126" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C126" s="739" t="s">
+      <c r="C126" s="756" t="s">
         <v>899</v>
       </c>
-      <c r="D126" s="740"/>
+      <c r="D126" s="757"/>
       <c r="E126" s="170"/>
       <c r="F126" s="170"/>
       <c r="G126" s="170"/>
@@ -18307,10 +18328,10 @@
       <c r="B127" s="57">
         <v>7400</v>
       </c>
-      <c r="C127" s="741" t="s">
+      <c r="C127" s="751" t="s">
         <v>900</v>
       </c>
-      <c r="D127" s="742"/>
+      <c r="D127" s="752"/>
       <c r="E127" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18347,10 +18368,10 @@
       <c r="B128" s="57">
         <v>7500</v>
       </c>
-      <c r="C128" s="729" t="s">
+      <c r="C128" s="689" t="s">
         <v>710</v>
       </c>
-      <c r="D128" s="730"/>
+      <c r="D128" s="690"/>
       <c r="E128" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18387,10 +18408,10 @@
       <c r="B129" s="57">
         <v>7600</v>
       </c>
-      <c r="C129" s="709" t="s">
+      <c r="C129" s="697" t="s">
         <v>641</v>
       </c>
-      <c r="D129" s="744"/>
+      <c r="D129" s="698"/>
       <c r="E129" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18427,10 +18448,10 @@
       <c r="B130" s="57">
         <v>7700</v>
       </c>
-      <c r="C130" s="709" t="s">
+      <c r="C130" s="697" t="s">
         <v>642</v>
       </c>
-      <c r="D130" s="700"/>
+      <c r="D130" s="727"/>
       <c r="E130" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18467,10 +18488,10 @@
       <c r="B131" s="96">
         <v>7800</v>
       </c>
-      <c r="C131" s="746" t="s">
-        <v>0</v>
-      </c>
-      <c r="D131" s="747"/>
+      <c r="C131" s="737" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="738"/>
       <c r="E131" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18505,10 +18526,10 @@
         <v>315</v>
       </c>
       <c r="B132" s="71"/>
-      <c r="C132" s="734" t="s">
+      <c r="C132" s="758" t="s">
         <v>898</v>
       </c>
-      <c r="D132" s="735"/>
+      <c r="D132" s="759"/>
       <c r="E132" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18566,12 +18587,12 @@
     </row>
     <row r="136" spans="1:11" ht="42" customHeight="1">
       <c r="A136" s="103"/>
-      <c r="B136" s="689" t="e">
+      <c r="B136" s="705" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C136" s="690"/>
-      <c r="D136" s="690"/>
+      <c r="C136" s="706"/>
+      <c r="D136" s="706"/>
       <c r="E136" s="79"/>
       <c r="F136" s="79"/>
       <c r="K136" s="167">
@@ -18594,12 +18615,12 @@
     </row>
     <row r="138" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A138" s="103"/>
-      <c r="B138" s="691" t="e">
+      <c r="B138" s="721" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C138" s="692"/>
-      <c r="D138" s="692"/>
+      <c r="C138" s="722"/>
+      <c r="D138" s="722"/>
       <c r="E138" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18638,12 +18659,12 @@
     </row>
     <row r="141" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A141" s="103"/>
-      <c r="B141" s="691" t="e">
+      <c r="B141" s="721" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C141" s="692"/>
-      <c r="D141" s="692"/>
+      <c r="C141" s="722"/>
+      <c r="D141" s="722"/>
       <c r="E141" s="79" t="s">
         <v>505</v>
       </c>
@@ -18833,12 +18854,12 @@
     </row>
     <row r="152" spans="1:11" ht="44.25" customHeight="1">
       <c r="A152" s="103"/>
-      <c r="B152" s="689" t="e">
+      <c r="B152" s="705" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C152" s="690"/>
-      <c r="D152" s="690"/>
+      <c r="C152" s="706"/>
+      <c r="D152" s="706"/>
       <c r="E152" s="79"/>
       <c r="F152" s="79"/>
       <c r="K152" s="167">
@@ -18861,12 +18882,12 @@
     </row>
     <row r="154" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A154" s="103"/>
-      <c r="B154" s="691" t="e">
+      <c r="B154" s="721" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C154" s="692"/>
-      <c r="D154" s="692"/>
+      <c r="C154" s="722"/>
+      <c r="D154" s="722"/>
       <c r="E154" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18905,12 +18926,12 @@
     </row>
     <row r="157" spans="1:11" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A157" s="103"/>
-      <c r="B157" s="691" t="e">
+      <c r="B157" s="721" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C157" s="692"/>
-      <c r="D157" s="692"/>
+      <c r="C157" s="722"/>
+      <c r="D157" s="722"/>
       <c r="E157" s="79" t="s">
         <v>505</v>
       </c>
@@ -18960,10 +18981,10 @@
     <row r="161" spans="1:65" ht="21.75" thickBot="1">
       <c r="A161" s="103"/>
       <c r="B161" s="112"/>
-      <c r="C161" s="695" t="s">
+      <c r="C161" s="744" t="s">
         <v>684</v>
       </c>
-      <c r="D161" s="696"/>
+      <c r="D161" s="702"/>
       <c r="E161" s="48" t="s">
         <v>509</v>
       </c>
@@ -18983,10 +19004,10 @@
       <c r="B162" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C162" s="697" t="s">
+      <c r="C162" s="701" t="s">
         <v>707</v>
       </c>
-      <c r="D162" s="698"/>
+      <c r="D162" s="700"/>
       <c r="E162" s="50">
         <v>2017</v>
       </c>
@@ -19014,10 +19035,10 @@
         <v>1</v>
       </c>
       <c r="B163" s="139"/>
-      <c r="C163" s="693" t="s">
+      <c r="C163" s="779" t="s">
         <v>685</v>
       </c>
-      <c r="D163" s="694"/>
+      <c r="D163" s="749"/>
       <c r="E163" s="10" t="s">
         <v>263</v>
       </c>
@@ -19047,10 +19068,10 @@
       <c r="B164" s="54">
         <v>7000</v>
       </c>
-      <c r="C164" s="736" t="s">
+      <c r="C164" s="753" t="s">
         <v>902</v>
       </c>
-      <c r="D164" s="737"/>
+      <c r="D164" s="726"/>
       <c r="E164" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19087,10 +19108,10 @@
       <c r="B165" s="57">
         <v>7100</v>
       </c>
-      <c r="C165" s="703" t="s">
+      <c r="C165" s="719" t="s">
         <v>903</v>
       </c>
-      <c r="D165" s="704"/>
+      <c r="D165" s="720"/>
       <c r="E165" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19127,10 +19148,10 @@
       <c r="B166" s="57">
         <v>7200</v>
       </c>
-      <c r="C166" s="703" t="s">
+      <c r="C166" s="719" t="s">
         <v>1414</v>
       </c>
-      <c r="D166" s="704"/>
+      <c r="D166" s="720"/>
       <c r="E166" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19167,10 +19188,10 @@
       <c r="B167" s="57">
         <v>7300</v>
       </c>
-      <c r="C167" s="731" t="s">
+      <c r="C167" s="712" t="s">
         <v>904</v>
       </c>
-      <c r="D167" s="726"/>
+      <c r="D167" s="713"/>
       <c r="E167" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19207,10 +19228,10 @@
       <c r="B168" s="57">
         <v>7900</v>
       </c>
-      <c r="C168" s="732" t="s">
+      <c r="C168" s="781" t="s">
         <v>905</v>
       </c>
-      <c r="D168" s="733"/>
+      <c r="D168" s="782"/>
       <c r="E168" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19300,10 +19321,10 @@
       <c r="B169" s="57">
         <v>8000</v>
       </c>
-      <c r="C169" s="723" t="s">
+      <c r="C169" s="707" t="s">
         <v>711</v>
       </c>
-      <c r="D169" s="724"/>
+      <c r="D169" s="708"/>
       <c r="E169" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19340,10 +19361,10 @@
       <c r="B170" s="57">
         <v>8100</v>
       </c>
-      <c r="C170" s="709" t="s">
+      <c r="C170" s="697" t="s">
         <v>712</v>
       </c>
-      <c r="D170" s="700"/>
+      <c r="D170" s="727"/>
       <c r="E170" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19380,10 +19401,10 @@
       <c r="B171" s="57">
         <v>8200</v>
       </c>
-      <c r="C171" s="709" t="s">
+      <c r="C171" s="697" t="s">
         <v>101</v>
       </c>
-      <c r="D171" s="700"/>
+      <c r="D171" s="727"/>
       <c r="E171" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19420,10 +19441,10 @@
       <c r="B172" s="57">
         <v>8300</v>
       </c>
-      <c r="C172" s="729" t="s">
+      <c r="C172" s="689" t="s">
         <v>713</v>
       </c>
-      <c r="D172" s="730"/>
+      <c r="D172" s="690"/>
       <c r="E172" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19460,10 +19481,10 @@
       <c r="B173" s="57">
         <v>8500</v>
       </c>
-      <c r="C173" s="723" t="s">
+      <c r="C173" s="707" t="s">
         <v>102</v>
       </c>
-      <c r="D173" s="724"/>
+      <c r="D173" s="708"/>
       <c r="E173" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19500,10 +19521,10 @@
       <c r="B174" s="57">
         <v>8600</v>
       </c>
-      <c r="C174" s="723" t="s">
+      <c r="C174" s="707" t="s">
         <v>103</v>
       </c>
-      <c r="D174" s="724"/>
+      <c r="D174" s="708"/>
       <c r="E174" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19540,10 +19561,10 @@
       <c r="B175" s="57">
         <v>8700</v>
       </c>
-      <c r="C175" s="709" t="s">
+      <c r="C175" s="697" t="s">
         <v>265</v>
       </c>
-      <c r="D175" s="700"/>
+      <c r="D175" s="727"/>
       <c r="E175" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19580,10 +19601,10 @@
       <c r="B176" s="57">
         <v>8800</v>
       </c>
-      <c r="C176" s="709" t="s">
+      <c r="C176" s="697" t="s">
         <v>910</v>
       </c>
-      <c r="D176" s="700"/>
+      <c r="D176" s="727"/>
       <c r="E176" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19620,10 +19641,10 @@
       <c r="B177" s="57">
         <v>8900</v>
       </c>
-      <c r="C177" s="725" t="s">
+      <c r="C177" s="741" t="s">
         <v>759</v>
       </c>
-      <c r="D177" s="726"/>
+      <c r="D177" s="713"/>
       <c r="E177" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19660,10 +19681,10 @@
       <c r="B178" s="57">
         <v>9000</v>
       </c>
-      <c r="C178" s="723" t="s">
+      <c r="C178" s="707" t="s">
         <v>104</v>
       </c>
-      <c r="D178" s="724"/>
+      <c r="D178" s="708"/>
       <c r="E178" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19700,10 +19721,10 @@
       <c r="B179" s="57">
         <v>9100</v>
       </c>
-      <c r="C179" s="725" t="s">
+      <c r="C179" s="741" t="s">
         <v>911</v>
       </c>
-      <c r="D179" s="728"/>
+      <c r="D179" s="754"/>
       <c r="E179" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19740,10 +19761,10 @@
       <c r="B180" s="57">
         <v>9200</v>
       </c>
-      <c r="C180" s="699" t="s">
+      <c r="C180" s="777" t="s">
         <v>714</v>
       </c>
-      <c r="D180" s="700"/>
+      <c r="D180" s="727"/>
       <c r="E180" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19780,10 +19801,10 @@
       <c r="B181" s="57">
         <v>9300</v>
       </c>
-      <c r="C181" s="723" t="s">
+      <c r="C181" s="707" t="s">
         <v>715</v>
       </c>
-      <c r="D181" s="724"/>
+      <c r="D181" s="708"/>
       <c r="E181" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19820,10 +19841,10 @@
       <c r="B182" s="57">
         <v>9500</v>
       </c>
-      <c r="C182" s="699" t="s">
+      <c r="C182" s="777" t="s">
         <v>716</v>
       </c>
-      <c r="D182" s="727"/>
+      <c r="D182" s="778"/>
       <c r="E182" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19860,10 +19881,10 @@
       <c r="B183" s="57">
         <v>9600</v>
       </c>
-      <c r="C183" s="699" t="s">
+      <c r="C183" s="777" t="s">
         <v>717</v>
       </c>
-      <c r="D183" s="700"/>
+      <c r="D183" s="727"/>
       <c r="E183" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19900,10 +19921,10 @@
       <c r="B184" s="57">
         <v>9800</v>
       </c>
-      <c r="C184" s="701" t="s">
+      <c r="C184" s="780" t="s">
         <v>465</v>
       </c>
-      <c r="D184" s="702"/>
+      <c r="D184" s="736"/>
       <c r="E184" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19938,10 +19959,10 @@
         <v>610</v>
       </c>
       <c r="B185" s="146"/>
-      <c r="C185" s="697" t="s">
+      <c r="C185" s="701" t="s">
         <v>930</v>
       </c>
-      <c r="D185" s="698"/>
+      <c r="D185" s="700"/>
       <c r="E185" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -20004,12 +20025,12 @@
       </c>
     </row>
     <row r="189" spans="1:11" ht="42" customHeight="1">
-      <c r="B189" s="689" t="e">
+      <c r="B189" s="705" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C189" s="690"/>
-      <c r="D189" s="690"/>
+      <c r="C189" s="706"/>
+      <c r="D189" s="706"/>
       <c r="E189" s="79"/>
       <c r="F189" s="79"/>
       <c r="G189" s="56"/>
@@ -20032,12 +20053,12 @@
       </c>
     </row>
     <row r="191" spans="1:11" ht="21.75" thickBot="1">
-      <c r="B191" s="691" t="e">
+      <c r="B191" s="721" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C191" s="692"/>
-      <c r="D191" s="692"/>
+      <c r="C191" s="722"/>
+      <c r="D191" s="722"/>
       <c r="E191" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -20076,12 +20097,12 @@
       </c>
     </row>
     <row r="194" spans="2:11" ht="22.5" thickTop="1" thickBot="1">
-      <c r="B194" s="691" t="e">
+      <c r="B194" s="721" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C194" s="692"/>
-      <c r="D194" s="692"/>
+      <c r="C194" s="722"/>
+      <c r="D194" s="722"/>
       <c r="E194" s="79" t="s">
         <v>505</v>
       </c>
@@ -20135,10 +20156,10 @@
       <c r="B198" s="153" t="s">
         <v>474</v>
       </c>
-      <c r="C198" s="707" t="s">
+      <c r="C198" s="762" t="s">
         <v>718</v>
       </c>
-      <c r="D198" s="698"/>
+      <c r="D198" s="700"/>
       <c r="E198" s="48" t="s">
         <v>509</v>
       </c>
@@ -20155,8 +20176,8 @@
     </row>
     <row r="199" spans="2:11" ht="45.75" thickBot="1">
       <c r="B199" s="154"/>
-      <c r="C199" s="708"/>
-      <c r="D199" s="696"/>
+      <c r="C199" s="763"/>
+      <c r="D199" s="702"/>
       <c r="E199" s="50">
         <v>2017</v>
       </c>
@@ -20183,10 +20204,10 @@
       <c r="B200" s="155" t="s">
         <v>719</v>
       </c>
-      <c r="C200" s="721" t="s">
+      <c r="C200" s="775" t="s">
         <v>720</v>
       </c>
-      <c r="D200" s="722"/>
+      <c r="D200" s="776"/>
       <c r="E200" s="187" t="e">
         <f>SUMIF(#REF!,1,#REF!)</f>
         <v>#REF!</v>
@@ -20219,10 +20240,10 @@
       <c r="B201" s="156" t="s">
         <v>721</v>
       </c>
-      <c r="C201" s="714" t="s">
+      <c r="C201" s="768" t="s">
         <v>722</v>
       </c>
-      <c r="D201" s="715"/>
+      <c r="D201" s="769"/>
       <c r="E201" s="188" t="e">
         <f>SUMIF(#REF!,2,#REF!)</f>
         <v>#REF!</v>
@@ -20255,10 +20276,10 @@
       <c r="B202" s="156" t="s">
         <v>723</v>
       </c>
-      <c r="C202" s="714" t="s">
+      <c r="C202" s="768" t="s">
         <v>724</v>
       </c>
-      <c r="D202" s="715"/>
+      <c r="D202" s="769"/>
       <c r="E202" s="188" t="e">
         <f>SUMIF(#REF!,3,#REF!)</f>
         <v>#REF!</v>
@@ -20291,10 +20312,10 @@
       <c r="B203" s="156" t="s">
         <v>725</v>
       </c>
-      <c r="C203" s="717" t="s">
+      <c r="C203" s="771" t="s">
         <v>726</v>
       </c>
-      <c r="D203" s="718"/>
+      <c r="D203" s="772"/>
       <c r="E203" s="188" t="e">
         <f>SUMIF(#REF!,4,#REF!)</f>
         <v>#REF!</v>
@@ -20327,10 +20348,10 @@
       <c r="B204" s="156" t="s">
         <v>727</v>
       </c>
-      <c r="C204" s="719" t="s">
+      <c r="C204" s="773" t="s">
         <v>728</v>
       </c>
-      <c r="D204" s="720"/>
+      <c r="D204" s="774"/>
       <c r="E204" s="188" t="e">
         <f>SUMIF(#REF!,5,#REF!)</f>
         <v>#REF!</v>
@@ -20363,10 +20384,10 @@
       <c r="B205" s="156" t="s">
         <v>729</v>
       </c>
-      <c r="C205" s="716" t="s">
+      <c r="C205" s="770" t="s">
         <v>730</v>
       </c>
-      <c r="D205" s="716"/>
+      <c r="D205" s="770"/>
       <c r="E205" s="188" t="e">
         <f>SUMIF(#REF!,6,#REF!)</f>
         <v>#REF!</v>
@@ -20399,10 +20420,10 @@
       <c r="B206" s="156" t="s">
         <v>731</v>
       </c>
-      <c r="C206" s="710" t="s">
+      <c r="C206" s="764" t="s">
         <v>732</v>
       </c>
-      <c r="D206" s="711"/>
+      <c r="D206" s="765"/>
       <c r="E206" s="188" t="e">
         <f>SUMIF(#REF!,7,#REF!)</f>
         <v>#REF!</v>
@@ -20435,10 +20456,10 @@
       <c r="B207" s="156" t="s">
         <v>733</v>
       </c>
-      <c r="C207" s="710" t="s">
+      <c r="C207" s="764" t="s">
         <v>734</v>
       </c>
-      <c r="D207" s="711"/>
+      <c r="D207" s="765"/>
       <c r="E207" s="188" t="e">
         <f>SUMIF(#REF!,8,#REF!)</f>
         <v>#REF!</v>
@@ -20471,10 +20492,10 @@
       <c r="B208" s="156" t="s">
         <v>735</v>
       </c>
-      <c r="C208" s="712" t="s">
+      <c r="C208" s="766" t="s">
         <v>736</v>
       </c>
-      <c r="D208" s="713"/>
+      <c r="D208" s="767"/>
       <c r="E208" s="189" t="e">
         <f>SUMIF(#REF!,9,#REF!)</f>
         <v>#REF!</v>
@@ -20505,10 +20526,10 @@
     </row>
     <row r="209" spans="2:11" ht="21.75" thickBot="1">
       <c r="B209" s="157"/>
-      <c r="C209" s="705" t="s">
+      <c r="C209" s="760" t="s">
         <v>737</v>
       </c>
-      <c r="D209" s="706"/>
+      <c r="D209" s="761"/>
       <c r="E209" s="158" t="e">
         <f t="shared" ref="E209:J209" si="5">SUM(E200:E208)</f>
         <v>#REF!</v>
@@ -22117,106 +22138,17 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="145">
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="N63:N65"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="O63:O65"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="L63:L65"/>
-    <mergeCell ref="M63:M65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="C164:D164"/>
-    <mergeCell ref="C165:D165"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
     <mergeCell ref="C209:D209"/>
     <mergeCell ref="C198:D198"/>
     <mergeCell ref="C199:D199"/>
@@ -22240,28 +22172,117 @@
     <mergeCell ref="C180:D180"/>
     <mergeCell ref="B189:D189"/>
     <mergeCell ref="B194:D194"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C183:D183"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
     <mergeCell ref="C161:D161"/>
     <mergeCell ref="C162:D162"/>
     <mergeCell ref="C163:D163"/>
-    <mergeCell ref="C183:D183"/>
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C172:D172"/>
-    <mergeCell ref="C173:D173"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
     <mergeCell ref="C132:D132"/>
     <mergeCell ref="B136:D136"/>
     <mergeCell ref="B138:D138"/>
     <mergeCell ref="B141:D141"/>
     <mergeCell ref="B152:D152"/>
     <mergeCell ref="B154:D154"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="N63:N65"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="O63:O65"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="L63:L65"/>
+    <mergeCell ref="M63:M65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
@@ -22313,8 +22334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -22464,12 +22485,12 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="209"/>
-      <c r="B7" s="783" t="str">
+      <c r="B7" s="793" t="str">
         <f>VLOOKUP(E8,SMETKA,2,FALSE)</f>
         <v>ОТЧЕТНИ ДАННИ ПО ЕБК ЗА ИЗПЪЛНЕНИЕТО НА БЮДЖЕТА</v>
       </c>
-      <c r="C7" s="784"/>
-      <c r="D7" s="784"/>
+      <c r="C7" s="794"/>
+      <c r="D7" s="794"/>
       <c r="E7" s="337"/>
       <c r="F7" s="337"/>
       <c r="G7" s="337"/>
@@ -22568,11 +22589,11 @@
     </row>
     <row r="13" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="210"/>
-      <c r="B13" s="789" t="s">
+      <c r="B13" s="787" t="s">
         <v>1498</v>
       </c>
-      <c r="C13" s="790"/>
-      <c r="D13" s="791"/>
+      <c r="C13" s="788"/>
+      <c r="D13" s="789"/>
       <c r="E13" s="338">
         <v>44927</v>
       </c>
@@ -22624,11 +22645,11 @@
     </row>
     <row r="16" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="792" t="s">
+      <c r="B16" s="790" t="s">
         <v>1498</v>
       </c>
-      <c r="C16" s="793"/>
-      <c r="D16" s="794"/>
+      <c r="C16" s="791"/>
+      <c r="D16" s="792"/>
       <c r="E16" s="356"/>
       <c r="F16" s="587"/>
       <c r="G16" s="326"/>
@@ -22806,27 +22827,28 @@
       <c r="B24" s="395">
         <v>100</v>
       </c>
-      <c r="C24" s="786" t="s">
+      <c r="C24" s="784" t="s">
         <v>388</v>
       </c>
-      <c r="D24" s="787"/>
+      <c r="D24" s="785"/>
       <c r="E24" s="241">
         <f>SUMIF($B$43:$B$44,$B24,E$43:E$44)</f>
         <v>0</v>
       </c>
       <c r="F24" s="242">
+        <f>G24+H24+I24</f>
         <v>0</v>
       </c>
       <c r="G24" s="266">
-        <f>SUMIF($B$43:$B$44,$B24,G$43:G$44)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="267">
-        <f>SUMIF($B$43:$B$44,$B24,H$43:H$44)</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="268">
-        <f>SUMIF($B$43:$B$44,$B24,I$43:I$44)</f>
+        <f>SUM(G25:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="266">
+        <f t="shared" ref="H24:I24" si="0">SUM(H25:H30)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="266">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J24" s="582" t="e">
@@ -22949,7 +22971,7 @@
         <v>551</v>
       </c>
       <c r="D27" s="409" t="s">
-        <v>580</v>
+        <v>1511</v>
       </c>
       <c r="E27" s="285">
         <v>0</v>
@@ -22981,7 +23003,7 @@
         <v>560</v>
       </c>
       <c r="D28" s="413" t="s">
-        <v>582</v>
+        <v>1509</v>
       </c>
       <c r="E28" s="287">
         <v>0</v>
@@ -23013,7 +23035,7 @@
         <v>580</v>
       </c>
       <c r="D29" s="411" t="s">
-        <v>583</v>
+        <v>1510</v>
       </c>
       <c r="E29" s="287">
         <v>0</v>
@@ -23070,23 +23092,27 @@
       <c r="B31" s="395">
         <v>1000</v>
       </c>
-      <c r="C31" s="788" t="s">
+      <c r="C31" s="786" t="s">
         <v>586</v>
       </c>
-      <c r="D31" s="788"/>
+      <c r="D31" s="786"/>
       <c r="E31" s="243">
         <v>0</v>
       </c>
-      <c r="F31" s="244">
+      <c r="F31" s="242">
+        <f>G31+H31+I31</f>
         <v>0</v>
       </c>
       <c r="G31" s="266">
-        <v>0</v>
-      </c>
-      <c r="H31" s="267">
-        <v>0</v>
-      </c>
-      <c r="I31" s="268">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="266">
+        <f t="shared" ref="H31:I31" si="1">SUM(H32:H34)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="266">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J31" s="582" t="e">
@@ -23210,23 +23236,27 @@
       <c r="B35" s="449" t="s">
         <v>1499</v>
       </c>
-      <c r="C35" s="785" t="s">
+      <c r="C35" s="783" t="s">
         <v>1500</v>
       </c>
-      <c r="D35" s="785"/>
+      <c r="D35" s="783"/>
       <c r="E35" s="243">
         <v>0</v>
       </c>
-      <c r="F35" s="244">
+      <c r="F35" s="242">
+        <f>G35+H35+I35</f>
         <v>0</v>
       </c>
       <c r="G35" s="266">
-        <v>0</v>
-      </c>
-      <c r="H35" s="267">
-        <v>0</v>
-      </c>
-      <c r="I35" s="268">
+        <f>SUM(G36:G38)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="266">
+        <f t="shared" ref="H35:I35" si="2">SUM(H36:H38)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="266">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J35" s="582"/>
@@ -23427,19 +23457,19 @@
         <v>0</v>
       </c>
       <c r="F42" s="248">
-        <f>SUMIF($C$43:$C$44,$C42,F$43:F$44)</f>
+        <f>F24+F31+F35</f>
         <v>0</v>
       </c>
       <c r="G42" s="312">
-        <f>SUMIF($C$43:$C$44,$C42,G$43:G$44)</f>
+        <f>G24+G31+G35</f>
         <v>0</v>
       </c>
       <c r="H42" s="313">
-        <f>SUMIF($C$43:$C$44,$C42,H$43:H$44)</f>
+        <f>H24+H31+H35</f>
         <v>0</v>
       </c>
       <c r="I42" s="314">
-        <f>SUMIF($C$43:$C$44,$C42,I$43:I$44)</f>
+        <f>I24+I31+I35</f>
         <v>0</v>
       </c>
       <c r="J42" s="4">
@@ -23457,83 +23487,83 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="44" priority="85" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="85" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="43" priority="74" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="74" stopIfTrue="1" operator="equal">
       <formula>98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="76" stopIfTrue="1" operator="equal">
       <formula>96</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="77" stopIfTrue="1" operator="equal">
       <formula>42</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="78" stopIfTrue="1" operator="equal">
       <formula>97</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="79" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="79" stopIfTrue="1" operator="equal">
       <formula>33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="38" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="70" stopIfTrue="1" operator="equal">
       <formula>"ЧУЖДИ СРЕДСТВА"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="71" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="71" stopIfTrue="1" operator="equal">
       <formula>"СЕС - ДМП"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="72" stopIfTrue="1" operator="equal">
       <formula>"СЕС - РА"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="73" stopIfTrue="1" operator="equal">
       <formula>"СЕС - ДЕС"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="75" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="75" stopIfTrue="1" operator="equal">
       <formula>"СЕС - КСФ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="33" priority="65" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="65" stopIfTrue="1" operator="equal">
       <formula>98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="66" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="66" stopIfTrue="1" operator="equal">
       <formula>96</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="67" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="67" stopIfTrue="1" operator="equal">
       <formula>42</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="68" stopIfTrue="1" operator="equal">
       <formula>97</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="69" stopIfTrue="1" operator="equal">
       <formula>33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="28" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="45" stopIfTrue="1" operator="equal">
       <formula>"ЧУЖДИ СРЕДСТВА"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="46" stopIfTrue="1" operator="equal">
       <formula>"СЕС - ДМП"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="47" stopIfTrue="1" operator="equal">
       <formula>"СЕС - РА"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="48" stopIfTrue="1" operator="equal">
       <formula>"СЕС - ДЕС"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="49" stopIfTrue="1" operator="equal">
       <formula>"СЕС - КСФ"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23698,12 +23728,12 @@
         <v>3</v>
       </c>
       <c r="H14" s="328"/>
-      <c r="I14" s="800">
+      <c r="I14" s="797">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J14" s="801"/>
-      <c r="K14" s="801"/>
+      <c r="J14" s="798"/>
+      <c r="K14" s="798"/>
       <c r="L14" s="346"/>
       <c r="M14" s="346"/>
       <c r="N14" s="347"/>
@@ -23747,12 +23777,12 @@
         <v>5</v>
       </c>
       <c r="H16" s="328"/>
-      <c r="I16" s="802">
+      <c r="I16" s="799">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J16" s="803"/>
-      <c r="K16" s="804"/>
+      <c r="J16" s="800"/>
+      <c r="K16" s="801"/>
       <c r="L16" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -23819,12 +23849,12 @@
         <v>8</v>
       </c>
       <c r="H19" s="328"/>
-      <c r="I19" s="805">
+      <c r="I19" s="802">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J19" s="806"/>
-      <c r="K19" s="807"/>
+      <c r="J19" s="803"/>
+      <c r="K19" s="804"/>
       <c r="L19" s="356" t="s">
         <v>934</v>
       </c>
@@ -24119,10 +24149,10 @@
       <c r="I30" s="395">
         <v>100</v>
       </c>
-      <c r="J30" s="786" t="s">
+      <c r="J30" s="784" t="s">
         <v>388</v>
       </c>
-      <c r="K30" s="787"/>
+      <c r="K30" s="785"/>
       <c r="L30" s="241">
         <f t="shared" ref="L30:Q30" si="0">SUM(L31:L32)</f>
         <v>0</v>
@@ -24215,10 +24245,10 @@
       <c r="I33" s="395">
         <v>200</v>
       </c>
-      <c r="J33" s="788" t="s">
+      <c r="J33" s="786" t="s">
         <v>391</v>
       </c>
-      <c r="K33" s="788"/>
+      <c r="K33" s="786"/>
       <c r="L33" s="241">
         <f t="shared" ref="L33:Q33" si="2">SUM(L34:L38)</f>
         <v>0</v>
@@ -24392,10 +24422,10 @@
       <c r="I39" s="395">
         <v>500</v>
       </c>
-      <c r="J39" s="813" t="s">
+      <c r="J39" s="796" t="s">
         <v>579</v>
       </c>
-      <c r="K39" s="813"/>
+      <c r="K39" s="796"/>
       <c r="L39" s="241">
         <f t="shared" ref="L39:Q39" si="3">SUM(L40:L46)</f>
         <v>0</v>
@@ -24664,10 +24694,10 @@
       <c r="I47" s="395">
         <v>800</v>
       </c>
-      <c r="J47" s="809" t="s">
+      <c r="J47" s="807" t="s">
         <v>698</v>
       </c>
-      <c r="K47" s="810"/>
+      <c r="K47" s="808"/>
       <c r="L47" s="567"/>
       <c r="M47" s="244">
         <f t="shared" si="4"/>
@@ -24691,10 +24721,10 @@
       <c r="I48" s="395">
         <v>1000</v>
       </c>
-      <c r="J48" s="788" t="s">
+      <c r="J48" s="786" t="s">
         <v>586</v>
       </c>
-      <c r="K48" s="788"/>
+      <c r="K48" s="786"/>
       <c r="L48" s="243">
         <f t="shared" ref="L48:Q48" si="5">SUM(L49:L65)</f>
         <v>0</v>
@@ -25622,7 +25652,7 @@
       <c r="J79" s="795" t="s">
         <v>606</v>
       </c>
-      <c r="K79" s="811"/>
+      <c r="K79" s="809"/>
       <c r="L79" s="567"/>
       <c r="M79" s="244">
         <f t="shared" si="10"/>
@@ -25646,10 +25676,10 @@
       <c r="I80" s="395">
         <v>2600</v>
       </c>
-      <c r="J80" s="812" t="s">
+      <c r="J80" s="805" t="s">
         <v>607</v>
       </c>
-      <c r="K80" s="787"/>
+      <c r="K80" s="785"/>
       <c r="L80" s="567"/>
       <c r="M80" s="244">
         <f t="shared" si="10"/>
@@ -25673,10 +25703,10 @@
       <c r="I81" s="395">
         <v>2700</v>
       </c>
-      <c r="J81" s="812" t="s">
+      <c r="J81" s="805" t="s">
         <v>608</v>
       </c>
-      <c r="K81" s="787"/>
+      <c r="K81" s="785"/>
       <c r="L81" s="567"/>
       <c r="M81" s="244">
         <f t="shared" si="10"/>
@@ -25700,10 +25730,10 @@
       <c r="I82" s="395">
         <v>2800</v>
       </c>
-      <c r="J82" s="812" t="s">
+      <c r="J82" s="805" t="s">
         <v>1011</v>
       </c>
-      <c r="K82" s="787"/>
+      <c r="K82" s="785"/>
       <c r="L82" s="567"/>
       <c r="M82" s="244">
         <f t="shared" si="10"/>
@@ -26644,10 +26674,10 @@
       <c r="I114" s="395">
         <v>4600</v>
       </c>
-      <c r="J114" s="812" t="s">
+      <c r="J114" s="805" t="s">
         <v>630</v>
       </c>
-      <c r="K114" s="787"/>
+      <c r="K114" s="785"/>
       <c r="L114" s="567"/>
       <c r="M114" s="244">
         <f t="shared" si="19"/>
@@ -26767,10 +26797,10 @@
       <c r="I118" s="449">
         <v>5100</v>
       </c>
-      <c r="J118" s="785" t="s">
+      <c r="J118" s="783" t="s">
         <v>631</v>
       </c>
-      <c r="K118" s="785"/>
+      <c r="K118" s="783"/>
       <c r="L118" s="567"/>
       <c r="M118" s="244">
         <f>N118+O118+P118+Q118</f>
@@ -26794,10 +26824,10 @@
       <c r="I119" s="449">
         <v>5200</v>
       </c>
-      <c r="J119" s="785" t="s">
+      <c r="J119" s="783" t="s">
         <v>632</v>
       </c>
-      <c r="K119" s="785"/>
+      <c r="K119" s="783"/>
       <c r="L119" s="243">
         <f t="shared" ref="L119:Q119" si="21">SUM(L120:L126)</f>
         <v>0</v>
@@ -27025,10 +27055,10 @@
       <c r="I127" s="449">
         <v>5300</v>
       </c>
-      <c r="J127" s="785" t="s">
+      <c r="J127" s="783" t="s">
         <v>191</v>
       </c>
-      <c r="K127" s="785"/>
+      <c r="K127" s="783"/>
       <c r="L127" s="243">
         <f t="shared" ref="L127:Q127" si="23">SUM(L128:L129)</f>
         <v>0</v>
@@ -27121,10 +27151,10 @@
       <c r="I130" s="449">
         <v>5400</v>
       </c>
-      <c r="J130" s="785" t="s">
+      <c r="J130" s="783" t="s">
         <v>643</v>
       </c>
-      <c r="K130" s="785"/>
+      <c r="K130" s="783"/>
       <c r="L130" s="567"/>
       <c r="M130" s="244">
         <f>N130+O130+P130+Q130</f>
@@ -27298,10 +27328,10 @@
       <c r="I136" s="449">
         <v>5700</v>
       </c>
-      <c r="J136" s="796" t="s">
+      <c r="J136" s="810" t="s">
         <v>943</v>
       </c>
-      <c r="K136" s="797"/>
+      <c r="K136" s="811"/>
       <c r="L136" s="243">
         <f t="shared" ref="L136:Q136" si="25">SUM(L137:L139)</f>
         <v>0</v>
@@ -27441,10 +27471,10 @@
       <c r="I141" s="464">
         <v>98</v>
       </c>
-      <c r="J141" s="798" t="s">
+      <c r="J141" s="812" t="s">
         <v>653</v>
       </c>
-      <c r="K141" s="799"/>
+      <c r="K141" s="813"/>
       <c r="L141" s="573"/>
       <c r="M141" s="324">
         <f>N141+O141+P141+Q141</f>
@@ -27640,12 +27670,12 @@
         <v>138</v>
       </c>
       <c r="H149" s="328"/>
-      <c r="I149" s="800">
+      <c r="I149" s="797">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J149" s="801"/>
-      <c r="K149" s="801"/>
+      <c r="J149" s="798"/>
+      <c r="K149" s="798"/>
       <c r="L149" s="326"/>
       <c r="M149" s="326"/>
       <c r="N149" s="326"/>
@@ -27687,12 +27717,12 @@
         <v>140</v>
       </c>
       <c r="H151" s="328"/>
-      <c r="I151" s="802">
+      <c r="I151" s="799">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J151" s="803"/>
-      <c r="K151" s="804"/>
+      <c r="J151" s="800"/>
+      <c r="K151" s="801"/>
       <c r="L151" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -27759,12 +27789,12 @@
         <v>143</v>
       </c>
       <c r="H154" s="328"/>
-      <c r="I154" s="805">
+      <c r="I154" s="802">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J154" s="806"/>
-      <c r="K154" s="807"/>
+      <c r="J154" s="803"/>
+      <c r="K154" s="804"/>
       <c r="L154" s="356" t="s">
         <v>934</v>
       </c>
@@ -28562,11 +28592,11 @@
         <v>175</v>
       </c>
       <c r="H186" s="328"/>
-      <c r="I186" s="808" t="s">
+      <c r="I186" s="806" t="s">
         <v>249</v>
       </c>
-      <c r="J186" s="808"/>
-      <c r="K186" s="808"/>
+      <c r="J186" s="806"/>
+      <c r="K186" s="806"/>
       <c r="L186" s="327"/>
       <c r="M186" s="327"/>
       <c r="N186" s="327"/>
@@ -29908,21 +29938,11 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="36">
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J141:K141"/>
     <mergeCell ref="I149:K149"/>
     <mergeCell ref="I151:K151"/>
     <mergeCell ref="I154:K154"/>
@@ -29939,11 +29959,21 @@
     <mergeCell ref="J99:K99"/>
     <mergeCell ref="J100:K100"/>
     <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L156:M156">

</xml_diff>

<commit_message>
Implemented Consolidated budgets handling.
</commit_message>
<xml_diff>
--- a/PaymentsBudgetSystem/wwwroot/Report.xlsx
+++ b/PaymentsBudgetSystem/wwwroot/Report.xlsx
@@ -13019,10 +13019,261 @@
     <xf numFmtId="3" fontId="13" fillId="12" borderId="102" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -13045,259 +13296,14 @@
     <xf numFmtId="0" fontId="45" fillId="5" borderId="114" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -13329,16 +13335,19 @@
     <xf numFmtId="0" fontId="152" fillId="20" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -13364,9 +13373,6 @@
     </xf>
     <xf numFmtId="0" fontId="149" fillId="20" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -13382,15 +13388,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -14443,12 +14443,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="42" customHeight="1">
-      <c r="B7" s="691" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="692"/>
-      <c r="D7" s="692"/>
+      <c r="B7" s="776" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C7" s="777"/>
+      <c r="D7" s="777"/>
       <c r="F7" s="38"/>
       <c r="K7" s="167">
         <v>1</v>
@@ -14468,12 +14468,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="36.75" customHeight="1" thickBot="1">
-      <c r="B9" s="693" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="694"/>
-      <c r="D9" s="694"/>
+      <c r="B9" s="778" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="779"/>
+      <c r="D9" s="779"/>
       <c r="E9" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14508,12 +14508,12 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="39" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B12" s="693" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C12" s="694"/>
-      <c r="D12" s="694"/>
+      <c r="B12" s="778" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C12" s="779"/>
+      <c r="D12" s="779"/>
       <c r="E12" s="38" t="s">
         <v>505</v>
       </c>
@@ -14588,10 +14588,10 @@
     <row r="19" spans="1:11" ht="21.75" thickBot="1">
       <c r="A19" s="46"/>
       <c r="B19" s="47"/>
-      <c r="C19" s="699" t="s">
+      <c r="C19" s="782" t="s">
         <v>508</v>
       </c>
-      <c r="D19" s="700"/>
+      <c r="D19" s="708"/>
       <c r="E19" s="48" t="s">
         <v>509</v>
       </c>
@@ -14610,10 +14610,10 @@
       <c r="B20" s="49" t="s">
         <v>474</v>
       </c>
-      <c r="C20" s="701" t="s">
+      <c r="C20" s="711" t="s">
         <v>705</v>
       </c>
-      <c r="D20" s="702"/>
+      <c r="D20" s="710"/>
       <c r="E20" s="50">
         <v>2017</v>
       </c>
@@ -14638,10 +14638,10 @@
     </row>
     <row r="21" spans="1:11" ht="21.75" thickBot="1">
       <c r="B21" s="51"/>
-      <c r="C21" s="779" t="s">
+      <c r="C21" s="744" t="s">
         <v>512</v>
       </c>
-      <c r="D21" s="749"/>
+      <c r="D21" s="741"/>
       <c r="E21" s="10" t="s">
         <v>263</v>
       </c>
@@ -14671,10 +14671,10 @@
       <c r="B22" s="54">
         <v>100</v>
       </c>
-      <c r="C22" s="695" t="s">
+      <c r="C22" s="780" t="s">
         <v>513</v>
       </c>
-      <c r="D22" s="696"/>
+      <c r="D22" s="781"/>
       <c r="E22" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14711,10 +14711,10 @@
       <c r="B23" s="57">
         <v>200</v>
       </c>
-      <c r="C23" s="689" t="s">
+      <c r="C23" s="699" t="s">
         <v>514</v>
       </c>
-      <c r="D23" s="690"/>
+      <c r="D23" s="700"/>
       <c r="E23" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14754,7 +14754,7 @@
       <c r="C24" s="697" t="s">
         <v>515</v>
       </c>
-      <c r="D24" s="698"/>
+      <c r="D24" s="742"/>
       <c r="E24" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14791,10 +14791,10 @@
       <c r="B25" s="57">
         <v>800</v>
       </c>
-      <c r="C25" s="689" t="s">
+      <c r="C25" s="699" t="s">
         <v>924</v>
       </c>
-      <c r="D25" s="690"/>
+      <c r="D25" s="700"/>
       <c r="E25" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14831,10 +14831,10 @@
       <c r="B26" s="57">
         <v>1000</v>
       </c>
-      <c r="C26" s="689" t="s">
+      <c r="C26" s="699" t="s">
         <v>516</v>
       </c>
-      <c r="D26" s="690"/>
+      <c r="D26" s="700"/>
       <c r="E26" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14871,10 +14871,10 @@
       <c r="B27" s="57">
         <v>1300</v>
       </c>
-      <c r="C27" s="689" t="s">
+      <c r="C27" s="699" t="s">
         <v>706</v>
       </c>
-      <c r="D27" s="690"/>
+      <c r="D27" s="700"/>
       <c r="E27" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14911,10 +14911,10 @@
       <c r="B28" s="57">
         <v>1400</v>
       </c>
-      <c r="C28" s="689" t="s">
+      <c r="C28" s="699" t="s">
         <v>517</v>
       </c>
-      <c r="D28" s="690"/>
+      <c r="D28" s="700"/>
       <c r="E28" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14951,10 +14951,10 @@
       <c r="B29" s="57">
         <v>1500</v>
       </c>
-      <c r="C29" s="689" t="s">
+      <c r="C29" s="699" t="s">
         <v>518</v>
       </c>
-      <c r="D29" s="690"/>
+      <c r="D29" s="700"/>
       <c r="E29" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14988,10 +14988,10 @@
       <c r="B30" s="57">
         <v>1600</v>
       </c>
-      <c r="C30" s="689" t="s">
+      <c r="C30" s="699" t="s">
         <v>519</v>
       </c>
-      <c r="D30" s="690"/>
+      <c r="D30" s="700"/>
       <c r="E30" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15028,10 +15028,10 @@
       <c r="B31" s="57">
         <v>1700</v>
       </c>
-      <c r="C31" s="689" t="s">
+      <c r="C31" s="699" t="s">
         <v>520</v>
       </c>
-      <c r="D31" s="690"/>
+      <c r="D31" s="700"/>
       <c r="E31" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15068,10 +15068,10 @@
       <c r="B32" s="57">
         <v>1800</v>
       </c>
-      <c r="C32" s="689" t="s">
+      <c r="C32" s="699" t="s">
         <v>521</v>
       </c>
-      <c r="D32" s="690"/>
+      <c r="D32" s="700"/>
       <c r="E32" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15108,10 +15108,10 @@
       <c r="B33" s="57">
         <v>1900</v>
       </c>
-      <c r="C33" s="689" t="s">
+      <c r="C33" s="699" t="s">
         <v>522</v>
       </c>
-      <c r="D33" s="690"/>
+      <c r="D33" s="700"/>
       <c r="E33" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15148,10 +15148,10 @@
       <c r="B34" s="57">
         <v>2000</v>
       </c>
-      <c r="C34" s="689" t="s">
+      <c r="C34" s="699" t="s">
         <v>523</v>
       </c>
-      <c r="D34" s="690"/>
+      <c r="D34" s="700"/>
       <c r="E34" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15188,10 +15188,10 @@
       <c r="B35" s="57">
         <v>2400</v>
       </c>
-      <c r="C35" s="689" t="s">
+      <c r="C35" s="699" t="s">
         <v>524</v>
       </c>
-      <c r="D35" s="690"/>
+      <c r="D35" s="700"/>
       <c r="E35" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15228,10 +15228,10 @@
       <c r="B36" s="62">
         <v>2500</v>
       </c>
-      <c r="C36" s="707" t="s">
+      <c r="C36" s="695" t="s">
         <v>525</v>
       </c>
-      <c r="D36" s="708"/>
+      <c r="D36" s="696"/>
       <c r="E36" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15268,10 +15268,10 @@
       <c r="B37" s="57">
         <v>2600</v>
       </c>
-      <c r="C37" s="707" t="s">
+      <c r="C37" s="695" t="s">
         <v>300</v>
       </c>
-      <c r="D37" s="708"/>
+      <c r="D37" s="696"/>
       <c r="E37" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15308,10 +15308,10 @@
       <c r="B38" s="57">
         <v>2700</v>
       </c>
-      <c r="C38" s="689" t="s">
+      <c r="C38" s="699" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="690"/>
+      <c r="D38" s="700"/>
       <c r="E38" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15348,10 +15348,10 @@
       <c r="B39" s="57">
         <v>2800</v>
       </c>
-      <c r="C39" s="689" t="s">
+      <c r="C39" s="699" t="s">
         <v>529</v>
       </c>
-      <c r="D39" s="690"/>
+      <c r="D39" s="700"/>
       <c r="E39" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15388,10 +15388,10 @@
       <c r="B40" s="57">
         <v>3600</v>
       </c>
-      <c r="C40" s="689" t="s">
+      <c r="C40" s="699" t="s">
         <v>530</v>
       </c>
-      <c r="D40" s="690"/>
+      <c r="D40" s="700"/>
       <c r="E40" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15428,10 +15428,10 @@
       <c r="B41" s="57">
         <v>3700</v>
       </c>
-      <c r="C41" s="689" t="s">
+      <c r="C41" s="699" t="s">
         <v>531</v>
       </c>
-      <c r="D41" s="690"/>
+      <c r="D41" s="700"/>
       <c r="E41" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15522,10 +15522,10 @@
       <c r="B43" s="57">
         <v>4100</v>
       </c>
-      <c r="C43" s="689" t="s">
+      <c r="C43" s="699" t="s">
         <v>381</v>
       </c>
-      <c r="D43" s="690"/>
+      <c r="D43" s="700"/>
       <c r="E43" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15563,10 +15563,10 @@
       <c r="B44" s="57">
         <v>4200</v>
       </c>
-      <c r="C44" s="689" t="s">
+      <c r="C44" s="699" t="s">
         <v>382</v>
       </c>
-      <c r="D44" s="690"/>
+      <c r="D44" s="700"/>
       <c r="E44" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15604,10 +15604,10 @@
       <c r="B45" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="C45" s="689" t="s">
+      <c r="C45" s="699" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="690"/>
+      <c r="D45" s="700"/>
       <c r="E45" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15645,10 +15645,10 @@
       <c r="B46" s="57">
         <v>4600</v>
       </c>
-      <c r="C46" s="689" t="s">
+      <c r="C46" s="699" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="690"/>
+      <c r="D46" s="700"/>
       <c r="E46" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15685,10 +15685,10 @@
       <c r="B47" s="57">
         <v>4700</v>
       </c>
-      <c r="C47" s="689" t="s">
+      <c r="C47" s="699" t="s">
         <v>1410</v>
       </c>
-      <c r="D47" s="690"/>
+      <c r="D47" s="700"/>
       <c r="E47" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15725,10 +15725,10 @@
       <c r="B48" s="57">
         <v>4800</v>
       </c>
-      <c r="C48" s="703" t="s">
+      <c r="C48" s="774" t="s">
         <v>455</v>
       </c>
-      <c r="D48" s="704"/>
+      <c r="D48" s="775"/>
       <c r="E48" s="202" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15857,12 +15857,12 @@
       <c r="L53" s="74"/>
     </row>
     <row r="54" spans="1:15" s="46" customFormat="1" ht="44.25" customHeight="1">
-      <c r="B54" s="705" t="e">
+      <c r="B54" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C54" s="706"/>
-      <c r="D54" s="706"/>
+      <c r="C54" s="730"/>
+      <c r="D54" s="730"/>
       <c r="E54" s="79"/>
       <c r="F54" s="79"/>
       <c r="G54" s="30"/>
@@ -15894,12 +15894,12 @@
       <c r="L55" s="74"/>
     </row>
     <row r="56" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickBot="1">
-      <c r="B56" s="721" t="e">
+      <c r="B56" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C56" s="722"/>
-      <c r="D56" s="722"/>
+      <c r="C56" s="692"/>
+      <c r="D56" s="692"/>
       <c r="E56" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -15954,12 +15954,12 @@
       <c r="L58" s="74"/>
     </row>
     <row r="59" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B59" s="721" t="e">
+      <c r="B59" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C59" s="722"/>
-      <c r="D59" s="722"/>
+      <c r="C59" s="692"/>
+      <c r="D59" s="692"/>
       <c r="E59" s="79" t="s">
         <v>505</v>
       </c>
@@ -16030,10 +16030,10 @@
     </row>
     <row r="63" spans="1:15" s="46" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="B63" s="87"/>
-      <c r="C63" s="717" t="s">
+      <c r="C63" s="770" t="s">
         <v>473</v>
       </c>
-      <c r="D63" s="718"/>
+      <c r="D63" s="771"/>
       <c r="E63" s="48" t="s">
         <v>509</v>
       </c>
@@ -16047,16 +16047,16 @@
       <c r="K63" s="169">
         <v>1</v>
       </c>
-      <c r="L63" s="709" t="s">
+      <c r="L63" s="764" t="s">
         <v>1429</v>
       </c>
-      <c r="M63" s="709" t="s">
+      <c r="M63" s="764" t="s">
         <v>1430</v>
       </c>
-      <c r="N63" s="709" t="s">
+      <c r="N63" s="764" t="s">
         <v>1431</v>
       </c>
-      <c r="O63" s="709" t="s">
+      <c r="O63" s="764" t="s">
         <v>1432</v>
       </c>
     </row>
@@ -16064,10 +16064,10 @@
       <c r="B64" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="C64" s="701" t="s">
+      <c r="C64" s="711" t="s">
         <v>707</v>
       </c>
-      <c r="D64" s="714"/>
+      <c r="D64" s="767"/>
       <c r="E64" s="50">
         <v>2017</v>
       </c>
@@ -16089,17 +16089,17 @@
       <c r="K64" s="169">
         <v>1</v>
       </c>
-      <c r="L64" s="723"/>
-      <c r="M64" s="723"/>
-      <c r="N64" s="710"/>
-      <c r="O64" s="710"/>
+      <c r="L64" s="772"/>
+      <c r="M64" s="772"/>
+      <c r="N64" s="765"/>
+      <c r="O64" s="765"/>
     </row>
     <row r="65" spans="1:15" s="46" customFormat="1" ht="21.75" thickBot="1">
       <c r="B65" s="88"/>
-      <c r="C65" s="715" t="s">
+      <c r="C65" s="768" t="s">
         <v>387</v>
       </c>
-      <c r="D65" s="716"/>
+      <c r="D65" s="769"/>
       <c r="E65" s="10" t="s">
         <v>263</v>
       </c>
@@ -16121,10 +16121,10 @@
       <c r="K65" s="169">
         <v>1</v>
       </c>
-      <c r="L65" s="724"/>
-      <c r="M65" s="724"/>
-      <c r="N65" s="711"/>
-      <c r="O65" s="711"/>
+      <c r="L65" s="773"/>
+      <c r="M65" s="773"/>
+      <c r="N65" s="766"/>
+      <c r="O65" s="766"/>
     </row>
     <row r="66" spans="1:15" s="56" customFormat="1" ht="34.5" customHeight="1">
       <c r="A66" s="63">
@@ -16133,10 +16133,10 @@
       <c r="B66" s="54">
         <v>100</v>
       </c>
-      <c r="C66" s="725" t="s">
+      <c r="C66" s="752" t="s">
         <v>388</v>
       </c>
-      <c r="D66" s="726"/>
+      <c r="D66" s="732"/>
       <c r="E66" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16177,10 +16177,10 @@
       <c r="B67" s="57">
         <v>200</v>
       </c>
-      <c r="C67" s="707" t="s">
+      <c r="C67" s="695" t="s">
         <v>391</v>
       </c>
-      <c r="D67" s="708"/>
+      <c r="D67" s="696"/>
       <c r="E67" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16221,10 +16221,10 @@
       <c r="B68" s="57">
         <v>500</v>
       </c>
-      <c r="C68" s="689" t="s">
+      <c r="C68" s="699" t="s">
         <v>579</v>
       </c>
-      <c r="D68" s="690"/>
+      <c r="D68" s="700"/>
       <c r="E68" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16268,7 +16268,7 @@
       <c r="C69" s="697" t="s">
         <v>585</v>
       </c>
-      <c r="D69" s="727"/>
+      <c r="D69" s="698"/>
       <c r="E69" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16309,10 +16309,10 @@
       <c r="B70" s="57">
         <v>1000</v>
       </c>
-      <c r="C70" s="707" t="s">
+      <c r="C70" s="695" t="s">
         <v>586</v>
       </c>
-      <c r="D70" s="708"/>
+      <c r="D70" s="696"/>
       <c r="E70" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16353,10 +16353,10 @@
       <c r="B71" s="57">
         <v>1900</v>
       </c>
-      <c r="C71" s="719" t="s">
+      <c r="C71" s="693" t="s">
         <v>456</v>
       </c>
-      <c r="D71" s="720"/>
+      <c r="D71" s="694"/>
       <c r="E71" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16397,10 +16397,10 @@
       <c r="B72" s="57">
         <v>2100</v>
       </c>
-      <c r="C72" s="719" t="s">
+      <c r="C72" s="693" t="s">
         <v>741</v>
       </c>
-      <c r="D72" s="720"/>
+      <c r="D72" s="694"/>
       <c r="E72" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16441,10 +16441,10 @@
       <c r="B73" s="57">
         <v>2200</v>
       </c>
-      <c r="C73" s="719" t="s">
+      <c r="C73" s="693" t="s">
         <v>604</v>
       </c>
-      <c r="D73" s="720"/>
+      <c r="D73" s="694"/>
       <c r="E73" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16485,10 +16485,10 @@
       <c r="B74" s="57">
         <v>2500</v>
       </c>
-      <c r="C74" s="719" t="s">
+      <c r="C74" s="693" t="s">
         <v>606</v>
       </c>
-      <c r="D74" s="720"/>
+      <c r="D74" s="694"/>
       <c r="E74" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16529,10 +16529,10 @@
       <c r="B75" s="57">
         <v>2600</v>
       </c>
-      <c r="C75" s="712" t="s">
+      <c r="C75" s="701" t="s">
         <v>607</v>
       </c>
-      <c r="D75" s="713"/>
+      <c r="D75" s="702"/>
       <c r="E75" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16573,10 +16573,10 @@
       <c r="B76" s="57">
         <v>2700</v>
       </c>
-      <c r="C76" s="712" t="s">
+      <c r="C76" s="701" t="s">
         <v>608</v>
       </c>
-      <c r="D76" s="713"/>
+      <c r="D76" s="702"/>
       <c r="E76" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16617,10 +16617,10 @@
       <c r="B77" s="57">
         <v>2800</v>
       </c>
-      <c r="C77" s="712" t="s">
+      <c r="C77" s="701" t="s">
         <v>1408</v>
       </c>
-      <c r="D77" s="713"/>
+      <c r="D77" s="702"/>
       <c r="E77" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16661,10 +16661,10 @@
       <c r="B78" s="57">
         <v>2900</v>
       </c>
-      <c r="C78" s="719" t="s">
+      <c r="C78" s="693" t="s">
         <v>609</v>
       </c>
-      <c r="D78" s="720"/>
+      <c r="D78" s="694"/>
       <c r="E78" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16749,10 +16749,10 @@
       <c r="B80" s="57">
         <v>3900</v>
       </c>
-      <c r="C80" s="719" t="s">
+      <c r="C80" s="693" t="s">
         <v>618</v>
       </c>
-      <c r="D80" s="720"/>
+      <c r="D80" s="694"/>
       <c r="E80" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16793,10 +16793,10 @@
       <c r="B81" s="57">
         <v>4000</v>
       </c>
-      <c r="C81" s="719" t="s">
+      <c r="C81" s="693" t="s">
         <v>619</v>
       </c>
-      <c r="D81" s="720"/>
+      <c r="D81" s="694"/>
       <c r="E81" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16837,10 +16837,10 @@
       <c r="B82" s="57">
         <v>4100</v>
       </c>
-      <c r="C82" s="719" t="s">
+      <c r="C82" s="693" t="s">
         <v>620</v>
       </c>
-      <c r="D82" s="720"/>
+      <c r="D82" s="694"/>
       <c r="E82" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16881,10 +16881,10 @@
       <c r="B83" s="57">
         <v>4200</v>
       </c>
-      <c r="C83" s="719" t="s">
+      <c r="C83" s="693" t="s">
         <v>621</v>
       </c>
-      <c r="D83" s="720"/>
+      <c r="D83" s="694"/>
       <c r="E83" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16925,10 +16925,10 @@
       <c r="B84" s="57">
         <v>4300</v>
       </c>
-      <c r="C84" s="719" t="s">
+      <c r="C84" s="693" t="s">
         <v>1015</v>
       </c>
-      <c r="D84" s="720"/>
+      <c r="D84" s="694"/>
       <c r="E84" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16969,10 +16969,10 @@
       <c r="B85" s="57">
         <v>4400</v>
       </c>
-      <c r="C85" s="719" t="s">
+      <c r="C85" s="693" t="s">
         <v>1012</v>
       </c>
-      <c r="D85" s="720"/>
+      <c r="D85" s="694"/>
       <c r="E85" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17013,10 +17013,10 @@
       <c r="B86" s="57">
         <v>4500</v>
       </c>
-      <c r="C86" s="719" t="s">
+      <c r="C86" s="693" t="s">
         <v>1409</v>
       </c>
-      <c r="D86" s="720"/>
+      <c r="D86" s="694"/>
       <c r="E86" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17057,10 +17057,10 @@
       <c r="B87" s="57">
         <v>4600</v>
       </c>
-      <c r="C87" s="712" t="s">
+      <c r="C87" s="701" t="s">
         <v>630</v>
       </c>
-      <c r="D87" s="713"/>
+      <c r="D87" s="702"/>
       <c r="E87" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17101,10 +17101,10 @@
       <c r="B88" s="57">
         <v>4900</v>
       </c>
-      <c r="C88" s="719" t="s">
+      <c r="C88" s="693" t="s">
         <v>460</v>
       </c>
-      <c r="D88" s="720"/>
+      <c r="D88" s="694"/>
       <c r="E88" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17145,10 +17145,10 @@
       <c r="B89" s="96">
         <v>5100</v>
       </c>
-      <c r="C89" s="728" t="s">
+      <c r="C89" s="757" t="s">
         <v>631</v>
       </c>
-      <c r="D89" s="729"/>
+      <c r="D89" s="758"/>
       <c r="E89" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17189,10 +17189,10 @@
       <c r="B90" s="96">
         <v>5200</v>
       </c>
-      <c r="C90" s="728" t="s">
+      <c r="C90" s="757" t="s">
         <v>632</v>
       </c>
-      <c r="D90" s="729"/>
+      <c r="D90" s="758"/>
       <c r="E90" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17233,10 +17233,10 @@
       <c r="B91" s="96">
         <v>5300</v>
       </c>
-      <c r="C91" s="728" t="s">
+      <c r="C91" s="757" t="s">
         <v>191</v>
       </c>
-      <c r="D91" s="729"/>
+      <c r="D91" s="758"/>
       <c r="E91" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17277,10 +17277,10 @@
       <c r="B92" s="96">
         <v>5400</v>
       </c>
-      <c r="C92" s="728" t="s">
+      <c r="C92" s="757" t="s">
         <v>643</v>
       </c>
-      <c r="D92" s="729"/>
+      <c r="D92" s="758"/>
       <c r="E92" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17321,10 +17321,10 @@
       <c r="B93" s="57">
         <v>5500</v>
       </c>
-      <c r="C93" s="719" t="s">
+      <c r="C93" s="693" t="s">
         <v>644</v>
       </c>
-      <c r="D93" s="720"/>
+      <c r="D93" s="694"/>
       <c r="E93" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17365,10 +17365,10 @@
       <c r="B94" s="96">
         <v>5700</v>
       </c>
-      <c r="C94" s="730" t="s">
+      <c r="C94" s="759" t="s">
         <v>649</v>
       </c>
-      <c r="D94" s="731"/>
+      <c r="D94" s="760"/>
       <c r="E94" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17409,10 +17409,10 @@
       <c r="B95" s="98" t="s">
         <v>708</v>
       </c>
-      <c r="C95" s="732" t="s">
+      <c r="C95" s="761" t="s">
         <v>653</v>
       </c>
-      <c r="D95" s="733"/>
+      <c r="D95" s="762"/>
       <c r="E95" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17451,10 +17451,10 @@
         <v>825</v>
       </c>
       <c r="B96" s="104"/>
-      <c r="C96" s="734" t="s">
+      <c r="C96" s="763" t="s">
         <v>654</v>
       </c>
-      <c r="D96" s="734"/>
+      <c r="D96" s="763"/>
       <c r="E96" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17520,12 +17520,12 @@
     </row>
     <row r="99" spans="1:11" ht="40.5" customHeight="1">
       <c r="A99" s="70"/>
-      <c r="B99" s="705" t="e">
+      <c r="B99" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C99" s="706"/>
-      <c r="D99" s="706"/>
+      <c r="C99" s="730"/>
+      <c r="D99" s="730"/>
       <c r="E99" s="79"/>
       <c r="F99" s="79"/>
       <c r="K99" s="167">
@@ -17548,12 +17548,12 @@
     </row>
     <row r="101" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A101" s="70"/>
-      <c r="B101" s="721" t="e">
+      <c r="B101" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C101" s="722"/>
-      <c r="D101" s="722"/>
+      <c r="C101" s="692"/>
+      <c r="D101" s="692"/>
       <c r="E101" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -17592,12 +17592,12 @@
     </row>
     <row r="104" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A104" s="70"/>
-      <c r="B104" s="721" t="e">
+      <c r="B104" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C104" s="722"/>
-      <c r="D104" s="722"/>
+      <c r="C104" s="692"/>
+      <c r="D104" s="692"/>
       <c r="E104" s="79" t="s">
         <v>505</v>
       </c>
@@ -17647,10 +17647,10 @@
     <row r="108" spans="1:11" ht="21.75" thickBot="1">
       <c r="A108" s="70"/>
       <c r="B108" s="138"/>
-      <c r="C108" s="744" t="s">
+      <c r="C108" s="743" t="s">
         <v>908</v>
       </c>
-      <c r="D108" s="745"/>
+      <c r="D108" s="753"/>
       <c r="E108" s="48" t="s">
         <v>509</v>
       </c>
@@ -17670,10 +17670,10 @@
       <c r="B109" s="107" t="s">
         <v>474</v>
       </c>
-      <c r="C109" s="746" t="s">
+      <c r="C109" s="754" t="s">
         <v>707</v>
       </c>
-      <c r="D109" s="747"/>
+      <c r="D109" s="755"/>
       <c r="E109" s="50">
         <v>2017</v>
       </c>
@@ -17701,10 +17701,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="748" t="s">
+      <c r="C110" s="740" t="s">
         <v>251</v>
       </c>
-      <c r="D110" s="749"/>
+      <c r="D110" s="741"/>
       <c r="E110" s="10" t="s">
         <v>263</v>
       </c>
@@ -17732,10 +17732,10 @@
         <v>2</v>
       </c>
       <c r="B111" s="14"/>
-      <c r="C111" s="750" t="s">
+      <c r="C111" s="756" t="s">
         <v>463</v>
       </c>
-      <c r="D111" s="749"/>
+      <c r="D111" s="741"/>
       <c r="E111" s="12"/>
       <c r="F111" s="29"/>
       <c r="G111" s="29"/>
@@ -17753,10 +17753,10 @@
       <c r="B112" s="54">
         <v>3000</v>
       </c>
-      <c r="C112" s="751" t="s">
+      <c r="C112" s="736" t="s">
         <v>909</v>
       </c>
-      <c r="D112" s="752"/>
+      <c r="D112" s="737"/>
       <c r="E112" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17793,10 +17793,10 @@
       <c r="B113" s="57">
         <v>3100</v>
       </c>
-      <c r="C113" s="689" t="s">
+      <c r="C113" s="699" t="s">
         <v>464</v>
       </c>
-      <c r="D113" s="690"/>
+      <c r="D113" s="700"/>
       <c r="E113" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17833,10 +17833,10 @@
       <c r="B114" s="110">
         <v>3200</v>
       </c>
-      <c r="C114" s="735" t="s">
+      <c r="C114" s="745" t="s">
         <v>758</v>
       </c>
-      <c r="D114" s="736"/>
+      <c r="D114" s="690"/>
       <c r="E114" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17873,10 +17873,10 @@
       <c r="B115" s="57">
         <v>6000</v>
       </c>
-      <c r="C115" s="725" t="s">
+      <c r="C115" s="752" t="s">
         <v>635</v>
       </c>
-      <c r="D115" s="726"/>
+      <c r="D115" s="732"/>
       <c r="E115" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17913,10 +17913,10 @@
       <c r="B116" s="57">
         <v>6100</v>
       </c>
-      <c r="C116" s="707" t="s">
+      <c r="C116" s="695" t="s">
         <v>636</v>
       </c>
-      <c r="D116" s="708"/>
+      <c r="D116" s="696"/>
       <c r="E116" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17953,10 +17953,10 @@
       <c r="B117" s="57">
         <v>6200</v>
       </c>
-      <c r="C117" s="754" t="s">
+      <c r="C117" s="728" t="s">
         <v>637</v>
       </c>
-      <c r="D117" s="755"/>
+      <c r="D117" s="733"/>
       <c r="E117" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17993,10 +17993,10 @@
       <c r="B118" s="57">
         <v>6300</v>
       </c>
-      <c r="C118" s="741" t="s">
+      <c r="C118" s="725" t="s">
         <v>638</v>
       </c>
-      <c r="D118" s="713"/>
+      <c r="D118" s="702"/>
       <c r="E118" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18033,10 +18033,10 @@
       <c r="B119" s="57">
         <v>6400</v>
       </c>
-      <c r="C119" s="739" t="s">
+      <c r="C119" s="748" t="s">
         <v>639</v>
       </c>
-      <c r="D119" s="740"/>
+      <c r="D119" s="749"/>
       <c r="E119" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18131,10 +18131,10 @@
       <c r="B121" s="57">
         <v>6600</v>
       </c>
-      <c r="C121" s="741" t="s">
+      <c r="C121" s="725" t="s">
         <v>254</v>
       </c>
-      <c r="D121" s="713"/>
+      <c r="D121" s="702"/>
       <c r="E121" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18171,10 +18171,10 @@
       <c r="B122" s="57">
         <v>6700</v>
       </c>
-      <c r="C122" s="741" t="s">
+      <c r="C122" s="725" t="s">
         <v>687</v>
       </c>
-      <c r="D122" s="713"/>
+      <c r="D122" s="702"/>
       <c r="E122" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18211,10 +18211,10 @@
       <c r="B123" s="57">
         <v>6900</v>
       </c>
-      <c r="C123" s="742" t="s">
+      <c r="C123" s="750" t="s">
         <v>640</v>
       </c>
-      <c r="D123" s="743"/>
+      <c r="D123" s="751"/>
       <c r="E123" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18249,10 +18249,10 @@
         <v>260</v>
       </c>
       <c r="B124" s="71"/>
-      <c r="C124" s="758" t="s">
+      <c r="C124" s="738" t="s">
         <v>252</v>
       </c>
-      <c r="D124" s="759"/>
+      <c r="D124" s="739"/>
       <c r="E124" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18286,10 +18286,10 @@
         <v>261</v>
       </c>
       <c r="B125" s="112"/>
-      <c r="C125" s="748" t="s">
+      <c r="C125" s="740" t="s">
         <v>253</v>
       </c>
-      <c r="D125" s="749"/>
+      <c r="D125" s="741"/>
       <c r="E125" s="113"/>
       <c r="F125" s="170"/>
       <c r="G125" s="170"/>
@@ -18307,10 +18307,10 @@
       <c r="B126" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C126" s="756" t="s">
+      <c r="C126" s="734" t="s">
         <v>899</v>
       </c>
-      <c r="D126" s="757"/>
+      <c r="D126" s="735"/>
       <c r="E126" s="170"/>
       <c r="F126" s="170"/>
       <c r="G126" s="170"/>
@@ -18328,10 +18328,10 @@
       <c r="B127" s="57">
         <v>7400</v>
       </c>
-      <c r="C127" s="751" t="s">
+      <c r="C127" s="736" t="s">
         <v>900</v>
       </c>
-      <c r="D127" s="752"/>
+      <c r="D127" s="737"/>
       <c r="E127" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18368,10 +18368,10 @@
       <c r="B128" s="57">
         <v>7500</v>
       </c>
-      <c r="C128" s="689" t="s">
+      <c r="C128" s="699" t="s">
         <v>710</v>
       </c>
-      <c r="D128" s="690"/>
+      <c r="D128" s="700"/>
       <c r="E128" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18411,7 +18411,7 @@
       <c r="C129" s="697" t="s">
         <v>641</v>
       </c>
-      <c r="D129" s="698"/>
+      <c r="D129" s="742"/>
       <c r="E129" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18451,7 +18451,7 @@
       <c r="C130" s="697" t="s">
         <v>642</v>
       </c>
-      <c r="D130" s="727"/>
+      <c r="D130" s="698"/>
       <c r="E130" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18488,10 +18488,10 @@
       <c r="B131" s="96">
         <v>7800</v>
       </c>
-      <c r="C131" s="737" t="s">
-        <v>0</v>
-      </c>
-      <c r="D131" s="738"/>
+      <c r="C131" s="746" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="747"/>
       <c r="E131" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18526,10 +18526,10 @@
         <v>315</v>
       </c>
       <c r="B132" s="71"/>
-      <c r="C132" s="758" t="s">
+      <c r="C132" s="738" t="s">
         <v>898</v>
       </c>
-      <c r="D132" s="759"/>
+      <c r="D132" s="739"/>
       <c r="E132" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18587,12 +18587,12 @@
     </row>
     <row r="136" spans="1:11" ht="42" customHeight="1">
       <c r="A136" s="103"/>
-      <c r="B136" s="705" t="e">
+      <c r="B136" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C136" s="706"/>
-      <c r="D136" s="706"/>
+      <c r="C136" s="730"/>
+      <c r="D136" s="730"/>
       <c r="E136" s="79"/>
       <c r="F136" s="79"/>
       <c r="K136" s="167">
@@ -18615,12 +18615,12 @@
     </row>
     <row r="138" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A138" s="103"/>
-      <c r="B138" s="721" t="e">
+      <c r="B138" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C138" s="722"/>
-      <c r="D138" s="722"/>
+      <c r="C138" s="692"/>
+      <c r="D138" s="692"/>
       <c r="E138" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18659,12 +18659,12 @@
     </row>
     <row r="141" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A141" s="103"/>
-      <c r="B141" s="721" t="e">
+      <c r="B141" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C141" s="722"/>
-      <c r="D141" s="722"/>
+      <c r="C141" s="692"/>
+      <c r="D141" s="692"/>
       <c r="E141" s="79" t="s">
         <v>505</v>
       </c>
@@ -18854,12 +18854,12 @@
     </row>
     <row r="152" spans="1:11" ht="44.25" customHeight="1">
       <c r="A152" s="103"/>
-      <c r="B152" s="705" t="e">
+      <c r="B152" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C152" s="706"/>
-      <c r="D152" s="706"/>
+      <c r="C152" s="730"/>
+      <c r="D152" s="730"/>
       <c r="E152" s="79"/>
       <c r="F152" s="79"/>
       <c r="K152" s="167">
@@ -18882,12 +18882,12 @@
     </row>
     <row r="154" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A154" s="103"/>
-      <c r="B154" s="721" t="e">
+      <c r="B154" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C154" s="722"/>
-      <c r="D154" s="722"/>
+      <c r="C154" s="692"/>
+      <c r="D154" s="692"/>
       <c r="E154" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18926,12 +18926,12 @@
     </row>
     <row r="157" spans="1:11" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A157" s="103"/>
-      <c r="B157" s="721" t="e">
+      <c r="B157" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C157" s="722"/>
-      <c r="D157" s="722"/>
+      <c r="C157" s="692"/>
+      <c r="D157" s="692"/>
       <c r="E157" s="79" t="s">
         <v>505</v>
       </c>
@@ -18981,10 +18981,10 @@
     <row r="161" spans="1:65" ht="21.75" thickBot="1">
       <c r="A161" s="103"/>
       <c r="B161" s="112"/>
-      <c r="C161" s="744" t="s">
+      <c r="C161" s="743" t="s">
         <v>684</v>
       </c>
-      <c r="D161" s="702"/>
+      <c r="D161" s="710"/>
       <c r="E161" s="48" t="s">
         <v>509</v>
       </c>
@@ -19004,10 +19004,10 @@
       <c r="B162" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C162" s="701" t="s">
+      <c r="C162" s="711" t="s">
         <v>707</v>
       </c>
-      <c r="D162" s="700"/>
+      <c r="D162" s="708"/>
       <c r="E162" s="50">
         <v>2017</v>
       </c>
@@ -19035,10 +19035,10 @@
         <v>1</v>
       </c>
       <c r="B163" s="139"/>
-      <c r="C163" s="779" t="s">
+      <c r="C163" s="744" t="s">
         <v>685</v>
       </c>
-      <c r="D163" s="749"/>
+      <c r="D163" s="741"/>
       <c r="E163" s="10" t="s">
         <v>263</v>
       </c>
@@ -19068,10 +19068,10 @@
       <c r="B164" s="54">
         <v>7000</v>
       </c>
-      <c r="C164" s="753" t="s">
+      <c r="C164" s="731" t="s">
         <v>902</v>
       </c>
-      <c r="D164" s="726"/>
+      <c r="D164" s="732"/>
       <c r="E164" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19108,10 +19108,10 @@
       <c r="B165" s="57">
         <v>7100</v>
       </c>
-      <c r="C165" s="719" t="s">
+      <c r="C165" s="693" t="s">
         <v>903</v>
       </c>
-      <c r="D165" s="720"/>
+      <c r="D165" s="694"/>
       <c r="E165" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19148,10 +19148,10 @@
       <c r="B166" s="57">
         <v>7200</v>
       </c>
-      <c r="C166" s="719" t="s">
+      <c r="C166" s="693" t="s">
         <v>1414</v>
       </c>
-      <c r="D166" s="720"/>
+      <c r="D166" s="694"/>
       <c r="E166" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19188,10 +19188,10 @@
       <c r="B167" s="57">
         <v>7300</v>
       </c>
-      <c r="C167" s="712" t="s">
+      <c r="C167" s="701" t="s">
         <v>904</v>
       </c>
-      <c r="D167" s="713"/>
+      <c r="D167" s="702"/>
       <c r="E167" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19228,10 +19228,10 @@
       <c r="B168" s="57">
         <v>7900</v>
       </c>
-      <c r="C168" s="781" t="s">
+      <c r="C168" s="703" t="s">
         <v>905</v>
       </c>
-      <c r="D168" s="782"/>
+      <c r="D168" s="704"/>
       <c r="E168" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19321,10 +19321,10 @@
       <c r="B169" s="57">
         <v>8000</v>
       </c>
-      <c r="C169" s="707" t="s">
+      <c r="C169" s="695" t="s">
         <v>711</v>
       </c>
-      <c r="D169" s="708"/>
+      <c r="D169" s="696"/>
       <c r="E169" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19364,7 +19364,7 @@
       <c r="C170" s="697" t="s">
         <v>712</v>
       </c>
-      <c r="D170" s="727"/>
+      <c r="D170" s="698"/>
       <c r="E170" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19404,7 +19404,7 @@
       <c r="C171" s="697" t="s">
         <v>101</v>
       </c>
-      <c r="D171" s="727"/>
+      <c r="D171" s="698"/>
       <c r="E171" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19441,10 +19441,10 @@
       <c r="B172" s="57">
         <v>8300</v>
       </c>
-      <c r="C172" s="689" t="s">
+      <c r="C172" s="699" t="s">
         <v>713</v>
       </c>
-      <c r="D172" s="690"/>
+      <c r="D172" s="700"/>
       <c r="E172" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19481,10 +19481,10 @@
       <c r="B173" s="57">
         <v>8500</v>
       </c>
-      <c r="C173" s="707" t="s">
+      <c r="C173" s="695" t="s">
         <v>102</v>
       </c>
-      <c r="D173" s="708"/>
+      <c r="D173" s="696"/>
       <c r="E173" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19521,10 +19521,10 @@
       <c r="B174" s="57">
         <v>8600</v>
       </c>
-      <c r="C174" s="707" t="s">
+      <c r="C174" s="695" t="s">
         <v>103</v>
       </c>
-      <c r="D174" s="708"/>
+      <c r="D174" s="696"/>
       <c r="E174" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19564,7 +19564,7 @@
       <c r="C175" s="697" t="s">
         <v>265</v>
       </c>
-      <c r="D175" s="727"/>
+      <c r="D175" s="698"/>
       <c r="E175" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19604,7 +19604,7 @@
       <c r="C176" s="697" t="s">
         <v>910</v>
       </c>
-      <c r="D176" s="727"/>
+      <c r="D176" s="698"/>
       <c r="E176" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19641,10 +19641,10 @@
       <c r="B177" s="57">
         <v>8900</v>
       </c>
-      <c r="C177" s="741" t="s">
+      <c r="C177" s="725" t="s">
         <v>759</v>
       </c>
-      <c r="D177" s="713"/>
+      <c r="D177" s="702"/>
       <c r="E177" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19681,10 +19681,10 @@
       <c r="B178" s="57">
         <v>9000</v>
       </c>
-      <c r="C178" s="707" t="s">
+      <c r="C178" s="695" t="s">
         <v>104</v>
       </c>
-      <c r="D178" s="708"/>
+      <c r="D178" s="696"/>
       <c r="E178" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19721,10 +19721,10 @@
       <c r="B179" s="57">
         <v>9100</v>
       </c>
-      <c r="C179" s="741" t="s">
+      <c r="C179" s="725" t="s">
         <v>911</v>
       </c>
-      <c r="D179" s="754"/>
+      <c r="D179" s="728"/>
       <c r="E179" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19761,10 +19761,10 @@
       <c r="B180" s="57">
         <v>9200</v>
       </c>
-      <c r="C180" s="777" t="s">
+      <c r="C180" s="726" t="s">
         <v>714</v>
       </c>
-      <c r="D180" s="727"/>
+      <c r="D180" s="698"/>
       <c r="E180" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19801,10 +19801,10 @@
       <c r="B181" s="57">
         <v>9300</v>
       </c>
-      <c r="C181" s="707" t="s">
+      <c r="C181" s="695" t="s">
         <v>715</v>
       </c>
-      <c r="D181" s="708"/>
+      <c r="D181" s="696"/>
       <c r="E181" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19841,10 +19841,10 @@
       <c r="B182" s="57">
         <v>9500</v>
       </c>
-      <c r="C182" s="777" t="s">
+      <c r="C182" s="726" t="s">
         <v>716</v>
       </c>
-      <c r="D182" s="778"/>
+      <c r="D182" s="727"/>
       <c r="E182" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19881,10 +19881,10 @@
       <c r="B183" s="57">
         <v>9600</v>
       </c>
-      <c r="C183" s="777" t="s">
+      <c r="C183" s="726" t="s">
         <v>717</v>
       </c>
-      <c r="D183" s="727"/>
+      <c r="D183" s="698"/>
       <c r="E183" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19921,10 +19921,10 @@
       <c r="B184" s="57">
         <v>9800</v>
       </c>
-      <c r="C184" s="780" t="s">
+      <c r="C184" s="689" t="s">
         <v>465</v>
       </c>
-      <c r="D184" s="736"/>
+      <c r="D184" s="690"/>
       <c r="E184" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19959,10 +19959,10 @@
         <v>610</v>
       </c>
       <c r="B185" s="146"/>
-      <c r="C185" s="701" t="s">
+      <c r="C185" s="711" t="s">
         <v>930</v>
       </c>
-      <c r="D185" s="700"/>
+      <c r="D185" s="708"/>
       <c r="E185" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -20025,12 +20025,12 @@
       </c>
     </row>
     <row r="189" spans="1:11" ht="42" customHeight="1">
-      <c r="B189" s="705" t="e">
+      <c r="B189" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C189" s="706"/>
-      <c r="D189" s="706"/>
+      <c r="C189" s="730"/>
+      <c r="D189" s="730"/>
       <c r="E189" s="79"/>
       <c r="F189" s="79"/>
       <c r="G189" s="56"/>
@@ -20053,12 +20053,12 @@
       </c>
     </row>
     <row r="191" spans="1:11" ht="21.75" thickBot="1">
-      <c r="B191" s="721" t="e">
+      <c r="B191" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C191" s="722"/>
-      <c r="D191" s="722"/>
+      <c r="C191" s="692"/>
+      <c r="D191" s="692"/>
       <c r="E191" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -20097,12 +20097,12 @@
       </c>
     </row>
     <row r="194" spans="2:11" ht="22.5" thickTop="1" thickBot="1">
-      <c r="B194" s="721" t="e">
+      <c r="B194" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C194" s="722"/>
-      <c r="D194" s="722"/>
+      <c r="C194" s="692"/>
+      <c r="D194" s="692"/>
       <c r="E194" s="79" t="s">
         <v>505</v>
       </c>
@@ -20156,10 +20156,10 @@
       <c r="B198" s="153" t="s">
         <v>474</v>
       </c>
-      <c r="C198" s="762" t="s">
+      <c r="C198" s="707" t="s">
         <v>718</v>
       </c>
-      <c r="D198" s="700"/>
+      <c r="D198" s="708"/>
       <c r="E198" s="48" t="s">
         <v>509</v>
       </c>
@@ -20176,8 +20176,8 @@
     </row>
     <row r="199" spans="2:11" ht="45.75" thickBot="1">
       <c r="B199" s="154"/>
-      <c r="C199" s="763"/>
-      <c r="D199" s="702"/>
+      <c r="C199" s="709"/>
+      <c r="D199" s="710"/>
       <c r="E199" s="50">
         <v>2017</v>
       </c>
@@ -20204,10 +20204,10 @@
       <c r="B200" s="155" t="s">
         <v>719</v>
       </c>
-      <c r="C200" s="775" t="s">
+      <c r="C200" s="723" t="s">
         <v>720</v>
       </c>
-      <c r="D200" s="776"/>
+      <c r="D200" s="724"/>
       <c r="E200" s="187" t="e">
         <f>SUMIF(#REF!,1,#REF!)</f>
         <v>#REF!</v>
@@ -20240,10 +20240,10 @@
       <c r="B201" s="156" t="s">
         <v>721</v>
       </c>
-      <c r="C201" s="768" t="s">
+      <c r="C201" s="716" t="s">
         <v>722</v>
       </c>
-      <c r="D201" s="769"/>
+      <c r="D201" s="717"/>
       <c r="E201" s="188" t="e">
         <f>SUMIF(#REF!,2,#REF!)</f>
         <v>#REF!</v>
@@ -20276,10 +20276,10 @@
       <c r="B202" s="156" t="s">
         <v>723</v>
       </c>
-      <c r="C202" s="768" t="s">
+      <c r="C202" s="716" t="s">
         <v>724</v>
       </c>
-      <c r="D202" s="769"/>
+      <c r="D202" s="717"/>
       <c r="E202" s="188" t="e">
         <f>SUMIF(#REF!,3,#REF!)</f>
         <v>#REF!</v>
@@ -20312,10 +20312,10 @@
       <c r="B203" s="156" t="s">
         <v>725</v>
       </c>
-      <c r="C203" s="771" t="s">
+      <c r="C203" s="719" t="s">
         <v>726</v>
       </c>
-      <c r="D203" s="772"/>
+      <c r="D203" s="720"/>
       <c r="E203" s="188" t="e">
         <f>SUMIF(#REF!,4,#REF!)</f>
         <v>#REF!</v>
@@ -20348,10 +20348,10 @@
       <c r="B204" s="156" t="s">
         <v>727</v>
       </c>
-      <c r="C204" s="773" t="s">
+      <c r="C204" s="721" t="s">
         <v>728</v>
       </c>
-      <c r="D204" s="774"/>
+      <c r="D204" s="722"/>
       <c r="E204" s="188" t="e">
         <f>SUMIF(#REF!,5,#REF!)</f>
         <v>#REF!</v>
@@ -20384,10 +20384,10 @@
       <c r="B205" s="156" t="s">
         <v>729</v>
       </c>
-      <c r="C205" s="770" t="s">
+      <c r="C205" s="718" t="s">
         <v>730</v>
       </c>
-      <c r="D205" s="770"/>
+      <c r="D205" s="718"/>
       <c r="E205" s="188" t="e">
         <f>SUMIF(#REF!,6,#REF!)</f>
         <v>#REF!</v>
@@ -20420,10 +20420,10 @@
       <c r="B206" s="156" t="s">
         <v>731</v>
       </c>
-      <c r="C206" s="764" t="s">
+      <c r="C206" s="712" t="s">
         <v>732</v>
       </c>
-      <c r="D206" s="765"/>
+      <c r="D206" s="713"/>
       <c r="E206" s="188" t="e">
         <f>SUMIF(#REF!,7,#REF!)</f>
         <v>#REF!</v>
@@ -20456,10 +20456,10 @@
       <c r="B207" s="156" t="s">
         <v>733</v>
       </c>
-      <c r="C207" s="764" t="s">
+      <c r="C207" s="712" t="s">
         <v>734</v>
       </c>
-      <c r="D207" s="765"/>
+      <c r="D207" s="713"/>
       <c r="E207" s="188" t="e">
         <f>SUMIF(#REF!,8,#REF!)</f>
         <v>#REF!</v>
@@ -20492,10 +20492,10 @@
       <c r="B208" s="156" t="s">
         <v>735</v>
       </c>
-      <c r="C208" s="766" t="s">
+      <c r="C208" s="714" t="s">
         <v>736</v>
       </c>
-      <c r="D208" s="767"/>
+      <c r="D208" s="715"/>
       <c r="E208" s="189" t="e">
         <f>SUMIF(#REF!,9,#REF!)</f>
         <v>#REF!</v>
@@ -20526,10 +20526,10 @@
     </row>
     <row r="209" spans="2:11" ht="21.75" thickBot="1">
       <c r="B209" s="157"/>
-      <c r="C209" s="760" t="s">
+      <c r="C209" s="705" t="s">
         <v>737</v>
       </c>
-      <c r="D209" s="761"/>
+      <c r="D209" s="706"/>
       <c r="E209" s="158" t="e">
         <f t="shared" ref="E209:J209" si="5">SUM(E200:E208)</f>
         <v>#REF!</v>
@@ -22138,17 +22138,116 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="145">
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C172:D172"/>
-    <mergeCell ref="C173:D173"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="N63:N65"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="O63:O65"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="L63:L65"/>
+    <mergeCell ref="M63:M65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C161:D161"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="C163:D163"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="B152:D152"/>
+    <mergeCell ref="B154:D154"/>
     <mergeCell ref="C209:D209"/>
     <mergeCell ref="C198:D198"/>
     <mergeCell ref="C199:D199"/>
@@ -22173,116 +22272,17 @@
     <mergeCell ref="B189:D189"/>
     <mergeCell ref="B194:D194"/>
     <mergeCell ref="C183:D183"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="C164:D164"/>
-    <mergeCell ref="C165:D165"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C161:D161"/>
-    <mergeCell ref="C162:D162"/>
-    <mergeCell ref="C163:D163"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="B136:D136"/>
-    <mergeCell ref="B138:D138"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B152:D152"/>
-    <mergeCell ref="B154:D154"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="N63:N65"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="O63:O65"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="L63:L65"/>
-    <mergeCell ref="M63:M65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
@@ -22335,7 +22335,7 @@
   <dimension ref="A1:Y44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -22485,12 +22485,12 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="209"/>
-      <c r="B7" s="793" t="str">
+      <c r="B7" s="783" t="str">
         <f>VLOOKUP(E8,SMETKA,2,FALSE)</f>
         <v>ОТЧЕТНИ ДАННИ ПО ЕБК ЗА ИЗПЪЛНЕНИЕТО НА БЮДЖЕТА</v>
       </c>
-      <c r="C7" s="794"/>
-      <c r="D7" s="794"/>
+      <c r="C7" s="784"/>
+      <c r="D7" s="784"/>
       <c r="E7" s="337"/>
       <c r="F7" s="337"/>
       <c r="G7" s="337"/>
@@ -22589,11 +22589,11 @@
     </row>
     <row r="13" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="210"/>
-      <c r="B13" s="787" t="s">
+      <c r="B13" s="789" t="s">
         <v>1498</v>
       </c>
-      <c r="C13" s="788"/>
-      <c r="D13" s="789"/>
+      <c r="C13" s="790"/>
+      <c r="D13" s="791"/>
       <c r="E13" s="338">
         <v>44927</v>
       </c>
@@ -22645,11 +22645,11 @@
     </row>
     <row r="16" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="790" t="s">
+      <c r="B16" s="792" t="s">
         <v>1498</v>
       </c>
-      <c r="C16" s="791"/>
-      <c r="D16" s="792"/>
+      <c r="C16" s="793"/>
+      <c r="D16" s="794"/>
       <c r="E16" s="356"/>
       <c r="F16" s="587"/>
       <c r="G16" s="326"/>
@@ -22827,10 +22827,10 @@
       <c r="B24" s="395">
         <v>100</v>
       </c>
-      <c r="C24" s="784" t="s">
+      <c r="C24" s="786" t="s">
         <v>388</v>
       </c>
-      <c r="D24" s="785"/>
+      <c r="D24" s="787"/>
       <c r="E24" s="241">
         <f>SUMIF($B$43:$B$44,$B24,E$43:E$44)</f>
         <v>0</v>
@@ -23092,10 +23092,10 @@
       <c r="B31" s="395">
         <v>1000</v>
       </c>
-      <c r="C31" s="786" t="s">
+      <c r="C31" s="788" t="s">
         <v>586</v>
       </c>
-      <c r="D31" s="786"/>
+      <c r="D31" s="788"/>
       <c r="E31" s="243">
         <v>0</v>
       </c>
@@ -23236,10 +23236,10 @@
       <c r="B35" s="449" t="s">
         <v>1499</v>
       </c>
-      <c r="C35" s="783" t="s">
+      <c r="C35" s="785" t="s">
         <v>1500</v>
       </c>
-      <c r="D35" s="783"/>
+      <c r="D35" s="785"/>
       <c r="E35" s="243">
         <v>0</v>
       </c>
@@ -23453,7 +23453,7 @@
         <v>944</v>
       </c>
       <c r="E42" s="247">
-        <f>SUMIF($C$43:$C$44,$C42,E$43:E$44)</f>
+        <f>E24+E31+E35</f>
         <v>0</v>
       </c>
       <c r="F42" s="248">
@@ -23728,12 +23728,12 @@
         <v>3</v>
       </c>
       <c r="H14" s="328"/>
-      <c r="I14" s="797">
+      <c r="I14" s="800">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J14" s="798"/>
-      <c r="K14" s="798"/>
+      <c r="J14" s="801"/>
+      <c r="K14" s="801"/>
       <c r="L14" s="346"/>
       <c r="M14" s="346"/>
       <c r="N14" s="347"/>
@@ -23777,12 +23777,12 @@
         <v>5</v>
       </c>
       <c r="H16" s="328"/>
-      <c r="I16" s="799">
+      <c r="I16" s="802">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J16" s="800"/>
-      <c r="K16" s="801"/>
+      <c r="J16" s="803"/>
+      <c r="K16" s="804"/>
       <c r="L16" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -23849,12 +23849,12 @@
         <v>8</v>
       </c>
       <c r="H19" s="328"/>
-      <c r="I19" s="802">
+      <c r="I19" s="805">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J19" s="803"/>
-      <c r="K19" s="804"/>
+      <c r="J19" s="806"/>
+      <c r="K19" s="807"/>
       <c r="L19" s="356" t="s">
         <v>934</v>
       </c>
@@ -24149,10 +24149,10 @@
       <c r="I30" s="395">
         <v>100</v>
       </c>
-      <c r="J30" s="784" t="s">
+      <c r="J30" s="786" t="s">
         <v>388</v>
       </c>
-      <c r="K30" s="785"/>
+      <c r="K30" s="787"/>
       <c r="L30" s="241">
         <f t="shared" ref="L30:Q30" si="0">SUM(L31:L32)</f>
         <v>0</v>
@@ -24245,10 +24245,10 @@
       <c r="I33" s="395">
         <v>200</v>
       </c>
-      <c r="J33" s="786" t="s">
+      <c r="J33" s="788" t="s">
         <v>391</v>
       </c>
-      <c r="K33" s="786"/>
+      <c r="K33" s="788"/>
       <c r="L33" s="241">
         <f t="shared" ref="L33:Q33" si="2">SUM(L34:L38)</f>
         <v>0</v>
@@ -24422,10 +24422,10 @@
       <c r="I39" s="395">
         <v>500</v>
       </c>
-      <c r="J39" s="796" t="s">
+      <c r="J39" s="813" t="s">
         <v>579</v>
       </c>
-      <c r="K39" s="796"/>
+      <c r="K39" s="813"/>
       <c r="L39" s="241">
         <f t="shared" ref="L39:Q39" si="3">SUM(L40:L46)</f>
         <v>0</v>
@@ -24694,10 +24694,10 @@
       <c r="I47" s="395">
         <v>800</v>
       </c>
-      <c r="J47" s="807" t="s">
+      <c r="J47" s="809" t="s">
         <v>698</v>
       </c>
-      <c r="K47" s="808"/>
+      <c r="K47" s="810"/>
       <c r="L47" s="567"/>
       <c r="M47" s="244">
         <f t="shared" si="4"/>
@@ -24721,10 +24721,10 @@
       <c r="I48" s="395">
         <v>1000</v>
       </c>
-      <c r="J48" s="786" t="s">
+      <c r="J48" s="788" t="s">
         <v>586</v>
       </c>
-      <c r="K48" s="786"/>
+      <c r="K48" s="788"/>
       <c r="L48" s="243">
         <f t="shared" ref="L48:Q48" si="5">SUM(L49:L65)</f>
         <v>0</v>
@@ -25652,7 +25652,7 @@
       <c r="J79" s="795" t="s">
         <v>606</v>
       </c>
-      <c r="K79" s="809"/>
+      <c r="K79" s="811"/>
       <c r="L79" s="567"/>
       <c r="M79" s="244">
         <f t="shared" si="10"/>
@@ -25676,10 +25676,10 @@
       <c r="I80" s="395">
         <v>2600</v>
       </c>
-      <c r="J80" s="805" t="s">
+      <c r="J80" s="812" t="s">
         <v>607</v>
       </c>
-      <c r="K80" s="785"/>
+      <c r="K80" s="787"/>
       <c r="L80" s="567"/>
       <c r="M80" s="244">
         <f t="shared" si="10"/>
@@ -25703,10 +25703,10 @@
       <c r="I81" s="395">
         <v>2700</v>
       </c>
-      <c r="J81" s="805" t="s">
+      <c r="J81" s="812" t="s">
         <v>608</v>
       </c>
-      <c r="K81" s="785"/>
+      <c r="K81" s="787"/>
       <c r="L81" s="567"/>
       <c r="M81" s="244">
         <f t="shared" si="10"/>
@@ -25730,10 +25730,10 @@
       <c r="I82" s="395">
         <v>2800</v>
       </c>
-      <c r="J82" s="805" t="s">
+      <c r="J82" s="812" t="s">
         <v>1011</v>
       </c>
-      <c r="K82" s="785"/>
+      <c r="K82" s="787"/>
       <c r="L82" s="567"/>
       <c r="M82" s="244">
         <f t="shared" si="10"/>
@@ -26674,10 +26674,10 @@
       <c r="I114" s="395">
         <v>4600</v>
       </c>
-      <c r="J114" s="805" t="s">
+      <c r="J114" s="812" t="s">
         <v>630</v>
       </c>
-      <c r="K114" s="785"/>
+      <c r="K114" s="787"/>
       <c r="L114" s="567"/>
       <c r="M114" s="244">
         <f t="shared" si="19"/>
@@ -26797,10 +26797,10 @@
       <c r="I118" s="449">
         <v>5100</v>
       </c>
-      <c r="J118" s="783" t="s">
+      <c r="J118" s="785" t="s">
         <v>631</v>
       </c>
-      <c r="K118" s="783"/>
+      <c r="K118" s="785"/>
       <c r="L118" s="567"/>
       <c r="M118" s="244">
         <f>N118+O118+P118+Q118</f>
@@ -26824,10 +26824,10 @@
       <c r="I119" s="449">
         <v>5200</v>
       </c>
-      <c r="J119" s="783" t="s">
+      <c r="J119" s="785" t="s">
         <v>632</v>
       </c>
-      <c r="K119" s="783"/>
+      <c r="K119" s="785"/>
       <c r="L119" s="243">
         <f t="shared" ref="L119:Q119" si="21">SUM(L120:L126)</f>
         <v>0</v>
@@ -27055,10 +27055,10 @@
       <c r="I127" s="449">
         <v>5300</v>
       </c>
-      <c r="J127" s="783" t="s">
+      <c r="J127" s="785" t="s">
         <v>191</v>
       </c>
-      <c r="K127" s="783"/>
+      <c r="K127" s="785"/>
       <c r="L127" s="243">
         <f t="shared" ref="L127:Q127" si="23">SUM(L128:L129)</f>
         <v>0</v>
@@ -27151,10 +27151,10 @@
       <c r="I130" s="449">
         <v>5400</v>
       </c>
-      <c r="J130" s="783" t="s">
+      <c r="J130" s="785" t="s">
         <v>643</v>
       </c>
-      <c r="K130" s="783"/>
+      <c r="K130" s="785"/>
       <c r="L130" s="567"/>
       <c r="M130" s="244">
         <f>N130+O130+P130+Q130</f>
@@ -27328,10 +27328,10 @@
       <c r="I136" s="449">
         <v>5700</v>
       </c>
-      <c r="J136" s="810" t="s">
+      <c r="J136" s="796" t="s">
         <v>943</v>
       </c>
-      <c r="K136" s="811"/>
+      <c r="K136" s="797"/>
       <c r="L136" s="243">
         <f t="shared" ref="L136:Q136" si="25">SUM(L137:L139)</f>
         <v>0</v>
@@ -27471,10 +27471,10 @@
       <c r="I141" s="464">
         <v>98</v>
       </c>
-      <c r="J141" s="812" t="s">
+      <c r="J141" s="798" t="s">
         <v>653</v>
       </c>
-      <c r="K141" s="813"/>
+      <c r="K141" s="799"/>
       <c r="L141" s="573"/>
       <c r="M141" s="324">
         <f>N141+O141+P141+Q141</f>
@@ -27670,12 +27670,12 @@
         <v>138</v>
       </c>
       <c r="H149" s="328"/>
-      <c r="I149" s="797">
+      <c r="I149" s="800">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J149" s="798"/>
-      <c r="K149" s="798"/>
+      <c r="J149" s="801"/>
+      <c r="K149" s="801"/>
       <c r="L149" s="326"/>
       <c r="M149" s="326"/>
       <c r="N149" s="326"/>
@@ -27717,12 +27717,12 @@
         <v>140</v>
       </c>
       <c r="H151" s="328"/>
-      <c r="I151" s="799">
+      <c r="I151" s="802">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J151" s="800"/>
-      <c r="K151" s="801"/>
+      <c r="J151" s="803"/>
+      <c r="K151" s="804"/>
       <c r="L151" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -27789,12 +27789,12 @@
         <v>143</v>
       </c>
       <c r="H154" s="328"/>
-      <c r="I154" s="802">
+      <c r="I154" s="805">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J154" s="803"/>
-      <c r="K154" s="804"/>
+      <c r="J154" s="806"/>
+      <c r="K154" s="807"/>
       <c r="L154" s="356" t="s">
         <v>934</v>
       </c>
@@ -28592,11 +28592,11 @@
         <v>175</v>
       </c>
       <c r="H186" s="328"/>
-      <c r="I186" s="806" t="s">
+      <c r="I186" s="808" t="s">
         <v>249</v>
       </c>
-      <c r="J186" s="806"/>
-      <c r="K186" s="806"/>
+      <c r="J186" s="808"/>
+      <c r="K186" s="808"/>
       <c r="L186" s="327"/>
       <c r="M186" s="327"/>
       <c r="N186" s="327"/>
@@ -29938,11 +29938,21 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="36">
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="I149:K149"/>
     <mergeCell ref="I151:K151"/>
     <mergeCell ref="I154:K154"/>
@@ -29959,21 +29969,11 @@
     <mergeCell ref="J99:K99"/>
     <mergeCell ref="J100:K100"/>
     <mergeCell ref="J114:K114"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J141:K141"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L156:M156">

</xml_diff>

<commit_message>
Payments now cannot accumulate to exceed their respective limits.
</commit_message>
<xml_diff>
--- a/PaymentsBudgetSystem/wwwroot/Report.xlsx
+++ b/PaymentsBudgetSystem/wwwroot/Report.xlsx
@@ -817,7 +817,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1511">
   <si>
     <t>Временни безлихвени заеми от/за държавни предприятия и други сметки, включени в консолидираната фискална програма (нето)</t>
   </si>
@@ -8057,9 +8057,6 @@
     <t>Министерство на електронното управление</t>
   </si>
   <si>
-    <t>Име</t>
-  </si>
-  <si>
     <t>50-00</t>
   </si>
   <si>
@@ -8096,9 +8093,6 @@
     <t>Придобиване на стопански инвентар</t>
   </si>
   <si>
-    <t>Наименование на първостепенния разпоредител с бюджет</t>
-  </si>
-  <si>
     <t>Наименование разпоредителя с бюджет</t>
   </si>
   <si>
@@ -8133,6 +8127,9 @@
       </rPr>
       <t>Държавното обществено осигуряване (ДОО)</t>
     </r>
+  </si>
+  <si>
+    <t>Вид на отчета</t>
   </si>
 </sst>
 </file>
@@ -13019,261 +13016,10 @@
     <xf numFmtId="3" fontId="13" fillId="12" borderId="102" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -13296,9 +13042,260 @@
     <xf numFmtId="0" fontId="45" fillId="5" borderId="114" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -13338,17 +13335,11 @@
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -13388,9 +13379,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -14443,12 +14440,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="42" customHeight="1">
-      <c r="B7" s="776" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="777"/>
-      <c r="D7" s="777"/>
+      <c r="B7" s="691" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C7" s="692"/>
+      <c r="D7" s="692"/>
       <c r="F7" s="38"/>
       <c r="K7" s="167">
         <v>1</v>
@@ -14468,12 +14465,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="36.75" customHeight="1" thickBot="1">
-      <c r="B9" s="778" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="779"/>
-      <c r="D9" s="779"/>
+      <c r="B9" s="693" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="694"/>
+      <c r="D9" s="694"/>
       <c r="E9" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14508,12 +14505,12 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="39" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B12" s="778" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C12" s="779"/>
-      <c r="D12" s="779"/>
+      <c r="B12" s="693" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C12" s="694"/>
+      <c r="D12" s="694"/>
       <c r="E12" s="38" t="s">
         <v>505</v>
       </c>
@@ -14588,10 +14585,10 @@
     <row r="19" spans="1:11" ht="21.75" thickBot="1">
       <c r="A19" s="46"/>
       <c r="B19" s="47"/>
-      <c r="C19" s="782" t="s">
+      <c r="C19" s="699" t="s">
         <v>508</v>
       </c>
-      <c r="D19" s="708"/>
+      <c r="D19" s="700"/>
       <c r="E19" s="48" t="s">
         <v>509</v>
       </c>
@@ -14610,10 +14607,10 @@
       <c r="B20" s="49" t="s">
         <v>474</v>
       </c>
-      <c r="C20" s="711" t="s">
+      <c r="C20" s="701" t="s">
         <v>705</v>
       </c>
-      <c r="D20" s="710"/>
+      <c r="D20" s="702"/>
       <c r="E20" s="50">
         <v>2017</v>
       </c>
@@ -14638,10 +14635,10 @@
     </row>
     <row r="21" spans="1:11" ht="21.75" thickBot="1">
       <c r="B21" s="51"/>
-      <c r="C21" s="744" t="s">
+      <c r="C21" s="703" t="s">
         <v>512</v>
       </c>
-      <c r="D21" s="741"/>
+      <c r="D21" s="704"/>
       <c r="E21" s="10" t="s">
         <v>263</v>
       </c>
@@ -14671,10 +14668,10 @@
       <c r="B22" s="54">
         <v>100</v>
       </c>
-      <c r="C22" s="780" t="s">
+      <c r="C22" s="695" t="s">
         <v>513</v>
       </c>
-      <c r="D22" s="781"/>
+      <c r="D22" s="696"/>
       <c r="E22" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14711,10 +14708,10 @@
       <c r="B23" s="57">
         <v>200</v>
       </c>
-      <c r="C23" s="699" t="s">
+      <c r="C23" s="689" t="s">
         <v>514</v>
       </c>
-      <c r="D23" s="700"/>
+      <c r="D23" s="690"/>
       <c r="E23" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14754,7 +14751,7 @@
       <c r="C24" s="697" t="s">
         <v>515</v>
       </c>
-      <c r="D24" s="742"/>
+      <c r="D24" s="698"/>
       <c r="E24" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14791,10 +14788,10 @@
       <c r="B25" s="57">
         <v>800</v>
       </c>
-      <c r="C25" s="699" t="s">
+      <c r="C25" s="689" t="s">
         <v>924</v>
       </c>
-      <c r="D25" s="700"/>
+      <c r="D25" s="690"/>
       <c r="E25" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14831,10 +14828,10 @@
       <c r="B26" s="57">
         <v>1000</v>
       </c>
-      <c r="C26" s="699" t="s">
+      <c r="C26" s="689" t="s">
         <v>516</v>
       </c>
-      <c r="D26" s="700"/>
+      <c r="D26" s="690"/>
       <c r="E26" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14871,10 +14868,10 @@
       <c r="B27" s="57">
         <v>1300</v>
       </c>
-      <c r="C27" s="699" t="s">
+      <c r="C27" s="689" t="s">
         <v>706</v>
       </c>
-      <c r="D27" s="700"/>
+      <c r="D27" s="690"/>
       <c r="E27" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14911,10 +14908,10 @@
       <c r="B28" s="57">
         <v>1400</v>
       </c>
-      <c r="C28" s="699" t="s">
+      <c r="C28" s="689" t="s">
         <v>517</v>
       </c>
-      <c r="D28" s="700"/>
+      <c r="D28" s="690"/>
       <c r="E28" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14951,10 +14948,10 @@
       <c r="B29" s="57">
         <v>1500</v>
       </c>
-      <c r="C29" s="699" t="s">
+      <c r="C29" s="689" t="s">
         <v>518</v>
       </c>
-      <c r="D29" s="700"/>
+      <c r="D29" s="690"/>
       <c r="E29" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14988,10 +14985,10 @@
       <c r="B30" s="57">
         <v>1600</v>
       </c>
-      <c r="C30" s="699" t="s">
+      <c r="C30" s="689" t="s">
         <v>519</v>
       </c>
-      <c r="D30" s="700"/>
+      <c r="D30" s="690"/>
       <c r="E30" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15028,10 +15025,10 @@
       <c r="B31" s="57">
         <v>1700</v>
       </c>
-      <c r="C31" s="699" t="s">
+      <c r="C31" s="689" t="s">
         <v>520</v>
       </c>
-      <c r="D31" s="700"/>
+      <c r="D31" s="690"/>
       <c r="E31" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15068,10 +15065,10 @@
       <c r="B32" s="57">
         <v>1800</v>
       </c>
-      <c r="C32" s="699" t="s">
+      <c r="C32" s="689" t="s">
         <v>521</v>
       </c>
-      <c r="D32" s="700"/>
+      <c r="D32" s="690"/>
       <c r="E32" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15108,10 +15105,10 @@
       <c r="B33" s="57">
         <v>1900</v>
       </c>
-      <c r="C33" s="699" t="s">
+      <c r="C33" s="689" t="s">
         <v>522</v>
       </c>
-      <c r="D33" s="700"/>
+      <c r="D33" s="690"/>
       <c r="E33" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15148,10 +15145,10 @@
       <c r="B34" s="57">
         <v>2000</v>
       </c>
-      <c r="C34" s="699" t="s">
+      <c r="C34" s="689" t="s">
         <v>523</v>
       </c>
-      <c r="D34" s="700"/>
+      <c r="D34" s="690"/>
       <c r="E34" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15188,10 +15185,10 @@
       <c r="B35" s="57">
         <v>2400</v>
       </c>
-      <c r="C35" s="699" t="s">
+      <c r="C35" s="689" t="s">
         <v>524</v>
       </c>
-      <c r="D35" s="700"/>
+      <c r="D35" s="690"/>
       <c r="E35" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15228,10 +15225,10 @@
       <c r="B36" s="62">
         <v>2500</v>
       </c>
-      <c r="C36" s="695" t="s">
+      <c r="C36" s="709" t="s">
         <v>525</v>
       </c>
-      <c r="D36" s="696"/>
+      <c r="D36" s="710"/>
       <c r="E36" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15268,10 +15265,10 @@
       <c r="B37" s="57">
         <v>2600</v>
       </c>
-      <c r="C37" s="695" t="s">
+      <c r="C37" s="709" t="s">
         <v>300</v>
       </c>
-      <c r="D37" s="696"/>
+      <c r="D37" s="710"/>
       <c r="E37" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15308,10 +15305,10 @@
       <c r="B38" s="57">
         <v>2700</v>
       </c>
-      <c r="C38" s="699" t="s">
+      <c r="C38" s="689" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="700"/>
+      <c r="D38" s="690"/>
       <c r="E38" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15348,10 +15345,10 @@
       <c r="B39" s="57">
         <v>2800</v>
       </c>
-      <c r="C39" s="699" t="s">
+      <c r="C39" s="689" t="s">
         <v>529</v>
       </c>
-      <c r="D39" s="700"/>
+      <c r="D39" s="690"/>
       <c r="E39" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15388,10 +15385,10 @@
       <c r="B40" s="57">
         <v>3600</v>
       </c>
-      <c r="C40" s="699" t="s">
+      <c r="C40" s="689" t="s">
         <v>530</v>
       </c>
-      <c r="D40" s="700"/>
+      <c r="D40" s="690"/>
       <c r="E40" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15428,10 +15425,10 @@
       <c r="B41" s="57">
         <v>3700</v>
       </c>
-      <c r="C41" s="699" t="s">
+      <c r="C41" s="689" t="s">
         <v>531</v>
       </c>
-      <c r="D41" s="700"/>
+      <c r="D41" s="690"/>
       <c r="E41" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15522,10 +15519,10 @@
       <c r="B43" s="57">
         <v>4100</v>
       </c>
-      <c r="C43" s="699" t="s">
+      <c r="C43" s="689" t="s">
         <v>381</v>
       </c>
-      <c r="D43" s="700"/>
+      <c r="D43" s="690"/>
       <c r="E43" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15563,10 +15560,10 @@
       <c r="B44" s="57">
         <v>4200</v>
       </c>
-      <c r="C44" s="699" t="s">
+      <c r="C44" s="689" t="s">
         <v>382</v>
       </c>
-      <c r="D44" s="700"/>
+      <c r="D44" s="690"/>
       <c r="E44" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15604,10 +15601,10 @@
       <c r="B45" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="C45" s="699" t="s">
+      <c r="C45" s="689" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="700"/>
+      <c r="D45" s="690"/>
       <c r="E45" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15645,10 +15642,10 @@
       <c r="B46" s="57">
         <v>4600</v>
       </c>
-      <c r="C46" s="699" t="s">
+      <c r="C46" s="689" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="700"/>
+      <c r="D46" s="690"/>
       <c r="E46" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15685,10 +15682,10 @@
       <c r="B47" s="57">
         <v>4700</v>
       </c>
-      <c r="C47" s="699" t="s">
+      <c r="C47" s="689" t="s">
         <v>1410</v>
       </c>
-      <c r="D47" s="700"/>
+      <c r="D47" s="690"/>
       <c r="E47" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15725,10 +15722,10 @@
       <c r="B48" s="57">
         <v>4800</v>
       </c>
-      <c r="C48" s="774" t="s">
+      <c r="C48" s="705" t="s">
         <v>455</v>
       </c>
-      <c r="D48" s="775"/>
+      <c r="D48" s="706"/>
       <c r="E48" s="202" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15857,12 +15854,12 @@
       <c r="L53" s="74"/>
     </row>
     <row r="54" spans="1:15" s="46" customFormat="1" ht="44.25" customHeight="1">
-      <c r="B54" s="729" t="e">
+      <c r="B54" s="707" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C54" s="730"/>
-      <c r="D54" s="730"/>
+      <c r="C54" s="708"/>
+      <c r="D54" s="708"/>
       <c r="E54" s="79"/>
       <c r="F54" s="79"/>
       <c r="G54" s="30"/>
@@ -15894,12 +15891,12 @@
       <c r="L55" s="74"/>
     </row>
     <row r="56" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickBot="1">
-      <c r="B56" s="691" t="e">
+      <c r="B56" s="723" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C56" s="692"/>
-      <c r="D56" s="692"/>
+      <c r="C56" s="724"/>
+      <c r="D56" s="724"/>
       <c r="E56" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -15954,12 +15951,12 @@
       <c r="L58" s="74"/>
     </row>
     <row r="59" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B59" s="691" t="e">
+      <c r="B59" s="723" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C59" s="692"/>
-      <c r="D59" s="692"/>
+      <c r="C59" s="724"/>
+      <c r="D59" s="724"/>
       <c r="E59" s="79" t="s">
         <v>505</v>
       </c>
@@ -16030,10 +16027,10 @@
     </row>
     <row r="63" spans="1:15" s="46" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="B63" s="87"/>
-      <c r="C63" s="770" t="s">
+      <c r="C63" s="719" t="s">
         <v>473</v>
       </c>
-      <c r="D63" s="771"/>
+      <c r="D63" s="720"/>
       <c r="E63" s="48" t="s">
         <v>509</v>
       </c>
@@ -16047,16 +16044,16 @@
       <c r="K63" s="169">
         <v>1</v>
       </c>
-      <c r="L63" s="764" t="s">
+      <c r="L63" s="711" t="s">
         <v>1429</v>
       </c>
-      <c r="M63" s="764" t="s">
+      <c r="M63" s="711" t="s">
         <v>1430</v>
       </c>
-      <c r="N63" s="764" t="s">
+      <c r="N63" s="711" t="s">
         <v>1431</v>
       </c>
-      <c r="O63" s="764" t="s">
+      <c r="O63" s="711" t="s">
         <v>1432</v>
       </c>
     </row>
@@ -16064,10 +16061,10 @@
       <c r="B64" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="C64" s="711" t="s">
+      <c r="C64" s="701" t="s">
         <v>707</v>
       </c>
-      <c r="D64" s="767"/>
+      <c r="D64" s="716"/>
       <c r="E64" s="50">
         <v>2017</v>
       </c>
@@ -16089,17 +16086,17 @@
       <c r="K64" s="169">
         <v>1</v>
       </c>
-      <c r="L64" s="772"/>
-      <c r="M64" s="772"/>
-      <c r="N64" s="765"/>
-      <c r="O64" s="765"/>
+      <c r="L64" s="725"/>
+      <c r="M64" s="725"/>
+      <c r="N64" s="712"/>
+      <c r="O64" s="712"/>
     </row>
     <row r="65" spans="1:15" s="46" customFormat="1" ht="21.75" thickBot="1">
       <c r="B65" s="88"/>
-      <c r="C65" s="768" t="s">
+      <c r="C65" s="717" t="s">
         <v>387</v>
       </c>
-      <c r="D65" s="769"/>
+      <c r="D65" s="718"/>
       <c r="E65" s="10" t="s">
         <v>263</v>
       </c>
@@ -16121,10 +16118,10 @@
       <c r="K65" s="169">
         <v>1</v>
       </c>
-      <c r="L65" s="773"/>
-      <c r="M65" s="773"/>
-      <c r="N65" s="766"/>
-      <c r="O65" s="766"/>
+      <c r="L65" s="726"/>
+      <c r="M65" s="726"/>
+      <c r="N65" s="713"/>
+      <c r="O65" s="713"/>
     </row>
     <row r="66" spans="1:15" s="56" customFormat="1" ht="34.5" customHeight="1">
       <c r="A66" s="63">
@@ -16133,10 +16130,10 @@
       <c r="B66" s="54">
         <v>100</v>
       </c>
-      <c r="C66" s="752" t="s">
+      <c r="C66" s="727" t="s">
         <v>388</v>
       </c>
-      <c r="D66" s="732"/>
+      <c r="D66" s="728"/>
       <c r="E66" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16177,10 +16174,10 @@
       <c r="B67" s="57">
         <v>200</v>
       </c>
-      <c r="C67" s="695" t="s">
+      <c r="C67" s="709" t="s">
         <v>391</v>
       </c>
-      <c r="D67" s="696"/>
+      <c r="D67" s="710"/>
       <c r="E67" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16221,10 +16218,10 @@
       <c r="B68" s="57">
         <v>500</v>
       </c>
-      <c r="C68" s="699" t="s">
+      <c r="C68" s="689" t="s">
         <v>579</v>
       </c>
-      <c r="D68" s="700"/>
+      <c r="D68" s="690"/>
       <c r="E68" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16268,7 +16265,7 @@
       <c r="C69" s="697" t="s">
         <v>585</v>
       </c>
-      <c r="D69" s="698"/>
+      <c r="D69" s="729"/>
       <c r="E69" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16309,10 +16306,10 @@
       <c r="B70" s="57">
         <v>1000</v>
       </c>
-      <c r="C70" s="695" t="s">
+      <c r="C70" s="709" t="s">
         <v>586</v>
       </c>
-      <c r="D70" s="696"/>
+      <c r="D70" s="710"/>
       <c r="E70" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16353,10 +16350,10 @@
       <c r="B71" s="57">
         <v>1900</v>
       </c>
-      <c r="C71" s="693" t="s">
+      <c r="C71" s="721" t="s">
         <v>456</v>
       </c>
-      <c r="D71" s="694"/>
+      <c r="D71" s="722"/>
       <c r="E71" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16397,10 +16394,10 @@
       <c r="B72" s="57">
         <v>2100</v>
       </c>
-      <c r="C72" s="693" t="s">
+      <c r="C72" s="721" t="s">
         <v>741</v>
       </c>
-      <c r="D72" s="694"/>
+      <c r="D72" s="722"/>
       <c r="E72" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16441,10 +16438,10 @@
       <c r="B73" s="57">
         <v>2200</v>
       </c>
-      <c r="C73" s="693" t="s">
+      <c r="C73" s="721" t="s">
         <v>604</v>
       </c>
-      <c r="D73" s="694"/>
+      <c r="D73" s="722"/>
       <c r="E73" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16485,10 +16482,10 @@
       <c r="B74" s="57">
         <v>2500</v>
       </c>
-      <c r="C74" s="693" t="s">
+      <c r="C74" s="721" t="s">
         <v>606</v>
       </c>
-      <c r="D74" s="694"/>
+      <c r="D74" s="722"/>
       <c r="E74" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16529,10 +16526,10 @@
       <c r="B75" s="57">
         <v>2600</v>
       </c>
-      <c r="C75" s="701" t="s">
+      <c r="C75" s="714" t="s">
         <v>607</v>
       </c>
-      <c r="D75" s="702"/>
+      <c r="D75" s="715"/>
       <c r="E75" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16573,10 +16570,10 @@
       <c r="B76" s="57">
         <v>2700</v>
       </c>
-      <c r="C76" s="701" t="s">
+      <c r="C76" s="714" t="s">
         <v>608</v>
       </c>
-      <c r="D76" s="702"/>
+      <c r="D76" s="715"/>
       <c r="E76" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16617,10 +16614,10 @@
       <c r="B77" s="57">
         <v>2800</v>
       </c>
-      <c r="C77" s="701" t="s">
+      <c r="C77" s="714" t="s">
         <v>1408</v>
       </c>
-      <c r="D77" s="702"/>
+      <c r="D77" s="715"/>
       <c r="E77" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16661,10 +16658,10 @@
       <c r="B78" s="57">
         <v>2900</v>
       </c>
-      <c r="C78" s="693" t="s">
+      <c r="C78" s="721" t="s">
         <v>609</v>
       </c>
-      <c r="D78" s="694"/>
+      <c r="D78" s="722"/>
       <c r="E78" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16749,10 +16746,10 @@
       <c r="B80" s="57">
         <v>3900</v>
       </c>
-      <c r="C80" s="693" t="s">
+      <c r="C80" s="721" t="s">
         <v>618</v>
       </c>
-      <c r="D80" s="694"/>
+      <c r="D80" s="722"/>
       <c r="E80" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16793,10 +16790,10 @@
       <c r="B81" s="57">
         <v>4000</v>
       </c>
-      <c r="C81" s="693" t="s">
+      <c r="C81" s="721" t="s">
         <v>619</v>
       </c>
-      <c r="D81" s="694"/>
+      <c r="D81" s="722"/>
       <c r="E81" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16837,10 +16834,10 @@
       <c r="B82" s="57">
         <v>4100</v>
       </c>
-      <c r="C82" s="693" t="s">
+      <c r="C82" s="721" t="s">
         <v>620</v>
       </c>
-      <c r="D82" s="694"/>
+      <c r="D82" s="722"/>
       <c r="E82" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16881,10 +16878,10 @@
       <c r="B83" s="57">
         <v>4200</v>
       </c>
-      <c r="C83" s="693" t="s">
+      <c r="C83" s="721" t="s">
         <v>621</v>
       </c>
-      <c r="D83" s="694"/>
+      <c r="D83" s="722"/>
       <c r="E83" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16925,10 +16922,10 @@
       <c r="B84" s="57">
         <v>4300</v>
       </c>
-      <c r="C84" s="693" t="s">
+      <c r="C84" s="721" t="s">
         <v>1015</v>
       </c>
-      <c r="D84" s="694"/>
+      <c r="D84" s="722"/>
       <c r="E84" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16969,10 +16966,10 @@
       <c r="B85" s="57">
         <v>4400</v>
       </c>
-      <c r="C85" s="693" t="s">
+      <c r="C85" s="721" t="s">
         <v>1012</v>
       </c>
-      <c r="D85" s="694"/>
+      <c r="D85" s="722"/>
       <c r="E85" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17013,10 +17010,10 @@
       <c r="B86" s="57">
         <v>4500</v>
       </c>
-      <c r="C86" s="693" t="s">
+      <c r="C86" s="721" t="s">
         <v>1409</v>
       </c>
-      <c r="D86" s="694"/>
+      <c r="D86" s="722"/>
       <c r="E86" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17057,10 +17054,10 @@
       <c r="B87" s="57">
         <v>4600</v>
       </c>
-      <c r="C87" s="701" t="s">
+      <c r="C87" s="714" t="s">
         <v>630</v>
       </c>
-      <c r="D87" s="702"/>
+      <c r="D87" s="715"/>
       <c r="E87" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17101,10 +17098,10 @@
       <c r="B88" s="57">
         <v>4900</v>
       </c>
-      <c r="C88" s="693" t="s">
+      <c r="C88" s="721" t="s">
         <v>460</v>
       </c>
-      <c r="D88" s="694"/>
+      <c r="D88" s="722"/>
       <c r="E88" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17145,10 +17142,10 @@
       <c r="B89" s="96">
         <v>5100</v>
       </c>
-      <c r="C89" s="757" t="s">
+      <c r="C89" s="730" t="s">
         <v>631</v>
       </c>
-      <c r="D89" s="758"/>
+      <c r="D89" s="731"/>
       <c r="E89" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17189,10 +17186,10 @@
       <c r="B90" s="96">
         <v>5200</v>
       </c>
-      <c r="C90" s="757" t="s">
+      <c r="C90" s="730" t="s">
         <v>632</v>
       </c>
-      <c r="D90" s="758"/>
+      <c r="D90" s="731"/>
       <c r="E90" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17233,10 +17230,10 @@
       <c r="B91" s="96">
         <v>5300</v>
       </c>
-      <c r="C91" s="757" t="s">
+      <c r="C91" s="730" t="s">
         <v>191</v>
       </c>
-      <c r="D91" s="758"/>
+      <c r="D91" s="731"/>
       <c r="E91" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17277,10 +17274,10 @@
       <c r="B92" s="96">
         <v>5400</v>
       </c>
-      <c r="C92" s="757" t="s">
+      <c r="C92" s="730" t="s">
         <v>643</v>
       </c>
-      <c r="D92" s="758"/>
+      <c r="D92" s="731"/>
       <c r="E92" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17321,10 +17318,10 @@
       <c r="B93" s="57">
         <v>5500</v>
       </c>
-      <c r="C93" s="693" t="s">
+      <c r="C93" s="721" t="s">
         <v>644</v>
       </c>
-      <c r="D93" s="694"/>
+      <c r="D93" s="722"/>
       <c r="E93" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17365,10 +17362,10 @@
       <c r="B94" s="96">
         <v>5700</v>
       </c>
-      <c r="C94" s="759" t="s">
+      <c r="C94" s="732" t="s">
         <v>649</v>
       </c>
-      <c r="D94" s="760"/>
+      <c r="D94" s="733"/>
       <c r="E94" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17409,10 +17406,10 @@
       <c r="B95" s="98" t="s">
         <v>708</v>
       </c>
-      <c r="C95" s="761" t="s">
+      <c r="C95" s="734" t="s">
         <v>653</v>
       </c>
-      <c r="D95" s="762"/>
+      <c r="D95" s="735"/>
       <c r="E95" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17451,10 +17448,10 @@
         <v>825</v>
       </c>
       <c r="B96" s="104"/>
-      <c r="C96" s="763" t="s">
+      <c r="C96" s="736" t="s">
         <v>654</v>
       </c>
-      <c r="D96" s="763"/>
+      <c r="D96" s="736"/>
       <c r="E96" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17520,12 +17517,12 @@
     </row>
     <row r="99" spans="1:11" ht="40.5" customHeight="1">
       <c r="A99" s="70"/>
-      <c r="B99" s="729" t="e">
+      <c r="B99" s="707" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C99" s="730"/>
-      <c r="D99" s="730"/>
+      <c r="C99" s="708"/>
+      <c r="D99" s="708"/>
       <c r="E99" s="79"/>
       <c r="F99" s="79"/>
       <c r="K99" s="167">
@@ -17548,12 +17545,12 @@
     </row>
     <row r="101" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A101" s="70"/>
-      <c r="B101" s="691" t="e">
+      <c r="B101" s="723" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C101" s="692"/>
-      <c r="D101" s="692"/>
+      <c r="C101" s="724"/>
+      <c r="D101" s="724"/>
       <c r="E101" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -17592,12 +17589,12 @@
     </row>
     <row r="104" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A104" s="70"/>
-      <c r="B104" s="691" t="e">
+      <c r="B104" s="723" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C104" s="692"/>
-      <c r="D104" s="692"/>
+      <c r="C104" s="724"/>
+      <c r="D104" s="724"/>
       <c r="E104" s="79" t="s">
         <v>505</v>
       </c>
@@ -17647,10 +17644,10 @@
     <row r="108" spans="1:11" ht="21.75" thickBot="1">
       <c r="A108" s="70"/>
       <c r="B108" s="138"/>
-      <c r="C108" s="743" t="s">
+      <c r="C108" s="746" t="s">
         <v>908</v>
       </c>
-      <c r="D108" s="753"/>
+      <c r="D108" s="747"/>
       <c r="E108" s="48" t="s">
         <v>509</v>
       </c>
@@ -17670,10 +17667,10 @@
       <c r="B109" s="107" t="s">
         <v>474</v>
       </c>
-      <c r="C109" s="754" t="s">
+      <c r="C109" s="748" t="s">
         <v>707</v>
       </c>
-      <c r="D109" s="755"/>
+      <c r="D109" s="749"/>
       <c r="E109" s="50">
         <v>2017</v>
       </c>
@@ -17701,10 +17698,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="740" t="s">
+      <c r="C110" s="750" t="s">
         <v>251</v>
       </c>
-      <c r="D110" s="741"/>
+      <c r="D110" s="704"/>
       <c r="E110" s="10" t="s">
         <v>263</v>
       </c>
@@ -17732,10 +17729,10 @@
         <v>2</v>
       </c>
       <c r="B111" s="14"/>
-      <c r="C111" s="756" t="s">
+      <c r="C111" s="751" t="s">
         <v>463</v>
       </c>
-      <c r="D111" s="741"/>
+      <c r="D111" s="704"/>
       <c r="E111" s="12"/>
       <c r="F111" s="29"/>
       <c r="G111" s="29"/>
@@ -17753,10 +17750,10 @@
       <c r="B112" s="54">
         <v>3000</v>
       </c>
-      <c r="C112" s="736" t="s">
+      <c r="C112" s="752" t="s">
         <v>909</v>
       </c>
-      <c r="D112" s="737"/>
+      <c r="D112" s="753"/>
       <c r="E112" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17793,10 +17790,10 @@
       <c r="B113" s="57">
         <v>3100</v>
       </c>
-      <c r="C113" s="699" t="s">
+      <c r="C113" s="689" t="s">
         <v>464</v>
       </c>
-      <c r="D113" s="700"/>
+      <c r="D113" s="690"/>
       <c r="E113" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17833,10 +17830,10 @@
       <c r="B114" s="110">
         <v>3200</v>
       </c>
-      <c r="C114" s="745" t="s">
+      <c r="C114" s="737" t="s">
         <v>758</v>
       </c>
-      <c r="D114" s="690"/>
+      <c r="D114" s="738"/>
       <c r="E114" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17873,10 +17870,10 @@
       <c r="B115" s="57">
         <v>6000</v>
       </c>
-      <c r="C115" s="752" t="s">
+      <c r="C115" s="727" t="s">
         <v>635</v>
       </c>
-      <c r="D115" s="732"/>
+      <c r="D115" s="728"/>
       <c r="E115" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17913,10 +17910,10 @@
       <c r="B116" s="57">
         <v>6100</v>
       </c>
-      <c r="C116" s="695" t="s">
+      <c r="C116" s="709" t="s">
         <v>636</v>
       </c>
-      <c r="D116" s="696"/>
+      <c r="D116" s="710"/>
       <c r="E116" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17953,10 +17950,10 @@
       <c r="B117" s="57">
         <v>6200</v>
       </c>
-      <c r="C117" s="728" t="s">
+      <c r="C117" s="755" t="s">
         <v>637</v>
       </c>
-      <c r="D117" s="733"/>
+      <c r="D117" s="756"/>
       <c r="E117" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17993,10 +17990,10 @@
       <c r="B118" s="57">
         <v>6300</v>
       </c>
-      <c r="C118" s="725" t="s">
+      <c r="C118" s="743" t="s">
         <v>638</v>
       </c>
-      <c r="D118" s="702"/>
+      <c r="D118" s="715"/>
       <c r="E118" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18033,10 +18030,10 @@
       <c r="B119" s="57">
         <v>6400</v>
       </c>
-      <c r="C119" s="748" t="s">
+      <c r="C119" s="741" t="s">
         <v>639</v>
       </c>
-      <c r="D119" s="749"/>
+      <c r="D119" s="742"/>
       <c r="E119" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18131,10 +18128,10 @@
       <c r="B121" s="57">
         <v>6600</v>
       </c>
-      <c r="C121" s="725" t="s">
+      <c r="C121" s="743" t="s">
         <v>254</v>
       </c>
-      <c r="D121" s="702"/>
+      <c r="D121" s="715"/>
       <c r="E121" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18171,10 +18168,10 @@
       <c r="B122" s="57">
         <v>6700</v>
       </c>
-      <c r="C122" s="725" t="s">
+      <c r="C122" s="743" t="s">
         <v>687</v>
       </c>
-      <c r="D122" s="702"/>
+      <c r="D122" s="715"/>
       <c r="E122" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18211,10 +18208,10 @@
       <c r="B123" s="57">
         <v>6900</v>
       </c>
-      <c r="C123" s="750" t="s">
+      <c r="C123" s="744" t="s">
         <v>640</v>
       </c>
-      <c r="D123" s="751"/>
+      <c r="D123" s="745"/>
       <c r="E123" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18249,10 +18246,10 @@
         <v>260</v>
       </c>
       <c r="B124" s="71"/>
-      <c r="C124" s="738" t="s">
+      <c r="C124" s="759" t="s">
         <v>252</v>
       </c>
-      <c r="D124" s="739"/>
+      <c r="D124" s="760"/>
       <c r="E124" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18286,10 +18283,10 @@
         <v>261</v>
       </c>
       <c r="B125" s="112"/>
-      <c r="C125" s="740" t="s">
+      <c r="C125" s="750" t="s">
         <v>253</v>
       </c>
-      <c r="D125" s="741"/>
+      <c r="D125" s="704"/>
       <c r="E125" s="113"/>
       <c r="F125" s="170"/>
       <c r="G125" s="170"/>
@@ -18307,10 +18304,10 @@
       <c r="B126" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C126" s="734" t="s">
+      <c r="C126" s="757" t="s">
         <v>899</v>
       </c>
-      <c r="D126" s="735"/>
+      <c r="D126" s="758"/>
       <c r="E126" s="170"/>
       <c r="F126" s="170"/>
       <c r="G126" s="170"/>
@@ -18328,10 +18325,10 @@
       <c r="B127" s="57">
         <v>7400</v>
       </c>
-      <c r="C127" s="736" t="s">
+      <c r="C127" s="752" t="s">
         <v>900</v>
       </c>
-      <c r="D127" s="737"/>
+      <c r="D127" s="753"/>
       <c r="E127" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18368,10 +18365,10 @@
       <c r="B128" s="57">
         <v>7500</v>
       </c>
-      <c r="C128" s="699" t="s">
+      <c r="C128" s="689" t="s">
         <v>710</v>
       </c>
-      <c r="D128" s="700"/>
+      <c r="D128" s="690"/>
       <c r="E128" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18411,7 +18408,7 @@
       <c r="C129" s="697" t="s">
         <v>641</v>
       </c>
-      <c r="D129" s="742"/>
+      <c r="D129" s="698"/>
       <c r="E129" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18451,7 +18448,7 @@
       <c r="C130" s="697" t="s">
         <v>642</v>
       </c>
-      <c r="D130" s="698"/>
+      <c r="D130" s="729"/>
       <c r="E130" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18488,10 +18485,10 @@
       <c r="B131" s="96">
         <v>7800</v>
       </c>
-      <c r="C131" s="746" t="s">
-        <v>0</v>
-      </c>
-      <c r="D131" s="747"/>
+      <c r="C131" s="739" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="740"/>
       <c r="E131" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18526,10 +18523,10 @@
         <v>315</v>
       </c>
       <c r="B132" s="71"/>
-      <c r="C132" s="738" t="s">
+      <c r="C132" s="759" t="s">
         <v>898</v>
       </c>
-      <c r="D132" s="739"/>
+      <c r="D132" s="760"/>
       <c r="E132" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18587,12 +18584,12 @@
     </row>
     <row r="136" spans="1:11" ht="42" customHeight="1">
       <c r="A136" s="103"/>
-      <c r="B136" s="729" t="e">
+      <c r="B136" s="707" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C136" s="730"/>
-      <c r="D136" s="730"/>
+      <c r="C136" s="708"/>
+      <c r="D136" s="708"/>
       <c r="E136" s="79"/>
       <c r="F136" s="79"/>
       <c r="K136" s="167">
@@ -18615,12 +18612,12 @@
     </row>
     <row r="138" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A138" s="103"/>
-      <c r="B138" s="691" t="e">
+      <c r="B138" s="723" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C138" s="692"/>
-      <c r="D138" s="692"/>
+      <c r="C138" s="724"/>
+      <c r="D138" s="724"/>
       <c r="E138" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18659,12 +18656,12 @@
     </row>
     <row r="141" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A141" s="103"/>
-      <c r="B141" s="691" t="e">
+      <c r="B141" s="723" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C141" s="692"/>
-      <c r="D141" s="692"/>
+      <c r="C141" s="724"/>
+      <c r="D141" s="724"/>
       <c r="E141" s="79" t="s">
         <v>505</v>
       </c>
@@ -18854,12 +18851,12 @@
     </row>
     <row r="152" spans="1:11" ht="44.25" customHeight="1">
       <c r="A152" s="103"/>
-      <c r="B152" s="729" t="e">
+      <c r="B152" s="707" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C152" s="730"/>
-      <c r="D152" s="730"/>
+      <c r="C152" s="708"/>
+      <c r="D152" s="708"/>
       <c r="E152" s="79"/>
       <c r="F152" s="79"/>
       <c r="K152" s="167">
@@ -18882,12 +18879,12 @@
     </row>
     <row r="154" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A154" s="103"/>
-      <c r="B154" s="691" t="e">
+      <c r="B154" s="723" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C154" s="692"/>
-      <c r="D154" s="692"/>
+      <c r="C154" s="724"/>
+      <c r="D154" s="724"/>
       <c r="E154" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18926,12 +18923,12 @@
     </row>
     <row r="157" spans="1:11" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A157" s="103"/>
-      <c r="B157" s="691" t="e">
+      <c r="B157" s="723" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C157" s="692"/>
-      <c r="D157" s="692"/>
+      <c r="C157" s="724"/>
+      <c r="D157" s="724"/>
       <c r="E157" s="79" t="s">
         <v>505</v>
       </c>
@@ -18981,10 +18978,10 @@
     <row r="161" spans="1:65" ht="21.75" thickBot="1">
       <c r="A161" s="103"/>
       <c r="B161" s="112"/>
-      <c r="C161" s="743" t="s">
+      <c r="C161" s="746" t="s">
         <v>684</v>
       </c>
-      <c r="D161" s="710"/>
+      <c r="D161" s="702"/>
       <c r="E161" s="48" t="s">
         <v>509</v>
       </c>
@@ -19004,10 +19001,10 @@
       <c r="B162" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C162" s="711" t="s">
+      <c r="C162" s="701" t="s">
         <v>707</v>
       </c>
-      <c r="D162" s="708"/>
+      <c r="D162" s="700"/>
       <c r="E162" s="50">
         <v>2017</v>
       </c>
@@ -19035,10 +19032,10 @@
         <v>1</v>
       </c>
       <c r="B163" s="139"/>
-      <c r="C163" s="744" t="s">
+      <c r="C163" s="703" t="s">
         <v>685</v>
       </c>
-      <c r="D163" s="741"/>
+      <c r="D163" s="704"/>
       <c r="E163" s="10" t="s">
         <v>263</v>
       </c>
@@ -19068,10 +19065,10 @@
       <c r="B164" s="54">
         <v>7000</v>
       </c>
-      <c r="C164" s="731" t="s">
+      <c r="C164" s="754" t="s">
         <v>902</v>
       </c>
-      <c r="D164" s="732"/>
+      <c r="D164" s="728"/>
       <c r="E164" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19108,10 +19105,10 @@
       <c r="B165" s="57">
         <v>7100</v>
       </c>
-      <c r="C165" s="693" t="s">
+      <c r="C165" s="721" t="s">
         <v>903</v>
       </c>
-      <c r="D165" s="694"/>
+      <c r="D165" s="722"/>
       <c r="E165" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19148,10 +19145,10 @@
       <c r="B166" s="57">
         <v>7200</v>
       </c>
-      <c r="C166" s="693" t="s">
+      <c r="C166" s="721" t="s">
         <v>1414</v>
       </c>
-      <c r="D166" s="694"/>
+      <c r="D166" s="722"/>
       <c r="E166" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19188,10 +19185,10 @@
       <c r="B167" s="57">
         <v>7300</v>
       </c>
-      <c r="C167" s="701" t="s">
+      <c r="C167" s="714" t="s">
         <v>904</v>
       </c>
-      <c r="D167" s="702"/>
+      <c r="D167" s="715"/>
       <c r="E167" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19228,10 +19225,10 @@
       <c r="B168" s="57">
         <v>7900</v>
       </c>
-      <c r="C168" s="703" t="s">
+      <c r="C168" s="781" t="s">
         <v>905</v>
       </c>
-      <c r="D168" s="704"/>
+      <c r="D168" s="782"/>
       <c r="E168" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19321,10 +19318,10 @@
       <c r="B169" s="57">
         <v>8000</v>
       </c>
-      <c r="C169" s="695" t="s">
+      <c r="C169" s="709" t="s">
         <v>711</v>
       </c>
-      <c r="D169" s="696"/>
+      <c r="D169" s="710"/>
       <c r="E169" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19364,7 +19361,7 @@
       <c r="C170" s="697" t="s">
         <v>712</v>
       </c>
-      <c r="D170" s="698"/>
+      <c r="D170" s="729"/>
       <c r="E170" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19404,7 +19401,7 @@
       <c r="C171" s="697" t="s">
         <v>101</v>
       </c>
-      <c r="D171" s="698"/>
+      <c r="D171" s="729"/>
       <c r="E171" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19441,10 +19438,10 @@
       <c r="B172" s="57">
         <v>8300</v>
       </c>
-      <c r="C172" s="699" t="s">
+      <c r="C172" s="689" t="s">
         <v>713</v>
       </c>
-      <c r="D172" s="700"/>
+      <c r="D172" s="690"/>
       <c r="E172" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19481,10 +19478,10 @@
       <c r="B173" s="57">
         <v>8500</v>
       </c>
-      <c r="C173" s="695" t="s">
+      <c r="C173" s="709" t="s">
         <v>102</v>
       </c>
-      <c r="D173" s="696"/>
+      <c r="D173" s="710"/>
       <c r="E173" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19521,10 +19518,10 @@
       <c r="B174" s="57">
         <v>8600</v>
       </c>
-      <c r="C174" s="695" t="s">
+      <c r="C174" s="709" t="s">
         <v>103</v>
       </c>
-      <c r="D174" s="696"/>
+      <c r="D174" s="710"/>
       <c r="E174" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19564,7 +19561,7 @@
       <c r="C175" s="697" t="s">
         <v>265</v>
       </c>
-      <c r="D175" s="698"/>
+      <c r="D175" s="729"/>
       <c r="E175" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19604,7 +19601,7 @@
       <c r="C176" s="697" t="s">
         <v>910</v>
       </c>
-      <c r="D176" s="698"/>
+      <c r="D176" s="729"/>
       <c r="E176" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19641,10 +19638,10 @@
       <c r="B177" s="57">
         <v>8900</v>
       </c>
-      <c r="C177" s="725" t="s">
+      <c r="C177" s="743" t="s">
         <v>759</v>
       </c>
-      <c r="D177" s="702"/>
+      <c r="D177" s="715"/>
       <c r="E177" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19681,10 +19678,10 @@
       <c r="B178" s="57">
         <v>9000</v>
       </c>
-      <c r="C178" s="695" t="s">
+      <c r="C178" s="709" t="s">
         <v>104</v>
       </c>
-      <c r="D178" s="696"/>
+      <c r="D178" s="710"/>
       <c r="E178" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19721,10 +19718,10 @@
       <c r="B179" s="57">
         <v>9100</v>
       </c>
-      <c r="C179" s="725" t="s">
+      <c r="C179" s="743" t="s">
         <v>911</v>
       </c>
-      <c r="D179" s="728"/>
+      <c r="D179" s="755"/>
       <c r="E179" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19761,10 +19758,10 @@
       <c r="B180" s="57">
         <v>9200</v>
       </c>
-      <c r="C180" s="726" t="s">
+      <c r="C180" s="778" t="s">
         <v>714</v>
       </c>
-      <c r="D180" s="698"/>
+      <c r="D180" s="729"/>
       <c r="E180" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19801,10 +19798,10 @@
       <c r="B181" s="57">
         <v>9300</v>
       </c>
-      <c r="C181" s="695" t="s">
+      <c r="C181" s="709" t="s">
         <v>715</v>
       </c>
-      <c r="D181" s="696"/>
+      <c r="D181" s="710"/>
       <c r="E181" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19841,10 +19838,10 @@
       <c r="B182" s="57">
         <v>9500</v>
       </c>
-      <c r="C182" s="726" t="s">
+      <c r="C182" s="778" t="s">
         <v>716</v>
       </c>
-      <c r="D182" s="727"/>
+      <c r="D182" s="779"/>
       <c r="E182" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19881,10 +19878,10 @@
       <c r="B183" s="57">
         <v>9600</v>
       </c>
-      <c r="C183" s="726" t="s">
+      <c r="C183" s="778" t="s">
         <v>717</v>
       </c>
-      <c r="D183" s="698"/>
+      <c r="D183" s="729"/>
       <c r="E183" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19921,10 +19918,10 @@
       <c r="B184" s="57">
         <v>9800</v>
       </c>
-      <c r="C184" s="689" t="s">
+      <c r="C184" s="780" t="s">
         <v>465</v>
       </c>
-      <c r="D184" s="690"/>
+      <c r="D184" s="738"/>
       <c r="E184" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19959,10 +19956,10 @@
         <v>610</v>
       </c>
       <c r="B185" s="146"/>
-      <c r="C185" s="711" t="s">
+      <c r="C185" s="701" t="s">
         <v>930</v>
       </c>
-      <c r="D185" s="708"/>
+      <c r="D185" s="700"/>
       <c r="E185" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -20025,12 +20022,12 @@
       </c>
     </row>
     <row r="189" spans="1:11" ht="42" customHeight="1">
-      <c r="B189" s="729" t="e">
+      <c r="B189" s="707" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C189" s="730"/>
-      <c r="D189" s="730"/>
+      <c r="C189" s="708"/>
+      <c r="D189" s="708"/>
       <c r="E189" s="79"/>
       <c r="F189" s="79"/>
       <c r="G189" s="56"/>
@@ -20053,12 +20050,12 @@
       </c>
     </row>
     <row r="191" spans="1:11" ht="21.75" thickBot="1">
-      <c r="B191" s="691" t="e">
+      <c r="B191" s="723" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C191" s="692"/>
-      <c r="D191" s="692"/>
+      <c r="C191" s="724"/>
+      <c r="D191" s="724"/>
       <c r="E191" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -20097,12 +20094,12 @@
       </c>
     </row>
     <row r="194" spans="2:11" ht="22.5" thickTop="1" thickBot="1">
-      <c r="B194" s="691" t="e">
+      <c r="B194" s="723" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C194" s="692"/>
-      <c r="D194" s="692"/>
+      <c r="C194" s="724"/>
+      <c r="D194" s="724"/>
       <c r="E194" s="79" t="s">
         <v>505</v>
       </c>
@@ -20156,10 +20153,10 @@
       <c r="B198" s="153" t="s">
         <v>474</v>
       </c>
-      <c r="C198" s="707" t="s">
+      <c r="C198" s="763" t="s">
         <v>718</v>
       </c>
-      <c r="D198" s="708"/>
+      <c r="D198" s="700"/>
       <c r="E198" s="48" t="s">
         <v>509</v>
       </c>
@@ -20176,8 +20173,8 @@
     </row>
     <row r="199" spans="2:11" ht="45.75" thickBot="1">
       <c r="B199" s="154"/>
-      <c r="C199" s="709"/>
-      <c r="D199" s="710"/>
+      <c r="C199" s="764"/>
+      <c r="D199" s="702"/>
       <c r="E199" s="50">
         <v>2017</v>
       </c>
@@ -20204,10 +20201,10 @@
       <c r="B200" s="155" t="s">
         <v>719</v>
       </c>
-      <c r="C200" s="723" t="s">
+      <c r="C200" s="776" t="s">
         <v>720</v>
       </c>
-      <c r="D200" s="724"/>
+      <c r="D200" s="777"/>
       <c r="E200" s="187" t="e">
         <f>SUMIF(#REF!,1,#REF!)</f>
         <v>#REF!</v>
@@ -20240,10 +20237,10 @@
       <c r="B201" s="156" t="s">
         <v>721</v>
       </c>
-      <c r="C201" s="716" t="s">
+      <c r="C201" s="769" t="s">
         <v>722</v>
       </c>
-      <c r="D201" s="717"/>
+      <c r="D201" s="770"/>
       <c r="E201" s="188" t="e">
         <f>SUMIF(#REF!,2,#REF!)</f>
         <v>#REF!</v>
@@ -20276,10 +20273,10 @@
       <c r="B202" s="156" t="s">
         <v>723</v>
       </c>
-      <c r="C202" s="716" t="s">
+      <c r="C202" s="769" t="s">
         <v>724</v>
       </c>
-      <c r="D202" s="717"/>
+      <c r="D202" s="770"/>
       <c r="E202" s="188" t="e">
         <f>SUMIF(#REF!,3,#REF!)</f>
         <v>#REF!</v>
@@ -20312,10 +20309,10 @@
       <c r="B203" s="156" t="s">
         <v>725</v>
       </c>
-      <c r="C203" s="719" t="s">
+      <c r="C203" s="772" t="s">
         <v>726</v>
       </c>
-      <c r="D203" s="720"/>
+      <c r="D203" s="773"/>
       <c r="E203" s="188" t="e">
         <f>SUMIF(#REF!,4,#REF!)</f>
         <v>#REF!</v>
@@ -20348,10 +20345,10 @@
       <c r="B204" s="156" t="s">
         <v>727</v>
       </c>
-      <c r="C204" s="721" t="s">
+      <c r="C204" s="774" t="s">
         <v>728</v>
       </c>
-      <c r="D204" s="722"/>
+      <c r="D204" s="775"/>
       <c r="E204" s="188" t="e">
         <f>SUMIF(#REF!,5,#REF!)</f>
         <v>#REF!</v>
@@ -20384,10 +20381,10 @@
       <c r="B205" s="156" t="s">
         <v>729</v>
       </c>
-      <c r="C205" s="718" t="s">
+      <c r="C205" s="771" t="s">
         <v>730</v>
       </c>
-      <c r="D205" s="718"/>
+      <c r="D205" s="771"/>
       <c r="E205" s="188" t="e">
         <f>SUMIF(#REF!,6,#REF!)</f>
         <v>#REF!</v>
@@ -20420,10 +20417,10 @@
       <c r="B206" s="156" t="s">
         <v>731</v>
       </c>
-      <c r="C206" s="712" t="s">
+      <c r="C206" s="765" t="s">
         <v>732</v>
       </c>
-      <c r="D206" s="713"/>
+      <c r="D206" s="766"/>
       <c r="E206" s="188" t="e">
         <f>SUMIF(#REF!,7,#REF!)</f>
         <v>#REF!</v>
@@ -20456,10 +20453,10 @@
       <c r="B207" s="156" t="s">
         <v>733</v>
       </c>
-      <c r="C207" s="712" t="s">
+      <c r="C207" s="765" t="s">
         <v>734</v>
       </c>
-      <c r="D207" s="713"/>
+      <c r="D207" s="766"/>
       <c r="E207" s="188" t="e">
         <f>SUMIF(#REF!,8,#REF!)</f>
         <v>#REF!</v>
@@ -20492,10 +20489,10 @@
       <c r="B208" s="156" t="s">
         <v>735</v>
       </c>
-      <c r="C208" s="714" t="s">
+      <c r="C208" s="767" t="s">
         <v>736</v>
       </c>
-      <c r="D208" s="715"/>
+      <c r="D208" s="768"/>
       <c r="E208" s="189" t="e">
         <f>SUMIF(#REF!,9,#REF!)</f>
         <v>#REF!</v>
@@ -20526,10 +20523,10 @@
     </row>
     <row r="209" spans="2:11" ht="21.75" thickBot="1">
       <c r="B209" s="157"/>
-      <c r="C209" s="705" t="s">
+      <c r="C209" s="761" t="s">
         <v>737</v>
       </c>
-      <c r="D209" s="706"/>
+      <c r="D209" s="762"/>
       <c r="E209" s="158" t="e">
         <f t="shared" ref="E209:J209" si="5">SUM(E200:E208)</f>
         <v>#REF!</v>
@@ -22138,116 +22135,17 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="145">
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="N63:N65"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="O63:O65"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="L63:L65"/>
-    <mergeCell ref="M63:M65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="C164:D164"/>
-    <mergeCell ref="C165:D165"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C161:D161"/>
-    <mergeCell ref="C162:D162"/>
-    <mergeCell ref="C163:D163"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="B136:D136"/>
-    <mergeCell ref="B138:D138"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B152:D152"/>
-    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
     <mergeCell ref="C209:D209"/>
     <mergeCell ref="C198:D198"/>
     <mergeCell ref="C199:D199"/>
@@ -22272,17 +22170,116 @@
     <mergeCell ref="B189:D189"/>
     <mergeCell ref="B194:D194"/>
     <mergeCell ref="C183:D183"/>
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C172:D172"/>
-    <mergeCell ref="C173:D173"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C161:D161"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="C163:D163"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="B152:D152"/>
+    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="N63:N65"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="O63:O65"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="L63:L65"/>
+    <mergeCell ref="M63:M65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
@@ -22334,8 +22331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -22589,9 +22586,7 @@
     </row>
     <row r="13" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="210"/>
-      <c r="B13" s="789" t="s">
-        <v>1498</v>
-      </c>
+      <c r="B13" s="789"/>
       <c r="C13" s="790"/>
       <c r="D13" s="791"/>
       <c r="E13" s="338">
@@ -22614,7 +22609,7 @@
       <c r="B14" s="354"/>
       <c r="C14" s="325"/>
       <c r="D14" s="211" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="E14" s="355"/>
       <c r="F14" s="355"/>
@@ -22645,9 +22640,7 @@
     </row>
     <row r="16" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="792" t="s">
-        <v>1498</v>
-      </c>
+      <c r="B16" s="792"/>
       <c r="C16" s="793"/>
       <c r="D16" s="794"/>
       <c r="E16" s="356"/>
@@ -22666,7 +22659,7 @@
       <c r="B17" s="358"/>
       <c r="C17" s="325"/>
       <c r="D17" s="211" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
       <c r="E17" s="540"/>
       <c r="F17" s="541"/>
@@ -22886,6 +22879,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="292">
+        <f>G25+H25+I25</f>
         <v>0</v>
       </c>
       <c r="G25" s="269">
@@ -22931,7 +22925,8 @@
       <c r="E26" s="290">
         <v>0</v>
       </c>
-      <c r="F26" s="293">
+      <c r="F26" s="292">
+        <f t="shared" ref="F26:F30" si="1">G26+H26+I26</f>
         <v>0</v>
       </c>
       <c r="G26" s="272">
@@ -22971,12 +22966,13 @@
         <v>551</v>
       </c>
       <c r="D27" s="409" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="E27" s="285">
         <v>0</v>
       </c>
       <c r="F27" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27" s="269">
@@ -23003,12 +22999,13 @@
         <v>560</v>
       </c>
       <c r="D28" s="413" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="E28" s="287">
         <v>0</v>
       </c>
-      <c r="F28" s="294">
+      <c r="F28" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G28" s="275">
@@ -23035,12 +23032,13 @@
         <v>580</v>
       </c>
       <c r="D29" s="411" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="E29" s="287">
         <v>0</v>
       </c>
-      <c r="F29" s="294">
+      <c r="F29" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G29" s="275">
@@ -23065,12 +23063,13 @@
         <v>590</v>
       </c>
       <c r="D30" s="411" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="E30" s="287">
         <v>0</v>
       </c>
-      <c r="F30" s="294">
+      <c r="F30" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G30" s="275">
@@ -23108,11 +23107,11 @@
         <v>0</v>
       </c>
       <c r="H31" s="266">
-        <f t="shared" ref="H31:I31" si="1">SUM(H32:H34)</f>
+        <f t="shared" ref="H31:I31" si="2">SUM(H32:H34)</f>
         <v>0</v>
       </c>
       <c r="I31" s="266">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J31" s="582" t="e">
@@ -23234,10 +23233,10 @@
     <row r="35" spans="1:25" ht="18.75" customHeight="1">
       <c r="A35" s="8"/>
       <c r="B35" s="449" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C35" s="785" t="s">
         <v>1499</v>
-      </c>
-      <c r="C35" s="785" t="s">
-        <v>1500</v>
       </c>
       <c r="D35" s="785"/>
       <c r="E35" s="243">
@@ -23252,11 +23251,11 @@
         <v>0</v>
       </c>
       <c r="H35" s="266">
-        <f t="shared" ref="H35:I35" si="2">SUM(H36:H38)</f>
+        <f t="shared" ref="H35:I35" si="3">SUM(H36:H38)</f>
         <v>0</v>
       </c>
       <c r="I35" s="266">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J35" s="582"/>
@@ -23268,10 +23267,10 @@
       </c>
       <c r="B36" s="402"/>
       <c r="C36" s="403" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D36" s="404" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="E36" s="287">
         <v>0</v>
@@ -23300,10 +23299,10 @@
       </c>
       <c r="B37" s="396"/>
       <c r="C37" s="419" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D37" s="420" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="E37" s="296">
         <v>0</v>
@@ -23332,7 +23331,7 @@
       </c>
       <c r="B38" s="402"/>
       <c r="C38" s="683" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="D38" s="684" t="s">
         <v>191</v>
@@ -23728,12 +23727,12 @@
         <v>3</v>
       </c>
       <c r="H14" s="328"/>
-      <c r="I14" s="800">
+      <c r="I14" s="798">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J14" s="801"/>
-      <c r="K14" s="801"/>
+      <c r="J14" s="799"/>
+      <c r="K14" s="799"/>
       <c r="L14" s="346"/>
       <c r="M14" s="346"/>
       <c r="N14" s="347"/>
@@ -23777,12 +23776,12 @@
         <v>5</v>
       </c>
       <c r="H16" s="328"/>
-      <c r="I16" s="802">
+      <c r="I16" s="800">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J16" s="803"/>
-      <c r="K16" s="804"/>
+      <c r="J16" s="801"/>
+      <c r="K16" s="802"/>
       <c r="L16" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -23849,12 +23848,12 @@
         <v>8</v>
       </c>
       <c r="H19" s="328"/>
-      <c r="I19" s="805">
+      <c r="I19" s="803">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J19" s="806"/>
-      <c r="K19" s="807"/>
+      <c r="J19" s="804"/>
+      <c r="K19" s="805"/>
       <c r="L19" s="356" t="s">
         <v>934</v>
       </c>
@@ -24422,10 +24421,10 @@
       <c r="I39" s="395">
         <v>500</v>
       </c>
-      <c r="J39" s="813" t="s">
+      <c r="J39" s="796" t="s">
         <v>579</v>
       </c>
-      <c r="K39" s="813"/>
+      <c r="K39" s="796"/>
       <c r="L39" s="241">
         <f t="shared" ref="L39:Q39" si="3">SUM(L40:L46)</f>
         <v>0</v>
@@ -24694,10 +24693,10 @@
       <c r="I47" s="395">
         <v>800</v>
       </c>
-      <c r="J47" s="809" t="s">
+      <c r="J47" s="807" t="s">
         <v>698</v>
       </c>
-      <c r="K47" s="810"/>
+      <c r="K47" s="808"/>
       <c r="L47" s="567"/>
       <c r="M47" s="244">
         <f t="shared" si="4"/>
@@ -25652,7 +25651,7 @@
       <c r="J79" s="795" t="s">
         <v>606</v>
       </c>
-      <c r="K79" s="811"/>
+      <c r="K79" s="809"/>
       <c r="L79" s="567"/>
       <c r="M79" s="244">
         <f t="shared" si="10"/>
@@ -25676,7 +25675,7 @@
       <c r="I80" s="395">
         <v>2600</v>
       </c>
-      <c r="J80" s="812" t="s">
+      <c r="J80" s="797" t="s">
         <v>607</v>
       </c>
       <c r="K80" s="787"/>
@@ -25703,7 +25702,7 @@
       <c r="I81" s="395">
         <v>2700</v>
       </c>
-      <c r="J81" s="812" t="s">
+      <c r="J81" s="797" t="s">
         <v>608</v>
       </c>
       <c r="K81" s="787"/>
@@ -25730,7 +25729,7 @@
       <c r="I82" s="395">
         <v>2800</v>
       </c>
-      <c r="J82" s="812" t="s">
+      <c r="J82" s="797" t="s">
         <v>1011</v>
       </c>
       <c r="K82" s="787"/>
@@ -26674,7 +26673,7 @@
       <c r="I114" s="395">
         <v>4600</v>
       </c>
-      <c r="J114" s="812" t="s">
+      <c r="J114" s="797" t="s">
         <v>630</v>
       </c>
       <c r="K114" s="787"/>
@@ -27328,10 +27327,10 @@
       <c r="I136" s="449">
         <v>5700</v>
       </c>
-      <c r="J136" s="796" t="s">
+      <c r="J136" s="810" t="s">
         <v>943</v>
       </c>
-      <c r="K136" s="797"/>
+      <c r="K136" s="811"/>
       <c r="L136" s="243">
         <f t="shared" ref="L136:Q136" si="25">SUM(L137:L139)</f>
         <v>0</v>
@@ -27471,10 +27470,10 @@
       <c r="I141" s="464">
         <v>98</v>
       </c>
-      <c r="J141" s="798" t="s">
+      <c r="J141" s="812" t="s">
         <v>653</v>
       </c>
-      <c r="K141" s="799"/>
+      <c r="K141" s="813"/>
       <c r="L141" s="573"/>
       <c r="M141" s="324">
         <f>N141+O141+P141+Q141</f>
@@ -27670,12 +27669,12 @@
         <v>138</v>
       </c>
       <c r="H149" s="328"/>
-      <c r="I149" s="800">
+      <c r="I149" s="798">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J149" s="801"/>
-      <c r="K149" s="801"/>
+      <c r="J149" s="799"/>
+      <c r="K149" s="799"/>
       <c r="L149" s="326"/>
       <c r="M149" s="326"/>
       <c r="N149" s="326"/>
@@ -27717,12 +27716,12 @@
         <v>140</v>
       </c>
       <c r="H151" s="328"/>
-      <c r="I151" s="802">
+      <c r="I151" s="800">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J151" s="803"/>
-      <c r="K151" s="804"/>
+      <c r="J151" s="801"/>
+      <c r="K151" s="802"/>
       <c r="L151" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -27789,12 +27788,12 @@
         <v>143</v>
       </c>
       <c r="H154" s="328"/>
-      <c r="I154" s="805">
+      <c r="I154" s="803">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J154" s="806"/>
-      <c r="K154" s="807"/>
+      <c r="J154" s="804"/>
+      <c r="K154" s="805"/>
       <c r="L154" s="356" t="s">
         <v>934</v>
       </c>
@@ -28592,11 +28591,11 @@
         <v>175</v>
       </c>
       <c r="H186" s="328"/>
-      <c r="I186" s="808" t="s">
+      <c r="I186" s="806" t="s">
         <v>249</v>
       </c>
-      <c r="J186" s="808"/>
-      <c r="K186" s="808"/>
+      <c r="J186" s="806"/>
+      <c r="K186" s="806"/>
       <c r="L186" s="327"/>
       <c r="M186" s="327"/>
       <c r="N186" s="327"/>
@@ -29938,21 +29937,11 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="36">
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J141:K141"/>
     <mergeCell ref="I149:K149"/>
     <mergeCell ref="I151:K151"/>
     <mergeCell ref="I154:K154"/>
@@ -29969,11 +29958,21 @@
     <mergeCell ref="J99:K99"/>
     <mergeCell ref="J100:K100"/>
     <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L156:M156">

</xml_diff>

<commit_message>
Fix a few minor issues with calculations and displaying salary information.
</commit_message>
<xml_diff>
--- a/PaymentsBudgetSystem/wwwroot/Report.xlsx
+++ b/PaymentsBudgetSystem/wwwroot/Report.xlsx
@@ -8093,9 +8093,6 @@
     <t>Придобиване на стопански инвентар</t>
   </si>
   <si>
-    <t>Наименование разпоредителя с бюджет</t>
-  </si>
-  <si>
     <t>здравно-осигурителни вноски</t>
   </si>
   <si>
@@ -8130,6 +8127,9 @@
   </si>
   <si>
     <t>Вид на отчета</t>
+  </si>
+  <si>
+    <t>Отчет за дейността</t>
   </si>
 </sst>
 </file>
@@ -8149,7 +8149,7 @@
     <numFmt numFmtId="173" formatCode="&quot;x&quot;"/>
     <numFmt numFmtId="174" formatCode="&quot;II. ОБЩО РАЗХОДИ ЗА ДЕЙНОСТ &quot;0&quot;&quot;0&quot;&quot;0&quot;&quot;0"/>
   </numFmts>
-  <fonts count="154">
+  <fonts count="153">
     <font>
       <sz val="10"/>
       <name val="Hebar"/>
@@ -9206,13 +9206,6 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman CYR"/>
-      <family val="1"/>
       <charset val="204"/>
     </font>
     <font>
@@ -10980,7 +10973,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="814">
+  <cellXfs count="815">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -13314,22 +13307,25 @@
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="16" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="16" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="152" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="151" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="152" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="151" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="152" fillId="20" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="151" fillId="20" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -22331,8 +22327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -22586,15 +22582,13 @@
     </row>
     <row r="13" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="210"/>
-      <c r="B13" s="789"/>
+      <c r="B13" s="789" t="s">
+        <v>1510</v>
+      </c>
       <c r="C13" s="790"/>
       <c r="D13" s="791"/>
-      <c r="E13" s="338">
-        <v>44927</v>
-      </c>
-      <c r="F13" s="353">
-        <v>44926</v>
-      </c>
+      <c r="E13" s="338"/>
+      <c r="F13" s="353"/>
       <c r="G13" s="326"/>
       <c r="H13" s="326"/>
       <c r="I13" s="326"/>
@@ -22608,9 +22602,7 @@
       <c r="A14" s="210"/>
       <c r="B14" s="354"/>
       <c r="C14" s="325"/>
-      <c r="D14" s="211" t="s">
-        <v>1506</v>
-      </c>
+      <c r="D14" s="211"/>
       <c r="E14" s="355"/>
       <c r="F14" s="355"/>
       <c r="G14" s="326"/>
@@ -22656,11 +22648,11 @@
     </row>
     <row r="17" spans="1:25" s="226" customFormat="1">
       <c r="A17" s="210"/>
-      <c r="B17" s="358"/>
-      <c r="C17" s="325"/>
-      <c r="D17" s="211" t="s">
-        <v>1510</v>
-      </c>
+      <c r="B17" s="795" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C17" s="795"/>
+      <c r="D17" s="795"/>
       <c r="E17" s="540"/>
       <c r="F17" s="541"/>
       <c r="G17" s="355"/>
@@ -22926,7 +22918,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="292">
-        <f t="shared" ref="F26:F30" si="1">G26+H26+I26</f>
+        <f t="shared" ref="F26:F38" si="1">G26+H26+I26</f>
         <v>0</v>
       </c>
       <c r="G26" s="272">
@@ -22966,7 +22958,7 @@
         <v>551</v>
       </c>
       <c r="D27" s="409" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="E27" s="285">
         <v>0</v>
@@ -22999,7 +22991,7 @@
         <v>560</v>
       </c>
       <c r="D28" s="413" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="E28" s="287">
         <v>0</v>
@@ -23032,7 +23024,7 @@
         <v>580</v>
       </c>
       <c r="D29" s="411" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="E29" s="287">
         <v>0</v>
@@ -23148,7 +23140,8 @@
       <c r="E32" s="287">
         <v>0</v>
       </c>
-      <c r="F32" s="294">
+      <c r="F32" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G32" s="275">
@@ -23180,7 +23173,8 @@
       <c r="E33" s="296">
         <v>0</v>
       </c>
-      <c r="F33" s="297">
+      <c r="F33" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G33" s="278">
@@ -23212,7 +23206,8 @@
       <c r="E34" s="296">
         <v>0</v>
       </c>
-      <c r="F34" s="297">
+      <c r="F34" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G34" s="278">
@@ -23275,7 +23270,8 @@
       <c r="E36" s="287">
         <v>0</v>
       </c>
-      <c r="F36" s="294">
+      <c r="F36" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G36" s="275">
@@ -23307,7 +23303,8 @@
       <c r="E37" s="296">
         <v>0</v>
       </c>
-      <c r="F37" s="297">
+      <c r="F37" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G37" s="278">
@@ -23339,7 +23336,8 @@
       <c r="E38" s="685">
         <v>0</v>
       </c>
-      <c r="F38" s="301">
+      <c r="F38" s="292">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G38" s="686">
@@ -23485,13 +23483,14 @@
       <c r="C44" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="40" priority="85" stopIfTrue="1" operator="equal">
@@ -23727,12 +23726,12 @@
         <v>3</v>
       </c>
       <c r="H14" s="328"/>
-      <c r="I14" s="798">
+      <c r="I14" s="799">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J14" s="799"/>
-      <c r="K14" s="799"/>
+      <c r="J14" s="800"/>
+      <c r="K14" s="800"/>
       <c r="L14" s="346"/>
       <c r="M14" s="346"/>
       <c r="N14" s="347"/>
@@ -23776,12 +23775,12 @@
         <v>5</v>
       </c>
       <c r="H16" s="328"/>
-      <c r="I16" s="800">
+      <c r="I16" s="801">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J16" s="801"/>
-      <c r="K16" s="802"/>
+      <c r="J16" s="802"/>
+      <c r="K16" s="803"/>
       <c r="L16" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -23848,12 +23847,12 @@
         <v>8</v>
       </c>
       <c r="H19" s="328"/>
-      <c r="I19" s="803">
+      <c r="I19" s="804">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J19" s="804"/>
-      <c r="K19" s="805"/>
+      <c r="J19" s="805"/>
+      <c r="K19" s="806"/>
       <c r="L19" s="356" t="s">
         <v>934</v>
       </c>
@@ -24421,10 +24420,10 @@
       <c r="I39" s="395">
         <v>500</v>
       </c>
-      <c r="J39" s="796" t="s">
+      <c r="J39" s="797" t="s">
         <v>579</v>
       </c>
-      <c r="K39" s="796"/>
+      <c r="K39" s="797"/>
       <c r="L39" s="241">
         <f t="shared" ref="L39:Q39" si="3">SUM(L40:L46)</f>
         <v>0</v>
@@ -24693,10 +24692,10 @@
       <c r="I47" s="395">
         <v>800</v>
       </c>
-      <c r="J47" s="807" t="s">
+      <c r="J47" s="808" t="s">
         <v>698</v>
       </c>
-      <c r="K47" s="808"/>
+      <c r="K47" s="809"/>
       <c r="L47" s="567"/>
       <c r="M47" s="244">
         <f t="shared" si="4"/>
@@ -25239,10 +25238,10 @@
       <c r="I66" s="395">
         <v>1900</v>
       </c>
-      <c r="J66" s="795" t="s">
+      <c r="J66" s="796" t="s">
         <v>456</v>
       </c>
-      <c r="K66" s="795"/>
+      <c r="K66" s="796"/>
       <c r="L66" s="243">
         <f t="shared" ref="L66:Q66" si="7">SUM(L67:L69)</f>
         <v>0</v>
@@ -25366,10 +25365,10 @@
       <c r="I70" s="395">
         <v>2100</v>
       </c>
-      <c r="J70" s="795" t="s">
+      <c r="J70" s="796" t="s">
         <v>741</v>
       </c>
-      <c r="K70" s="795"/>
+      <c r="K70" s="796"/>
       <c r="L70" s="243">
         <f t="shared" ref="L70:Q70" si="8">SUM(L71:L75)</f>
         <v>0</v>
@@ -25552,10 +25551,10 @@
       <c r="I76" s="395">
         <v>2200</v>
       </c>
-      <c r="J76" s="795" t="s">
+      <c r="J76" s="796" t="s">
         <v>604</v>
       </c>
-      <c r="K76" s="795"/>
+      <c r="K76" s="796"/>
       <c r="L76" s="243">
         <f t="shared" ref="L76:Q76" si="9">SUM(L77:L78)</f>
         <v>0</v>
@@ -25648,10 +25647,10 @@
       <c r="I79" s="395">
         <v>2500</v>
       </c>
-      <c r="J79" s="795" t="s">
+      <c r="J79" s="796" t="s">
         <v>606</v>
       </c>
-      <c r="K79" s="809"/>
+      <c r="K79" s="810"/>
       <c r="L79" s="567"/>
       <c r="M79" s="244">
         <f t="shared" si="10"/>
@@ -25675,7 +25674,7 @@
       <c r="I80" s="395">
         <v>2600</v>
       </c>
-      <c r="J80" s="797" t="s">
+      <c r="J80" s="798" t="s">
         <v>607</v>
       </c>
       <c r="K80" s="787"/>
@@ -25702,7 +25701,7 @@
       <c r="I81" s="395">
         <v>2700</v>
       </c>
-      <c r="J81" s="797" t="s">
+      <c r="J81" s="798" t="s">
         <v>608</v>
       </c>
       <c r="K81" s="787"/>
@@ -25729,7 +25728,7 @@
       <c r="I82" s="395">
         <v>2800</v>
       </c>
-      <c r="J82" s="797" t="s">
+      <c r="J82" s="798" t="s">
         <v>1011</v>
       </c>
       <c r="K82" s="787"/>
@@ -25756,10 +25755,10 @@
       <c r="I83" s="395">
         <v>2900</v>
       </c>
-      <c r="J83" s="795" t="s">
+      <c r="J83" s="796" t="s">
         <v>609</v>
       </c>
-      <c r="K83" s="795"/>
+      <c r="K83" s="796"/>
       <c r="L83" s="243">
         <f t="shared" ref="L83:Q83" si="11">SUM(L84:L91)</f>
         <v>0</v>
@@ -26211,10 +26210,10 @@
       <c r="I98" s="395">
         <v>3900</v>
       </c>
-      <c r="J98" s="795" t="s">
+      <c r="J98" s="796" t="s">
         <v>618</v>
       </c>
-      <c r="K98" s="795"/>
+      <c r="K98" s="796"/>
       <c r="L98" s="567"/>
       <c r="M98" s="244">
         <f t="shared" si="14"/>
@@ -26238,10 +26237,10 @@
       <c r="I99" s="395">
         <v>4000</v>
       </c>
-      <c r="J99" s="795" t="s">
+      <c r="J99" s="796" t="s">
         <v>619</v>
       </c>
-      <c r="K99" s="795"/>
+      <c r="K99" s="796"/>
       <c r="L99" s="567"/>
       <c r="M99" s="244">
         <f t="shared" si="14"/>
@@ -26265,10 +26264,10 @@
       <c r="I100" s="395">
         <v>4100</v>
       </c>
-      <c r="J100" s="795" t="s">
+      <c r="J100" s="796" t="s">
         <v>620</v>
       </c>
-      <c r="K100" s="795"/>
+      <c r="K100" s="796"/>
       <c r="L100" s="567"/>
       <c r="M100" s="244">
         <f t="shared" si="14"/>
@@ -26292,10 +26291,10 @@
       <c r="I101" s="395">
         <v>4200</v>
       </c>
-      <c r="J101" s="795" t="s">
+      <c r="J101" s="796" t="s">
         <v>621</v>
       </c>
-      <c r="K101" s="795"/>
+      <c r="K101" s="796"/>
       <c r="L101" s="243">
         <f t="shared" ref="L101:Q101" si="16">SUM(L102:L107)</f>
         <v>0</v>
@@ -26496,10 +26495,10 @@
       <c r="I108" s="395">
         <v>4300</v>
       </c>
-      <c r="J108" s="795" t="s">
+      <c r="J108" s="796" t="s">
         <v>1015</v>
       </c>
-      <c r="K108" s="795"/>
+      <c r="K108" s="796"/>
       <c r="L108" s="243">
         <f t="shared" ref="L108:Q108" si="18">SUM(L109:L111)</f>
         <v>0</v>
@@ -26619,10 +26618,10 @@
       <c r="I112" s="395">
         <v>4400</v>
       </c>
-      <c r="J112" s="795" t="s">
+      <c r="J112" s="796" t="s">
         <v>1012</v>
       </c>
-      <c r="K112" s="795"/>
+      <c r="K112" s="796"/>
       <c r="L112" s="567"/>
       <c r="M112" s="244">
         <f t="shared" si="19"/>
@@ -26646,10 +26645,10 @@
       <c r="I113" s="395">
         <v>4500</v>
       </c>
-      <c r="J113" s="795" t="s">
+      <c r="J113" s="796" t="s">
         <v>1013</v>
       </c>
-      <c r="K113" s="795"/>
+      <c r="K113" s="796"/>
       <c r="L113" s="567"/>
       <c r="M113" s="244">
         <f t="shared" si="19"/>
@@ -26673,7 +26672,7 @@
       <c r="I114" s="395">
         <v>4600</v>
       </c>
-      <c r="J114" s="797" t="s">
+      <c r="J114" s="798" t="s">
         <v>630</v>
       </c>
       <c r="K114" s="787"/>
@@ -26700,10 +26699,10 @@
       <c r="I115" s="395">
         <v>4900</v>
       </c>
-      <c r="J115" s="795" t="s">
+      <c r="J115" s="796" t="s">
         <v>460</v>
       </c>
-      <c r="K115" s="795"/>
+      <c r="K115" s="796"/>
       <c r="L115" s="243">
         <f t="shared" ref="L115:Q115" si="20">+L116+L117</f>
         <v>0</v>
@@ -27177,10 +27176,10 @@
       <c r="I131" s="395">
         <v>5500</v>
       </c>
-      <c r="J131" s="795" t="s">
+      <c r="J131" s="796" t="s">
         <v>644</v>
       </c>
-      <c r="K131" s="795"/>
+      <c r="K131" s="796"/>
       <c r="L131" s="243">
         <f t="shared" ref="L131:Q131" si="24">SUM(L132:L135)</f>
         <v>0</v>
@@ -27327,10 +27326,10 @@
       <c r="I136" s="449">
         <v>5700</v>
       </c>
-      <c r="J136" s="810" t="s">
+      <c r="J136" s="811" t="s">
         <v>943</v>
       </c>
-      <c r="K136" s="811"/>
+      <c r="K136" s="812"/>
       <c r="L136" s="243">
         <f t="shared" ref="L136:Q136" si="25">SUM(L137:L139)</f>
         <v>0</v>
@@ -27470,10 +27469,10 @@
       <c r="I141" s="464">
         <v>98</v>
       </c>
-      <c r="J141" s="812" t="s">
+      <c r="J141" s="813" t="s">
         <v>653</v>
       </c>
-      <c r="K141" s="813"/>
+      <c r="K141" s="814"/>
       <c r="L141" s="573"/>
       <c r="M141" s="324">
         <f>N141+O141+P141+Q141</f>
@@ -27669,12 +27668,12 @@
         <v>138</v>
       </c>
       <c r="H149" s="328"/>
-      <c r="I149" s="798">
+      <c r="I149" s="799">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J149" s="799"/>
-      <c r="K149" s="799"/>
+      <c r="J149" s="800"/>
+      <c r="K149" s="800"/>
       <c r="L149" s="326"/>
       <c r="M149" s="326"/>
       <c r="N149" s="326"/>
@@ -27716,12 +27715,12 @@
         <v>140</v>
       </c>
       <c r="H151" s="328"/>
-      <c r="I151" s="800">
+      <c r="I151" s="801">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J151" s="801"/>
-      <c r="K151" s="802"/>
+      <c r="J151" s="802"/>
+      <c r="K151" s="803"/>
       <c r="L151" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -27788,12 +27787,12 @@
         <v>143</v>
       </c>
       <c r="H154" s="328"/>
-      <c r="I154" s="803">
+      <c r="I154" s="804">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J154" s="804"/>
-      <c r="K154" s="805"/>
+      <c r="J154" s="805"/>
+      <c r="K154" s="806"/>
       <c r="L154" s="356" t="s">
         <v>934</v>
       </c>
@@ -28591,11 +28590,11 @@
         <v>175</v>
       </c>
       <c r="H186" s="328"/>
-      <c r="I186" s="806" t="s">
+      <c r="I186" s="807" t="s">
         <v>249</v>
       </c>
-      <c r="J186" s="806"/>
-      <c r="K186" s="806"/>
+      <c r="J186" s="807"/>
+      <c r="K186" s="807"/>
       <c r="L186" s="327"/>
       <c r="M186" s="327"/>
       <c r="N186" s="327"/>

</xml_diff>

<commit_message>
Modified CashPayment view. Fixed a bug in Asset Controller logic.
</commit_message>
<xml_diff>
--- a/PaymentsBudgetSystem/wwwroot/Report.xlsx
+++ b/PaymentsBudgetSystem/wwwroot/Report.xlsx
@@ -10973,7 +10973,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="815">
+  <cellXfs count="816">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -13009,10 +13009,261 @@
     <xf numFmtId="3" fontId="13" fillId="12" borderId="102" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -13035,260 +13286,9 @@
     <xf numFmtId="0" fontId="45" fillId="5" borderId="114" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -13331,11 +13331,17 @@
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -13375,16 +13381,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -14436,12 +14439,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="42" customHeight="1">
-      <c r="B7" s="691" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="692"/>
-      <c r="D7" s="692"/>
+      <c r="B7" s="776" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C7" s="777"/>
+      <c r="D7" s="777"/>
       <c r="F7" s="38"/>
       <c r="K7" s="167">
         <v>1</v>
@@ -14461,12 +14464,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="36.75" customHeight="1" thickBot="1">
-      <c r="B9" s="693" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="694"/>
-      <c r="D9" s="694"/>
+      <c r="B9" s="778" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="779"/>
+      <c r="D9" s="779"/>
       <c r="E9" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14501,12 +14504,12 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="39" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B12" s="693" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C12" s="694"/>
-      <c r="D12" s="694"/>
+      <c r="B12" s="778" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C12" s="779"/>
+      <c r="D12" s="779"/>
       <c r="E12" s="38" t="s">
         <v>505</v>
       </c>
@@ -14581,10 +14584,10 @@
     <row r="19" spans="1:11" ht="21.75" thickBot="1">
       <c r="A19" s="46"/>
       <c r="B19" s="47"/>
-      <c r="C19" s="699" t="s">
+      <c r="C19" s="782" t="s">
         <v>508</v>
       </c>
-      <c r="D19" s="700"/>
+      <c r="D19" s="708"/>
       <c r="E19" s="48" t="s">
         <v>509</v>
       </c>
@@ -14603,10 +14606,10 @@
       <c r="B20" s="49" t="s">
         <v>474</v>
       </c>
-      <c r="C20" s="701" t="s">
+      <c r="C20" s="711" t="s">
         <v>705</v>
       </c>
-      <c r="D20" s="702"/>
+      <c r="D20" s="710"/>
       <c r="E20" s="50">
         <v>2017</v>
       </c>
@@ -14631,10 +14634,10 @@
     </row>
     <row r="21" spans="1:11" ht="21.75" thickBot="1">
       <c r="B21" s="51"/>
-      <c r="C21" s="703" t="s">
+      <c r="C21" s="744" t="s">
         <v>512</v>
       </c>
-      <c r="D21" s="704"/>
+      <c r="D21" s="741"/>
       <c r="E21" s="10" t="s">
         <v>263</v>
       </c>
@@ -14664,10 +14667,10 @@
       <c r="B22" s="54">
         <v>100</v>
       </c>
-      <c r="C22" s="695" t="s">
+      <c r="C22" s="780" t="s">
         <v>513</v>
       </c>
-      <c r="D22" s="696"/>
+      <c r="D22" s="781"/>
       <c r="E22" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14704,10 +14707,10 @@
       <c r="B23" s="57">
         <v>200</v>
       </c>
-      <c r="C23" s="689" t="s">
+      <c r="C23" s="699" t="s">
         <v>514</v>
       </c>
-      <c r="D23" s="690"/>
+      <c r="D23" s="700"/>
       <c r="E23" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14747,7 +14750,7 @@
       <c r="C24" s="697" t="s">
         <v>515</v>
       </c>
-      <c r="D24" s="698"/>
+      <c r="D24" s="742"/>
       <c r="E24" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14784,10 +14787,10 @@
       <c r="B25" s="57">
         <v>800</v>
       </c>
-      <c r="C25" s="689" t="s">
+      <c r="C25" s="699" t="s">
         <v>924</v>
       </c>
-      <c r="D25" s="690"/>
+      <c r="D25" s="700"/>
       <c r="E25" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14824,10 +14827,10 @@
       <c r="B26" s="57">
         <v>1000</v>
       </c>
-      <c r="C26" s="689" t="s">
+      <c r="C26" s="699" t="s">
         <v>516</v>
       </c>
-      <c r="D26" s="690"/>
+      <c r="D26" s="700"/>
       <c r="E26" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14864,10 +14867,10 @@
       <c r="B27" s="57">
         <v>1300</v>
       </c>
-      <c r="C27" s="689" t="s">
+      <c r="C27" s="699" t="s">
         <v>706</v>
       </c>
-      <c r="D27" s="690"/>
+      <c r="D27" s="700"/>
       <c r="E27" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14904,10 +14907,10 @@
       <c r="B28" s="57">
         <v>1400</v>
       </c>
-      <c r="C28" s="689" t="s">
+      <c r="C28" s="699" t="s">
         <v>517</v>
       </c>
-      <c r="D28" s="690"/>
+      <c r="D28" s="700"/>
       <c r="E28" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14944,10 +14947,10 @@
       <c r="B29" s="57">
         <v>1500</v>
       </c>
-      <c r="C29" s="689" t="s">
+      <c r="C29" s="699" t="s">
         <v>518</v>
       </c>
-      <c r="D29" s="690"/>
+      <c r="D29" s="700"/>
       <c r="E29" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14981,10 +14984,10 @@
       <c r="B30" s="57">
         <v>1600</v>
       </c>
-      <c r="C30" s="689" t="s">
+      <c r="C30" s="699" t="s">
         <v>519</v>
       </c>
-      <c r="D30" s="690"/>
+      <c r="D30" s="700"/>
       <c r="E30" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15021,10 +15024,10 @@
       <c r="B31" s="57">
         <v>1700</v>
       </c>
-      <c r="C31" s="689" t="s">
+      <c r="C31" s="699" t="s">
         <v>520</v>
       </c>
-      <c r="D31" s="690"/>
+      <c r="D31" s="700"/>
       <c r="E31" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15061,10 +15064,10 @@
       <c r="B32" s="57">
         <v>1800</v>
       </c>
-      <c r="C32" s="689" t="s">
+      <c r="C32" s="699" t="s">
         <v>521</v>
       </c>
-      <c r="D32" s="690"/>
+      <c r="D32" s="700"/>
       <c r="E32" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15101,10 +15104,10 @@
       <c r="B33" s="57">
         <v>1900</v>
       </c>
-      <c r="C33" s="689" t="s">
+      <c r="C33" s="699" t="s">
         <v>522</v>
       </c>
-      <c r="D33" s="690"/>
+      <c r="D33" s="700"/>
       <c r="E33" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15141,10 +15144,10 @@
       <c r="B34" s="57">
         <v>2000</v>
       </c>
-      <c r="C34" s="689" t="s">
+      <c r="C34" s="699" t="s">
         <v>523</v>
       </c>
-      <c r="D34" s="690"/>
+      <c r="D34" s="700"/>
       <c r="E34" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15181,10 +15184,10 @@
       <c r="B35" s="57">
         <v>2400</v>
       </c>
-      <c r="C35" s="689" t="s">
+      <c r="C35" s="699" t="s">
         <v>524</v>
       </c>
-      <c r="D35" s="690"/>
+      <c r="D35" s="700"/>
       <c r="E35" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15221,10 +15224,10 @@
       <c r="B36" s="62">
         <v>2500</v>
       </c>
-      <c r="C36" s="709" t="s">
+      <c r="C36" s="695" t="s">
         <v>525</v>
       </c>
-      <c r="D36" s="710"/>
+      <c r="D36" s="696"/>
       <c r="E36" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15261,10 +15264,10 @@
       <c r="B37" s="57">
         <v>2600</v>
       </c>
-      <c r="C37" s="709" t="s">
+      <c r="C37" s="695" t="s">
         <v>300</v>
       </c>
-      <c r="D37" s="710"/>
+      <c r="D37" s="696"/>
       <c r="E37" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15301,10 +15304,10 @@
       <c r="B38" s="57">
         <v>2700</v>
       </c>
-      <c r="C38" s="689" t="s">
+      <c r="C38" s="699" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="690"/>
+      <c r="D38" s="700"/>
       <c r="E38" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15341,10 +15344,10 @@
       <c r="B39" s="57">
         <v>2800</v>
       </c>
-      <c r="C39" s="689" t="s">
+      <c r="C39" s="699" t="s">
         <v>529</v>
       </c>
-      <c r="D39" s="690"/>
+      <c r="D39" s="700"/>
       <c r="E39" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15381,10 +15384,10 @@
       <c r="B40" s="57">
         <v>3600</v>
       </c>
-      <c r="C40" s="689" t="s">
+      <c r="C40" s="699" t="s">
         <v>530</v>
       </c>
-      <c r="D40" s="690"/>
+      <c r="D40" s="700"/>
       <c r="E40" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15421,10 +15424,10 @@
       <c r="B41" s="57">
         <v>3700</v>
       </c>
-      <c r="C41" s="689" t="s">
+      <c r="C41" s="699" t="s">
         <v>531</v>
       </c>
-      <c r="D41" s="690"/>
+      <c r="D41" s="700"/>
       <c r="E41" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15515,10 +15518,10 @@
       <c r="B43" s="57">
         <v>4100</v>
       </c>
-      <c r="C43" s="689" t="s">
+      <c r="C43" s="699" t="s">
         <v>381</v>
       </c>
-      <c r="D43" s="690"/>
+      <c r="D43" s="700"/>
       <c r="E43" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15556,10 +15559,10 @@
       <c r="B44" s="57">
         <v>4200</v>
       </c>
-      <c r="C44" s="689" t="s">
+      <c r="C44" s="699" t="s">
         <v>382</v>
       </c>
-      <c r="D44" s="690"/>
+      <c r="D44" s="700"/>
       <c r="E44" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15597,10 +15600,10 @@
       <c r="B45" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="C45" s="689" t="s">
+      <c r="C45" s="699" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="690"/>
+      <c r="D45" s="700"/>
       <c r="E45" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15638,10 +15641,10 @@
       <c r="B46" s="57">
         <v>4600</v>
       </c>
-      <c r="C46" s="689" t="s">
+      <c r="C46" s="699" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="690"/>
+      <c r="D46" s="700"/>
       <c r="E46" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15678,10 +15681,10 @@
       <c r="B47" s="57">
         <v>4700</v>
       </c>
-      <c r="C47" s="689" t="s">
+      <c r="C47" s="699" t="s">
         <v>1410</v>
       </c>
-      <c r="D47" s="690"/>
+      <c r="D47" s="700"/>
       <c r="E47" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15718,10 +15721,10 @@
       <c r="B48" s="57">
         <v>4800</v>
       </c>
-      <c r="C48" s="705" t="s">
+      <c r="C48" s="774" t="s">
         <v>455</v>
       </c>
-      <c r="D48" s="706"/>
+      <c r="D48" s="775"/>
       <c r="E48" s="202" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15850,12 +15853,12 @@
       <c r="L53" s="74"/>
     </row>
     <row r="54" spans="1:15" s="46" customFormat="1" ht="44.25" customHeight="1">
-      <c r="B54" s="707" t="e">
+      <c r="B54" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C54" s="708"/>
-      <c r="D54" s="708"/>
+      <c r="C54" s="730"/>
+      <c r="D54" s="730"/>
       <c r="E54" s="79"/>
       <c r="F54" s="79"/>
       <c r="G54" s="30"/>
@@ -15887,12 +15890,12 @@
       <c r="L55" s="74"/>
     </row>
     <row r="56" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickBot="1">
-      <c r="B56" s="723" t="e">
+      <c r="B56" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C56" s="724"/>
-      <c r="D56" s="724"/>
+      <c r="C56" s="692"/>
+      <c r="D56" s="692"/>
       <c r="E56" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -15947,12 +15950,12 @@
       <c r="L58" s="74"/>
     </row>
     <row r="59" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B59" s="723" t="e">
+      <c r="B59" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C59" s="724"/>
-      <c r="D59" s="724"/>
+      <c r="C59" s="692"/>
+      <c r="D59" s="692"/>
       <c r="E59" s="79" t="s">
         <v>505</v>
       </c>
@@ -16023,10 +16026,10 @@
     </row>
     <row r="63" spans="1:15" s="46" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="B63" s="87"/>
-      <c r="C63" s="719" t="s">
+      <c r="C63" s="770" t="s">
         <v>473</v>
       </c>
-      <c r="D63" s="720"/>
+      <c r="D63" s="771"/>
       <c r="E63" s="48" t="s">
         <v>509</v>
       </c>
@@ -16040,16 +16043,16 @@
       <c r="K63" s="169">
         <v>1</v>
       </c>
-      <c r="L63" s="711" t="s">
+      <c r="L63" s="764" t="s">
         <v>1429</v>
       </c>
-      <c r="M63" s="711" t="s">
+      <c r="M63" s="764" t="s">
         <v>1430</v>
       </c>
-      <c r="N63" s="711" t="s">
+      <c r="N63" s="764" t="s">
         <v>1431</v>
       </c>
-      <c r="O63" s="711" t="s">
+      <c r="O63" s="764" t="s">
         <v>1432</v>
       </c>
     </row>
@@ -16057,10 +16060,10 @@
       <c r="B64" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="C64" s="701" t="s">
+      <c r="C64" s="711" t="s">
         <v>707</v>
       </c>
-      <c r="D64" s="716"/>
+      <c r="D64" s="767"/>
       <c r="E64" s="50">
         <v>2017</v>
       </c>
@@ -16082,17 +16085,17 @@
       <c r="K64" s="169">
         <v>1</v>
       </c>
-      <c r="L64" s="725"/>
-      <c r="M64" s="725"/>
-      <c r="N64" s="712"/>
-      <c r="O64" s="712"/>
+      <c r="L64" s="772"/>
+      <c r="M64" s="772"/>
+      <c r="N64" s="765"/>
+      <c r="O64" s="765"/>
     </row>
     <row r="65" spans="1:15" s="46" customFormat="1" ht="21.75" thickBot="1">
       <c r="B65" s="88"/>
-      <c r="C65" s="717" t="s">
+      <c r="C65" s="768" t="s">
         <v>387</v>
       </c>
-      <c r="D65" s="718"/>
+      <c r="D65" s="769"/>
       <c r="E65" s="10" t="s">
         <v>263</v>
       </c>
@@ -16114,10 +16117,10 @@
       <c r="K65" s="169">
         <v>1</v>
       </c>
-      <c r="L65" s="726"/>
-      <c r="M65" s="726"/>
-      <c r="N65" s="713"/>
-      <c r="O65" s="713"/>
+      <c r="L65" s="773"/>
+      <c r="M65" s="773"/>
+      <c r="N65" s="766"/>
+      <c r="O65" s="766"/>
     </row>
     <row r="66" spans="1:15" s="56" customFormat="1" ht="34.5" customHeight="1">
       <c r="A66" s="63">
@@ -16126,10 +16129,10 @@
       <c r="B66" s="54">
         <v>100</v>
       </c>
-      <c r="C66" s="727" t="s">
+      <c r="C66" s="752" t="s">
         <v>388</v>
       </c>
-      <c r="D66" s="728"/>
+      <c r="D66" s="732"/>
       <c r="E66" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16170,10 +16173,10 @@
       <c r="B67" s="57">
         <v>200</v>
       </c>
-      <c r="C67" s="709" t="s">
+      <c r="C67" s="695" t="s">
         <v>391</v>
       </c>
-      <c r="D67" s="710"/>
+      <c r="D67" s="696"/>
       <c r="E67" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16214,10 +16217,10 @@
       <c r="B68" s="57">
         <v>500</v>
       </c>
-      <c r="C68" s="689" t="s">
+      <c r="C68" s="699" t="s">
         <v>579</v>
       </c>
-      <c r="D68" s="690"/>
+      <c r="D68" s="700"/>
       <c r="E68" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16261,7 +16264,7 @@
       <c r="C69" s="697" t="s">
         <v>585</v>
       </c>
-      <c r="D69" s="729"/>
+      <c r="D69" s="698"/>
       <c r="E69" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16302,10 +16305,10 @@
       <c r="B70" s="57">
         <v>1000</v>
       </c>
-      <c r="C70" s="709" t="s">
+      <c r="C70" s="695" t="s">
         <v>586</v>
       </c>
-      <c r="D70" s="710"/>
+      <c r="D70" s="696"/>
       <c r="E70" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16346,10 +16349,10 @@
       <c r="B71" s="57">
         <v>1900</v>
       </c>
-      <c r="C71" s="721" t="s">
+      <c r="C71" s="693" t="s">
         <v>456</v>
       </c>
-      <c r="D71" s="722"/>
+      <c r="D71" s="694"/>
       <c r="E71" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16390,10 +16393,10 @@
       <c r="B72" s="57">
         <v>2100</v>
       </c>
-      <c r="C72" s="721" t="s">
+      <c r="C72" s="693" t="s">
         <v>741</v>
       </c>
-      <c r="D72" s="722"/>
+      <c r="D72" s="694"/>
       <c r="E72" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16434,10 +16437,10 @@
       <c r="B73" s="57">
         <v>2200</v>
       </c>
-      <c r="C73" s="721" t="s">
+      <c r="C73" s="693" t="s">
         <v>604</v>
       </c>
-      <c r="D73" s="722"/>
+      <c r="D73" s="694"/>
       <c r="E73" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16478,10 +16481,10 @@
       <c r="B74" s="57">
         <v>2500</v>
       </c>
-      <c r="C74" s="721" t="s">
+      <c r="C74" s="693" t="s">
         <v>606</v>
       </c>
-      <c r="D74" s="722"/>
+      <c r="D74" s="694"/>
       <c r="E74" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16522,10 +16525,10 @@
       <c r="B75" s="57">
         <v>2600</v>
       </c>
-      <c r="C75" s="714" t="s">
+      <c r="C75" s="701" t="s">
         <v>607</v>
       </c>
-      <c r="D75" s="715"/>
+      <c r="D75" s="702"/>
       <c r="E75" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16566,10 +16569,10 @@
       <c r="B76" s="57">
         <v>2700</v>
       </c>
-      <c r="C76" s="714" t="s">
+      <c r="C76" s="701" t="s">
         <v>608</v>
       </c>
-      <c r="D76" s="715"/>
+      <c r="D76" s="702"/>
       <c r="E76" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16610,10 +16613,10 @@
       <c r="B77" s="57">
         <v>2800</v>
       </c>
-      <c r="C77" s="714" t="s">
+      <c r="C77" s="701" t="s">
         <v>1408</v>
       </c>
-      <c r="D77" s="715"/>
+      <c r="D77" s="702"/>
       <c r="E77" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16654,10 +16657,10 @@
       <c r="B78" s="57">
         <v>2900</v>
       </c>
-      <c r="C78" s="721" t="s">
+      <c r="C78" s="693" t="s">
         <v>609</v>
       </c>
-      <c r="D78" s="722"/>
+      <c r="D78" s="694"/>
       <c r="E78" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16742,10 +16745,10 @@
       <c r="B80" s="57">
         <v>3900</v>
       </c>
-      <c r="C80" s="721" t="s">
+      <c r="C80" s="693" t="s">
         <v>618</v>
       </c>
-      <c r="D80" s="722"/>
+      <c r="D80" s="694"/>
       <c r="E80" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16786,10 +16789,10 @@
       <c r="B81" s="57">
         <v>4000</v>
       </c>
-      <c r="C81" s="721" t="s">
+      <c r="C81" s="693" t="s">
         <v>619</v>
       </c>
-      <c r="D81" s="722"/>
+      <c r="D81" s="694"/>
       <c r="E81" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16830,10 +16833,10 @@
       <c r="B82" s="57">
         <v>4100</v>
       </c>
-      <c r="C82" s="721" t="s">
+      <c r="C82" s="693" t="s">
         <v>620</v>
       </c>
-      <c r="D82" s="722"/>
+      <c r="D82" s="694"/>
       <c r="E82" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16874,10 +16877,10 @@
       <c r="B83" s="57">
         <v>4200</v>
       </c>
-      <c r="C83" s="721" t="s">
+      <c r="C83" s="693" t="s">
         <v>621</v>
       </c>
-      <c r="D83" s="722"/>
+      <c r="D83" s="694"/>
       <c r="E83" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16918,10 +16921,10 @@
       <c r="B84" s="57">
         <v>4300</v>
       </c>
-      <c r="C84" s="721" t="s">
+      <c r="C84" s="693" t="s">
         <v>1015</v>
       </c>
-      <c r="D84" s="722"/>
+      <c r="D84" s="694"/>
       <c r="E84" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16962,10 +16965,10 @@
       <c r="B85" s="57">
         <v>4400</v>
       </c>
-      <c r="C85" s="721" t="s">
+      <c r="C85" s="693" t="s">
         <v>1012</v>
       </c>
-      <c r="D85" s="722"/>
+      <c r="D85" s="694"/>
       <c r="E85" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17006,10 +17009,10 @@
       <c r="B86" s="57">
         <v>4500</v>
       </c>
-      <c r="C86" s="721" t="s">
+      <c r="C86" s="693" t="s">
         <v>1409</v>
       </c>
-      <c r="D86" s="722"/>
+      <c r="D86" s="694"/>
       <c r="E86" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17050,10 +17053,10 @@
       <c r="B87" s="57">
         <v>4600</v>
       </c>
-      <c r="C87" s="714" t="s">
+      <c r="C87" s="701" t="s">
         <v>630</v>
       </c>
-      <c r="D87" s="715"/>
+      <c r="D87" s="702"/>
       <c r="E87" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17094,10 +17097,10 @@
       <c r="B88" s="57">
         <v>4900</v>
       </c>
-      <c r="C88" s="721" t="s">
+      <c r="C88" s="693" t="s">
         <v>460</v>
       </c>
-      <c r="D88" s="722"/>
+      <c r="D88" s="694"/>
       <c r="E88" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17138,10 +17141,10 @@
       <c r="B89" s="96">
         <v>5100</v>
       </c>
-      <c r="C89" s="730" t="s">
+      <c r="C89" s="757" t="s">
         <v>631</v>
       </c>
-      <c r="D89" s="731"/>
+      <c r="D89" s="758"/>
       <c r="E89" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17182,10 +17185,10 @@
       <c r="B90" s="96">
         <v>5200</v>
       </c>
-      <c r="C90" s="730" t="s">
+      <c r="C90" s="757" t="s">
         <v>632</v>
       </c>
-      <c r="D90" s="731"/>
+      <c r="D90" s="758"/>
       <c r="E90" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17226,10 +17229,10 @@
       <c r="B91" s="96">
         <v>5300</v>
       </c>
-      <c r="C91" s="730" t="s">
+      <c r="C91" s="757" t="s">
         <v>191</v>
       </c>
-      <c r="D91" s="731"/>
+      <c r="D91" s="758"/>
       <c r="E91" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17270,10 +17273,10 @@
       <c r="B92" s="96">
         <v>5400</v>
       </c>
-      <c r="C92" s="730" t="s">
+      <c r="C92" s="757" t="s">
         <v>643</v>
       </c>
-      <c r="D92" s="731"/>
+      <c r="D92" s="758"/>
       <c r="E92" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17314,10 +17317,10 @@
       <c r="B93" s="57">
         <v>5500</v>
       </c>
-      <c r="C93" s="721" t="s">
+      <c r="C93" s="693" t="s">
         <v>644</v>
       </c>
-      <c r="D93" s="722"/>
+      <c r="D93" s="694"/>
       <c r="E93" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17358,10 +17361,10 @@
       <c r="B94" s="96">
         <v>5700</v>
       </c>
-      <c r="C94" s="732" t="s">
+      <c r="C94" s="759" t="s">
         <v>649</v>
       </c>
-      <c r="D94" s="733"/>
+      <c r="D94" s="760"/>
       <c r="E94" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17402,10 +17405,10 @@
       <c r="B95" s="98" t="s">
         <v>708</v>
       </c>
-      <c r="C95" s="734" t="s">
+      <c r="C95" s="761" t="s">
         <v>653</v>
       </c>
-      <c r="D95" s="735"/>
+      <c r="D95" s="762"/>
       <c r="E95" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17444,10 +17447,10 @@
         <v>825</v>
       </c>
       <c r="B96" s="104"/>
-      <c r="C96" s="736" t="s">
+      <c r="C96" s="763" t="s">
         <v>654</v>
       </c>
-      <c r="D96" s="736"/>
+      <c r="D96" s="763"/>
       <c r="E96" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17513,12 +17516,12 @@
     </row>
     <row r="99" spans="1:11" ht="40.5" customHeight="1">
       <c r="A99" s="70"/>
-      <c r="B99" s="707" t="e">
+      <c r="B99" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C99" s="708"/>
-      <c r="D99" s="708"/>
+      <c r="C99" s="730"/>
+      <c r="D99" s="730"/>
       <c r="E99" s="79"/>
       <c r="F99" s="79"/>
       <c r="K99" s="167">
@@ -17541,12 +17544,12 @@
     </row>
     <row r="101" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A101" s="70"/>
-      <c r="B101" s="723" t="e">
+      <c r="B101" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C101" s="724"/>
-      <c r="D101" s="724"/>
+      <c r="C101" s="692"/>
+      <c r="D101" s="692"/>
       <c r="E101" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -17585,12 +17588,12 @@
     </row>
     <row r="104" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A104" s="70"/>
-      <c r="B104" s="723" t="e">
+      <c r="B104" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C104" s="724"/>
-      <c r="D104" s="724"/>
+      <c r="C104" s="692"/>
+      <c r="D104" s="692"/>
       <c r="E104" s="79" t="s">
         <v>505</v>
       </c>
@@ -17640,10 +17643,10 @@
     <row r="108" spans="1:11" ht="21.75" thickBot="1">
       <c r="A108" s="70"/>
       <c r="B108" s="138"/>
-      <c r="C108" s="746" t="s">
+      <c r="C108" s="743" t="s">
         <v>908</v>
       </c>
-      <c r="D108" s="747"/>
+      <c r="D108" s="753"/>
       <c r="E108" s="48" t="s">
         <v>509</v>
       </c>
@@ -17663,10 +17666,10 @@
       <c r="B109" s="107" t="s">
         <v>474</v>
       </c>
-      <c r="C109" s="748" t="s">
+      <c r="C109" s="754" t="s">
         <v>707</v>
       </c>
-      <c r="D109" s="749"/>
+      <c r="D109" s="755"/>
       <c r="E109" s="50">
         <v>2017</v>
       </c>
@@ -17694,10 +17697,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="750" t="s">
+      <c r="C110" s="740" t="s">
         <v>251</v>
       </c>
-      <c r="D110" s="704"/>
+      <c r="D110" s="741"/>
       <c r="E110" s="10" t="s">
         <v>263</v>
       </c>
@@ -17725,10 +17728,10 @@
         <v>2</v>
       </c>
       <c r="B111" s="14"/>
-      <c r="C111" s="751" t="s">
+      <c r="C111" s="756" t="s">
         <v>463</v>
       </c>
-      <c r="D111" s="704"/>
+      <c r="D111" s="741"/>
       <c r="E111" s="12"/>
       <c r="F111" s="29"/>
       <c r="G111" s="29"/>
@@ -17746,10 +17749,10 @@
       <c r="B112" s="54">
         <v>3000</v>
       </c>
-      <c r="C112" s="752" t="s">
+      <c r="C112" s="736" t="s">
         <v>909</v>
       </c>
-      <c r="D112" s="753"/>
+      <c r="D112" s="737"/>
       <c r="E112" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17786,10 +17789,10 @@
       <c r="B113" s="57">
         <v>3100</v>
       </c>
-      <c r="C113" s="689" t="s">
+      <c r="C113" s="699" t="s">
         <v>464</v>
       </c>
-      <c r="D113" s="690"/>
+      <c r="D113" s="700"/>
       <c r="E113" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17826,10 +17829,10 @@
       <c r="B114" s="110">
         <v>3200</v>
       </c>
-      <c r="C114" s="737" t="s">
+      <c r="C114" s="745" t="s">
         <v>758</v>
       </c>
-      <c r="D114" s="738"/>
+      <c r="D114" s="690"/>
       <c r="E114" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17866,10 +17869,10 @@
       <c r="B115" s="57">
         <v>6000</v>
       </c>
-      <c r="C115" s="727" t="s">
+      <c r="C115" s="752" t="s">
         <v>635</v>
       </c>
-      <c r="D115" s="728"/>
+      <c r="D115" s="732"/>
       <c r="E115" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17906,10 +17909,10 @@
       <c r="B116" s="57">
         <v>6100</v>
       </c>
-      <c r="C116" s="709" t="s">
+      <c r="C116" s="695" t="s">
         <v>636</v>
       </c>
-      <c r="D116" s="710"/>
+      <c r="D116" s="696"/>
       <c r="E116" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17946,10 +17949,10 @@
       <c r="B117" s="57">
         <v>6200</v>
       </c>
-      <c r="C117" s="755" t="s">
+      <c r="C117" s="728" t="s">
         <v>637</v>
       </c>
-      <c r="D117" s="756"/>
+      <c r="D117" s="733"/>
       <c r="E117" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17986,10 +17989,10 @@
       <c r="B118" s="57">
         <v>6300</v>
       </c>
-      <c r="C118" s="743" t="s">
+      <c r="C118" s="725" t="s">
         <v>638</v>
       </c>
-      <c r="D118" s="715"/>
+      <c r="D118" s="702"/>
       <c r="E118" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18026,10 +18029,10 @@
       <c r="B119" s="57">
         <v>6400</v>
       </c>
-      <c r="C119" s="741" t="s">
+      <c r="C119" s="748" t="s">
         <v>639</v>
       </c>
-      <c r="D119" s="742"/>
+      <c r="D119" s="749"/>
       <c r="E119" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18124,10 +18127,10 @@
       <c r="B121" s="57">
         <v>6600</v>
       </c>
-      <c r="C121" s="743" t="s">
+      <c r="C121" s="725" t="s">
         <v>254</v>
       </c>
-      <c r="D121" s="715"/>
+      <c r="D121" s="702"/>
       <c r="E121" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18164,10 +18167,10 @@
       <c r="B122" s="57">
         <v>6700</v>
       </c>
-      <c r="C122" s="743" t="s">
+      <c r="C122" s="725" t="s">
         <v>687</v>
       </c>
-      <c r="D122" s="715"/>
+      <c r="D122" s="702"/>
       <c r="E122" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18204,10 +18207,10 @@
       <c r="B123" s="57">
         <v>6900</v>
       </c>
-      <c r="C123" s="744" t="s">
+      <c r="C123" s="750" t="s">
         <v>640</v>
       </c>
-      <c r="D123" s="745"/>
+      <c r="D123" s="751"/>
       <c r="E123" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18242,10 +18245,10 @@
         <v>260</v>
       </c>
       <c r="B124" s="71"/>
-      <c r="C124" s="759" t="s">
+      <c r="C124" s="738" t="s">
         <v>252</v>
       </c>
-      <c r="D124" s="760"/>
+      <c r="D124" s="739"/>
       <c r="E124" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18279,10 +18282,10 @@
         <v>261</v>
       </c>
       <c r="B125" s="112"/>
-      <c r="C125" s="750" t="s">
+      <c r="C125" s="740" t="s">
         <v>253</v>
       </c>
-      <c r="D125" s="704"/>
+      <c r="D125" s="741"/>
       <c r="E125" s="113"/>
       <c r="F125" s="170"/>
       <c r="G125" s="170"/>
@@ -18300,10 +18303,10 @@
       <c r="B126" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C126" s="757" t="s">
+      <c r="C126" s="734" t="s">
         <v>899</v>
       </c>
-      <c r="D126" s="758"/>
+      <c r="D126" s="735"/>
       <c r="E126" s="170"/>
       <c r="F126" s="170"/>
       <c r="G126" s="170"/>
@@ -18321,10 +18324,10 @@
       <c r="B127" s="57">
         <v>7400</v>
       </c>
-      <c r="C127" s="752" t="s">
+      <c r="C127" s="736" t="s">
         <v>900</v>
       </c>
-      <c r="D127" s="753"/>
+      <c r="D127" s="737"/>
       <c r="E127" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18361,10 +18364,10 @@
       <c r="B128" s="57">
         <v>7500</v>
       </c>
-      <c r="C128" s="689" t="s">
+      <c r="C128" s="699" t="s">
         <v>710</v>
       </c>
-      <c r="D128" s="690"/>
+      <c r="D128" s="700"/>
       <c r="E128" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18404,7 +18407,7 @@
       <c r="C129" s="697" t="s">
         <v>641</v>
       </c>
-      <c r="D129" s="698"/>
+      <c r="D129" s="742"/>
       <c r="E129" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18444,7 +18447,7 @@
       <c r="C130" s="697" t="s">
         <v>642</v>
       </c>
-      <c r="D130" s="729"/>
+      <c r="D130" s="698"/>
       <c r="E130" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18481,10 +18484,10 @@
       <c r="B131" s="96">
         <v>7800</v>
       </c>
-      <c r="C131" s="739" t="s">
-        <v>0</v>
-      </c>
-      <c r="D131" s="740"/>
+      <c r="C131" s="746" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="747"/>
       <c r="E131" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18519,10 +18522,10 @@
         <v>315</v>
       </c>
       <c r="B132" s="71"/>
-      <c r="C132" s="759" t="s">
+      <c r="C132" s="738" t="s">
         <v>898</v>
       </c>
-      <c r="D132" s="760"/>
+      <c r="D132" s="739"/>
       <c r="E132" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18580,12 +18583,12 @@
     </row>
     <row r="136" spans="1:11" ht="42" customHeight="1">
       <c r="A136" s="103"/>
-      <c r="B136" s="707" t="e">
+      <c r="B136" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C136" s="708"/>
-      <c r="D136" s="708"/>
+      <c r="C136" s="730"/>
+      <c r="D136" s="730"/>
       <c r="E136" s="79"/>
       <c r="F136" s="79"/>
       <c r="K136" s="167">
@@ -18608,12 +18611,12 @@
     </row>
     <row r="138" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A138" s="103"/>
-      <c r="B138" s="723" t="e">
+      <c r="B138" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C138" s="724"/>
-      <c r="D138" s="724"/>
+      <c r="C138" s="692"/>
+      <c r="D138" s="692"/>
       <c r="E138" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18652,12 +18655,12 @@
     </row>
     <row r="141" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A141" s="103"/>
-      <c r="B141" s="723" t="e">
+      <c r="B141" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C141" s="724"/>
-      <c r="D141" s="724"/>
+      <c r="C141" s="692"/>
+      <c r="D141" s="692"/>
       <c r="E141" s="79" t="s">
         <v>505</v>
       </c>
@@ -18847,12 +18850,12 @@
     </row>
     <row r="152" spans="1:11" ht="44.25" customHeight="1">
       <c r="A152" s="103"/>
-      <c r="B152" s="707" t="e">
+      <c r="B152" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C152" s="708"/>
-      <c r="D152" s="708"/>
+      <c r="C152" s="730"/>
+      <c r="D152" s="730"/>
       <c r="E152" s="79"/>
       <c r="F152" s="79"/>
       <c r="K152" s="167">
@@ -18875,12 +18878,12 @@
     </row>
     <row r="154" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A154" s="103"/>
-      <c r="B154" s="723" t="e">
+      <c r="B154" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C154" s="724"/>
-      <c r="D154" s="724"/>
+      <c r="C154" s="692"/>
+      <c r="D154" s="692"/>
       <c r="E154" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18919,12 +18922,12 @@
     </row>
     <row r="157" spans="1:11" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A157" s="103"/>
-      <c r="B157" s="723" t="e">
+      <c r="B157" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C157" s="724"/>
-      <c r="D157" s="724"/>
+      <c r="C157" s="692"/>
+      <c r="D157" s="692"/>
       <c r="E157" s="79" t="s">
         <v>505</v>
       </c>
@@ -18974,10 +18977,10 @@
     <row r="161" spans="1:65" ht="21.75" thickBot="1">
       <c r="A161" s="103"/>
       <c r="B161" s="112"/>
-      <c r="C161" s="746" t="s">
+      <c r="C161" s="743" t="s">
         <v>684</v>
       </c>
-      <c r="D161" s="702"/>
+      <c r="D161" s="710"/>
       <c r="E161" s="48" t="s">
         <v>509</v>
       </c>
@@ -18997,10 +19000,10 @@
       <c r="B162" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C162" s="701" t="s">
+      <c r="C162" s="711" t="s">
         <v>707</v>
       </c>
-      <c r="D162" s="700"/>
+      <c r="D162" s="708"/>
       <c r="E162" s="50">
         <v>2017</v>
       </c>
@@ -19028,10 +19031,10 @@
         <v>1</v>
       </c>
       <c r="B163" s="139"/>
-      <c r="C163" s="703" t="s">
+      <c r="C163" s="744" t="s">
         <v>685</v>
       </c>
-      <c r="D163" s="704"/>
+      <c r="D163" s="741"/>
       <c r="E163" s="10" t="s">
         <v>263</v>
       </c>
@@ -19061,10 +19064,10 @@
       <c r="B164" s="54">
         <v>7000</v>
       </c>
-      <c r="C164" s="754" t="s">
+      <c r="C164" s="731" t="s">
         <v>902</v>
       </c>
-      <c r="D164" s="728"/>
+      <c r="D164" s="732"/>
       <c r="E164" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19101,10 +19104,10 @@
       <c r="B165" s="57">
         <v>7100</v>
       </c>
-      <c r="C165" s="721" t="s">
+      <c r="C165" s="693" t="s">
         <v>903</v>
       </c>
-      <c r="D165" s="722"/>
+      <c r="D165" s="694"/>
       <c r="E165" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19141,10 +19144,10 @@
       <c r="B166" s="57">
         <v>7200</v>
       </c>
-      <c r="C166" s="721" t="s">
+      <c r="C166" s="693" t="s">
         <v>1414</v>
       </c>
-      <c r="D166" s="722"/>
+      <c r="D166" s="694"/>
       <c r="E166" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19181,10 +19184,10 @@
       <c r="B167" s="57">
         <v>7300</v>
       </c>
-      <c r="C167" s="714" t="s">
+      <c r="C167" s="701" t="s">
         <v>904</v>
       </c>
-      <c r="D167" s="715"/>
+      <c r="D167" s="702"/>
       <c r="E167" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19221,10 +19224,10 @@
       <c r="B168" s="57">
         <v>7900</v>
       </c>
-      <c r="C168" s="781" t="s">
+      <c r="C168" s="703" t="s">
         <v>905</v>
       </c>
-      <c r="D168" s="782"/>
+      <c r="D168" s="704"/>
       <c r="E168" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19314,10 +19317,10 @@
       <c r="B169" s="57">
         <v>8000</v>
       </c>
-      <c r="C169" s="709" t="s">
+      <c r="C169" s="695" t="s">
         <v>711</v>
       </c>
-      <c r="D169" s="710"/>
+      <c r="D169" s="696"/>
       <c r="E169" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19357,7 +19360,7 @@
       <c r="C170" s="697" t="s">
         <v>712</v>
       </c>
-      <c r="D170" s="729"/>
+      <c r="D170" s="698"/>
       <c r="E170" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19397,7 +19400,7 @@
       <c r="C171" s="697" t="s">
         <v>101</v>
       </c>
-      <c r="D171" s="729"/>
+      <c r="D171" s="698"/>
       <c r="E171" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19434,10 +19437,10 @@
       <c r="B172" s="57">
         <v>8300</v>
       </c>
-      <c r="C172" s="689" t="s">
+      <c r="C172" s="699" t="s">
         <v>713</v>
       </c>
-      <c r="D172" s="690"/>
+      <c r="D172" s="700"/>
       <c r="E172" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19474,10 +19477,10 @@
       <c r="B173" s="57">
         <v>8500</v>
       </c>
-      <c r="C173" s="709" t="s">
+      <c r="C173" s="695" t="s">
         <v>102</v>
       </c>
-      <c r="D173" s="710"/>
+      <c r="D173" s="696"/>
       <c r="E173" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19514,10 +19517,10 @@
       <c r="B174" s="57">
         <v>8600</v>
       </c>
-      <c r="C174" s="709" t="s">
+      <c r="C174" s="695" t="s">
         <v>103</v>
       </c>
-      <c r="D174" s="710"/>
+      <c r="D174" s="696"/>
       <c r="E174" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19557,7 +19560,7 @@
       <c r="C175" s="697" t="s">
         <v>265</v>
       </c>
-      <c r="D175" s="729"/>
+      <c r="D175" s="698"/>
       <c r="E175" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19597,7 +19600,7 @@
       <c r="C176" s="697" t="s">
         <v>910</v>
       </c>
-      <c r="D176" s="729"/>
+      <c r="D176" s="698"/>
       <c r="E176" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19634,10 +19637,10 @@
       <c r="B177" s="57">
         <v>8900</v>
       </c>
-      <c r="C177" s="743" t="s">
+      <c r="C177" s="725" t="s">
         <v>759</v>
       </c>
-      <c r="D177" s="715"/>
+      <c r="D177" s="702"/>
       <c r="E177" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19674,10 +19677,10 @@
       <c r="B178" s="57">
         <v>9000</v>
       </c>
-      <c r="C178" s="709" t="s">
+      <c r="C178" s="695" t="s">
         <v>104</v>
       </c>
-      <c r="D178" s="710"/>
+      <c r="D178" s="696"/>
       <c r="E178" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19714,10 +19717,10 @@
       <c r="B179" s="57">
         <v>9100</v>
       </c>
-      <c r="C179" s="743" t="s">
+      <c r="C179" s="725" t="s">
         <v>911</v>
       </c>
-      <c r="D179" s="755"/>
+      <c r="D179" s="728"/>
       <c r="E179" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19754,10 +19757,10 @@
       <c r="B180" s="57">
         <v>9200</v>
       </c>
-      <c r="C180" s="778" t="s">
+      <c r="C180" s="726" t="s">
         <v>714</v>
       </c>
-      <c r="D180" s="729"/>
+      <c r="D180" s="698"/>
       <c r="E180" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19794,10 +19797,10 @@
       <c r="B181" s="57">
         <v>9300</v>
       </c>
-      <c r="C181" s="709" t="s">
+      <c r="C181" s="695" t="s">
         <v>715</v>
       </c>
-      <c r="D181" s="710"/>
+      <c r="D181" s="696"/>
       <c r="E181" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19834,10 +19837,10 @@
       <c r="B182" s="57">
         <v>9500</v>
       </c>
-      <c r="C182" s="778" t="s">
+      <c r="C182" s="726" t="s">
         <v>716</v>
       </c>
-      <c r="D182" s="779"/>
+      <c r="D182" s="727"/>
       <c r="E182" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19874,10 +19877,10 @@
       <c r="B183" s="57">
         <v>9600</v>
       </c>
-      <c r="C183" s="778" t="s">
+      <c r="C183" s="726" t="s">
         <v>717</v>
       </c>
-      <c r="D183" s="729"/>
+      <c r="D183" s="698"/>
       <c r="E183" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19914,10 +19917,10 @@
       <c r="B184" s="57">
         <v>9800</v>
       </c>
-      <c r="C184" s="780" t="s">
+      <c r="C184" s="689" t="s">
         <v>465</v>
       </c>
-      <c r="D184" s="738"/>
+      <c r="D184" s="690"/>
       <c r="E184" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19952,10 +19955,10 @@
         <v>610</v>
       </c>
       <c r="B185" s="146"/>
-      <c r="C185" s="701" t="s">
+      <c r="C185" s="711" t="s">
         <v>930</v>
       </c>
-      <c r="D185" s="700"/>
+      <c r="D185" s="708"/>
       <c r="E185" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -20018,12 +20021,12 @@
       </c>
     </row>
     <row r="189" spans="1:11" ht="42" customHeight="1">
-      <c r="B189" s="707" t="e">
+      <c r="B189" s="729" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C189" s="708"/>
-      <c r="D189" s="708"/>
+      <c r="C189" s="730"/>
+      <c r="D189" s="730"/>
       <c r="E189" s="79"/>
       <c r="F189" s="79"/>
       <c r="G189" s="56"/>
@@ -20046,12 +20049,12 @@
       </c>
     </row>
     <row r="191" spans="1:11" ht="21.75" thickBot="1">
-      <c r="B191" s="723" t="e">
+      <c r="B191" s="691" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C191" s="724"/>
-      <c r="D191" s="724"/>
+      <c r="C191" s="692"/>
+      <c r="D191" s="692"/>
       <c r="E191" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -20090,12 +20093,12 @@
       </c>
     </row>
     <row r="194" spans="2:11" ht="22.5" thickTop="1" thickBot="1">
-      <c r="B194" s="723" t="e">
+      <c r="B194" s="691" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C194" s="724"/>
-      <c r="D194" s="724"/>
+      <c r="C194" s="692"/>
+      <c r="D194" s="692"/>
       <c r="E194" s="79" t="s">
         <v>505</v>
       </c>
@@ -20149,10 +20152,10 @@
       <c r="B198" s="153" t="s">
         <v>474</v>
       </c>
-      <c r="C198" s="763" t="s">
+      <c r="C198" s="707" t="s">
         <v>718</v>
       </c>
-      <c r="D198" s="700"/>
+      <c r="D198" s="708"/>
       <c r="E198" s="48" t="s">
         <v>509</v>
       </c>
@@ -20169,8 +20172,8 @@
     </row>
     <row r="199" spans="2:11" ht="45.75" thickBot="1">
       <c r="B199" s="154"/>
-      <c r="C199" s="764"/>
-      <c r="D199" s="702"/>
+      <c r="C199" s="709"/>
+      <c r="D199" s="710"/>
       <c r="E199" s="50">
         <v>2017</v>
       </c>
@@ -20197,10 +20200,10 @@
       <c r="B200" s="155" t="s">
         <v>719</v>
       </c>
-      <c r="C200" s="776" t="s">
+      <c r="C200" s="723" t="s">
         <v>720</v>
       </c>
-      <c r="D200" s="777"/>
+      <c r="D200" s="724"/>
       <c r="E200" s="187" t="e">
         <f>SUMIF(#REF!,1,#REF!)</f>
         <v>#REF!</v>
@@ -20233,10 +20236,10 @@
       <c r="B201" s="156" t="s">
         <v>721</v>
       </c>
-      <c r="C201" s="769" t="s">
+      <c r="C201" s="716" t="s">
         <v>722</v>
       </c>
-      <c r="D201" s="770"/>
+      <c r="D201" s="717"/>
       <c r="E201" s="188" t="e">
         <f>SUMIF(#REF!,2,#REF!)</f>
         <v>#REF!</v>
@@ -20269,10 +20272,10 @@
       <c r="B202" s="156" t="s">
         <v>723</v>
       </c>
-      <c r="C202" s="769" t="s">
+      <c r="C202" s="716" t="s">
         <v>724</v>
       </c>
-      <c r="D202" s="770"/>
+      <c r="D202" s="717"/>
       <c r="E202" s="188" t="e">
         <f>SUMIF(#REF!,3,#REF!)</f>
         <v>#REF!</v>
@@ -20305,10 +20308,10 @@
       <c r="B203" s="156" t="s">
         <v>725</v>
       </c>
-      <c r="C203" s="772" t="s">
+      <c r="C203" s="719" t="s">
         <v>726</v>
       </c>
-      <c r="D203" s="773"/>
+      <c r="D203" s="720"/>
       <c r="E203" s="188" t="e">
         <f>SUMIF(#REF!,4,#REF!)</f>
         <v>#REF!</v>
@@ -20341,10 +20344,10 @@
       <c r="B204" s="156" t="s">
         <v>727</v>
       </c>
-      <c r="C204" s="774" t="s">
+      <c r="C204" s="721" t="s">
         <v>728</v>
       </c>
-      <c r="D204" s="775"/>
+      <c r="D204" s="722"/>
       <c r="E204" s="188" t="e">
         <f>SUMIF(#REF!,5,#REF!)</f>
         <v>#REF!</v>
@@ -20377,10 +20380,10 @@
       <c r="B205" s="156" t="s">
         <v>729</v>
       </c>
-      <c r="C205" s="771" t="s">
+      <c r="C205" s="718" t="s">
         <v>730</v>
       </c>
-      <c r="D205" s="771"/>
+      <c r="D205" s="718"/>
       <c r="E205" s="188" t="e">
         <f>SUMIF(#REF!,6,#REF!)</f>
         <v>#REF!</v>
@@ -20413,10 +20416,10 @@
       <c r="B206" s="156" t="s">
         <v>731</v>
       </c>
-      <c r="C206" s="765" t="s">
+      <c r="C206" s="712" t="s">
         <v>732</v>
       </c>
-      <c r="D206" s="766"/>
+      <c r="D206" s="713"/>
       <c r="E206" s="188" t="e">
         <f>SUMIF(#REF!,7,#REF!)</f>
         <v>#REF!</v>
@@ -20449,10 +20452,10 @@
       <c r="B207" s="156" t="s">
         <v>733</v>
       </c>
-      <c r="C207" s="765" t="s">
+      <c r="C207" s="712" t="s">
         <v>734</v>
       </c>
-      <c r="D207" s="766"/>
+      <c r="D207" s="713"/>
       <c r="E207" s="188" t="e">
         <f>SUMIF(#REF!,8,#REF!)</f>
         <v>#REF!</v>
@@ -20485,10 +20488,10 @@
       <c r="B208" s="156" t="s">
         <v>735</v>
       </c>
-      <c r="C208" s="767" t="s">
+      <c r="C208" s="714" t="s">
         <v>736</v>
       </c>
-      <c r="D208" s="768"/>
+      <c r="D208" s="715"/>
       <c r="E208" s="189" t="e">
         <f>SUMIF(#REF!,9,#REF!)</f>
         <v>#REF!</v>
@@ -20519,10 +20522,10 @@
     </row>
     <row r="209" spans="2:11" ht="21.75" thickBot="1">
       <c r="B209" s="157"/>
-      <c r="C209" s="761" t="s">
+      <c r="C209" s="705" t="s">
         <v>737</v>
       </c>
-      <c r="D209" s="762"/>
+      <c r="D209" s="706"/>
       <c r="E209" s="158" t="e">
         <f t="shared" ref="E209:J209" si="5">SUM(E200:E208)</f>
         <v>#REF!</v>
@@ -22131,17 +22134,116 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="145">
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C172:D172"/>
-    <mergeCell ref="C173:D173"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="N63:N65"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="O63:O65"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="L63:L65"/>
+    <mergeCell ref="M63:M65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C161:D161"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="C163:D163"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="B152:D152"/>
+    <mergeCell ref="B154:D154"/>
     <mergeCell ref="C209:D209"/>
     <mergeCell ref="C198:D198"/>
     <mergeCell ref="C199:D199"/>
@@ -22166,116 +22268,17 @@
     <mergeCell ref="B189:D189"/>
     <mergeCell ref="B194:D194"/>
     <mergeCell ref="C183:D183"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="C164:D164"/>
-    <mergeCell ref="C165:D165"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C161:D161"/>
-    <mergeCell ref="C162:D162"/>
-    <mergeCell ref="C163:D163"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="B136:D136"/>
-    <mergeCell ref="B138:D138"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B152:D152"/>
-    <mergeCell ref="B154:D154"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="N63:N65"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="O63:O65"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="L63:L65"/>
-    <mergeCell ref="M63:M65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
@@ -22328,7 +22331,7 @@
   <dimension ref="A1:Y44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -23336,7 +23339,7 @@
       <c r="E38" s="685">
         <v>0</v>
       </c>
-      <c r="F38" s="292">
+      <c r="F38" s="815">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -23726,12 +23729,12 @@
         <v>3</v>
       </c>
       <c r="H14" s="328"/>
-      <c r="I14" s="799">
+      <c r="I14" s="801">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J14" s="800"/>
-      <c r="K14" s="800"/>
+      <c r="J14" s="802"/>
+      <c r="K14" s="802"/>
       <c r="L14" s="346"/>
       <c r="M14" s="346"/>
       <c r="N14" s="347"/>
@@ -23775,12 +23778,12 @@
         <v>5</v>
       </c>
       <c r="H16" s="328"/>
-      <c r="I16" s="801">
+      <c r="I16" s="803">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J16" s="802"/>
-      <c r="K16" s="803"/>
+      <c r="J16" s="804"/>
+      <c r="K16" s="805"/>
       <c r="L16" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -23847,12 +23850,12 @@
         <v>8</v>
       </c>
       <c r="H19" s="328"/>
-      <c r="I19" s="804">
+      <c r="I19" s="806">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J19" s="805"/>
-      <c r="K19" s="806"/>
+      <c r="J19" s="807"/>
+      <c r="K19" s="808"/>
       <c r="L19" s="356" t="s">
         <v>934</v>
       </c>
@@ -24420,10 +24423,10 @@
       <c r="I39" s="395">
         <v>500</v>
       </c>
-      <c r="J39" s="797" t="s">
+      <c r="J39" s="814" t="s">
         <v>579</v>
       </c>
-      <c r="K39" s="797"/>
+      <c r="K39" s="814"/>
       <c r="L39" s="241">
         <f t="shared" ref="L39:Q39" si="3">SUM(L40:L46)</f>
         <v>0</v>
@@ -24692,10 +24695,10 @@
       <c r="I47" s="395">
         <v>800</v>
       </c>
-      <c r="J47" s="808" t="s">
+      <c r="J47" s="810" t="s">
         <v>698</v>
       </c>
-      <c r="K47" s="809"/>
+      <c r="K47" s="811"/>
       <c r="L47" s="567"/>
       <c r="M47" s="244">
         <f t="shared" si="4"/>
@@ -25650,7 +25653,7 @@
       <c r="J79" s="796" t="s">
         <v>606</v>
       </c>
-      <c r="K79" s="810"/>
+      <c r="K79" s="812"/>
       <c r="L79" s="567"/>
       <c r="M79" s="244">
         <f t="shared" si="10"/>
@@ -25674,7 +25677,7 @@
       <c r="I80" s="395">
         <v>2600</v>
       </c>
-      <c r="J80" s="798" t="s">
+      <c r="J80" s="813" t="s">
         <v>607</v>
       </c>
       <c r="K80" s="787"/>
@@ -25701,7 +25704,7 @@
       <c r="I81" s="395">
         <v>2700</v>
       </c>
-      <c r="J81" s="798" t="s">
+      <c r="J81" s="813" t="s">
         <v>608</v>
       </c>
       <c r="K81" s="787"/>
@@ -25728,7 +25731,7 @@
       <c r="I82" s="395">
         <v>2800</v>
       </c>
-      <c r="J82" s="798" t="s">
+      <c r="J82" s="813" t="s">
         <v>1011</v>
       </c>
       <c r="K82" s="787"/>
@@ -26672,7 +26675,7 @@
       <c r="I114" s="395">
         <v>4600</v>
       </c>
-      <c r="J114" s="798" t="s">
+      <c r="J114" s="813" t="s">
         <v>630</v>
       </c>
       <c r="K114" s="787"/>
@@ -27326,10 +27329,10 @@
       <c r="I136" s="449">
         <v>5700</v>
       </c>
-      <c r="J136" s="811" t="s">
+      <c r="J136" s="797" t="s">
         <v>943</v>
       </c>
-      <c r="K136" s="812"/>
+      <c r="K136" s="798"/>
       <c r="L136" s="243">
         <f t="shared" ref="L136:Q136" si="25">SUM(L137:L139)</f>
         <v>0</v>
@@ -27469,10 +27472,10 @@
       <c r="I141" s="464">
         <v>98</v>
       </c>
-      <c r="J141" s="813" t="s">
+      <c r="J141" s="799" t="s">
         <v>653</v>
       </c>
-      <c r="K141" s="814"/>
+      <c r="K141" s="800"/>
       <c r="L141" s="573"/>
       <c r="M141" s="324">
         <f>N141+O141+P141+Q141</f>
@@ -27668,12 +27671,12 @@
         <v>138</v>
       </c>
       <c r="H149" s="328"/>
-      <c r="I149" s="799">
+      <c r="I149" s="801">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J149" s="800"/>
-      <c r="K149" s="800"/>
+      <c r="J149" s="802"/>
+      <c r="K149" s="802"/>
       <c r="L149" s="326"/>
       <c r="M149" s="326"/>
       <c r="N149" s="326"/>
@@ -27715,12 +27718,12 @@
         <v>140</v>
       </c>
       <c r="H151" s="328"/>
-      <c r="I151" s="801">
+      <c r="I151" s="803">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J151" s="802"/>
-      <c r="K151" s="803"/>
+      <c r="J151" s="804"/>
+      <c r="K151" s="805"/>
       <c r="L151" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -27787,12 +27790,12 @@
         <v>143</v>
       </c>
       <c r="H154" s="328"/>
-      <c r="I154" s="804">
+      <c r="I154" s="806">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J154" s="805"/>
-      <c r="K154" s="806"/>
+      <c r="J154" s="807"/>
+      <c r="K154" s="808"/>
       <c r="L154" s="356" t="s">
         <v>934</v>
       </c>
@@ -28590,11 +28593,11 @@
         <v>175</v>
       </c>
       <c r="H186" s="328"/>
-      <c r="I186" s="807" t="s">
+      <c r="I186" s="809" t="s">
         <v>249</v>
       </c>
-      <c r="J186" s="807"/>
-      <c r="K186" s="807"/>
+      <c r="J186" s="809"/>
+      <c r="K186" s="809"/>
       <c r="L186" s="327"/>
       <c r="M186" s="327"/>
       <c r="N186" s="327"/>
@@ -29936,11 +29939,21 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="36">
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="I149:K149"/>
     <mergeCell ref="I151:K151"/>
     <mergeCell ref="I154:K154"/>
@@ -29957,21 +29970,11 @@
     <mergeCell ref="J99:K99"/>
     <mergeCell ref="J100:K100"/>
     <mergeCell ref="J114:K114"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J141:K141"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L156:M156">

</xml_diff>

<commit_message>
Small adjustments to the report template and README.md
</commit_message>
<xml_diff>
--- a/PaymentsBudgetSystem/wwwroot/Report.xlsx
+++ b/PaymentsBudgetSystem/wwwroot/Report.xlsx
@@ -8060,9 +8060,6 @@
     <t>50-00</t>
   </si>
   <si>
-    <t>Капиталови разходи</t>
-  </si>
-  <si>
     <t>51-00</t>
   </si>
   <si>
@@ -8130,6 +8127,9 @@
   </si>
   <si>
     <t>Отчет за дейността</t>
+  </si>
+  <si>
+    <t>Капиталови разходи - придобиване на активи</t>
   </si>
 </sst>
 </file>
@@ -13009,261 +13009,13 @@
     <xf numFmtId="3" fontId="13" fillId="12" borderId="102" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -13286,9 +13038,260 @@
     <xf numFmtId="0" fontId="45" fillId="5" borderId="114" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="117" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="11" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="116" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="115" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="107" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="114" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="110" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="111" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="108" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="109" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="112" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="113" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -13331,17 +13334,11 @@
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -13381,13 +13378,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="16" borderId="78" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -14439,12 +14439,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="42" customHeight="1">
-      <c r="B7" s="776" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="777"/>
-      <c r="D7" s="777"/>
+      <c r="B7" s="692" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C7" s="693"/>
+      <c r="D7" s="693"/>
       <c r="F7" s="38"/>
       <c r="K7" s="167">
         <v>1</v>
@@ -14464,12 +14464,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="36.75" customHeight="1" thickBot="1">
-      <c r="B9" s="778" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="779"/>
-      <c r="D9" s="779"/>
+      <c r="B9" s="694" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="695"/>
+      <c r="D9" s="695"/>
       <c r="E9" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14504,12 +14504,12 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="39" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B12" s="778" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C12" s="779"/>
-      <c r="D12" s="779"/>
+      <c r="B12" s="694" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C12" s="695"/>
+      <c r="D12" s="695"/>
       <c r="E12" s="38" t="s">
         <v>505</v>
       </c>
@@ -14584,10 +14584,10 @@
     <row r="19" spans="1:11" ht="21.75" thickBot="1">
       <c r="A19" s="46"/>
       <c r="B19" s="47"/>
-      <c r="C19" s="782" t="s">
+      <c r="C19" s="700" t="s">
         <v>508</v>
       </c>
-      <c r="D19" s="708"/>
+      <c r="D19" s="701"/>
       <c r="E19" s="48" t="s">
         <v>509</v>
       </c>
@@ -14606,10 +14606,10 @@
       <c r="B20" s="49" t="s">
         <v>474</v>
       </c>
-      <c r="C20" s="711" t="s">
+      <c r="C20" s="702" t="s">
         <v>705</v>
       </c>
-      <c r="D20" s="710"/>
+      <c r="D20" s="703"/>
       <c r="E20" s="50">
         <v>2017</v>
       </c>
@@ -14634,10 +14634,10 @@
     </row>
     <row r="21" spans="1:11" ht="21.75" thickBot="1">
       <c r="B21" s="51"/>
-      <c r="C21" s="744" t="s">
+      <c r="C21" s="704" t="s">
         <v>512</v>
       </c>
-      <c r="D21" s="741"/>
+      <c r="D21" s="705"/>
       <c r="E21" s="10" t="s">
         <v>263</v>
       </c>
@@ -14667,10 +14667,10 @@
       <c r="B22" s="54">
         <v>100</v>
       </c>
-      <c r="C22" s="780" t="s">
+      <c r="C22" s="696" t="s">
         <v>513</v>
       </c>
-      <c r="D22" s="781"/>
+      <c r="D22" s="697"/>
       <c r="E22" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14707,10 +14707,10 @@
       <c r="B23" s="57">
         <v>200</v>
       </c>
-      <c r="C23" s="699" t="s">
+      <c r="C23" s="690" t="s">
         <v>514</v>
       </c>
-      <c r="D23" s="700"/>
+      <c r="D23" s="691"/>
       <c r="E23" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14747,10 +14747,10 @@
       <c r="B24" s="57">
         <v>400</v>
       </c>
-      <c r="C24" s="697" t="s">
+      <c r="C24" s="698" t="s">
         <v>515</v>
       </c>
-      <c r="D24" s="742"/>
+      <c r="D24" s="699"/>
       <c r="E24" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14787,10 +14787,10 @@
       <c r="B25" s="57">
         <v>800</v>
       </c>
-      <c r="C25" s="699" t="s">
+      <c r="C25" s="690" t="s">
         <v>924</v>
       </c>
-      <c r="D25" s="700"/>
+      <c r="D25" s="691"/>
       <c r="E25" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14827,10 +14827,10 @@
       <c r="B26" s="57">
         <v>1000</v>
       </c>
-      <c r="C26" s="699" t="s">
+      <c r="C26" s="690" t="s">
         <v>516</v>
       </c>
-      <c r="D26" s="700"/>
+      <c r="D26" s="691"/>
       <c r="E26" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14867,10 +14867,10 @@
       <c r="B27" s="57">
         <v>1300</v>
       </c>
-      <c r="C27" s="699" t="s">
+      <c r="C27" s="690" t="s">
         <v>706</v>
       </c>
-      <c r="D27" s="700"/>
+      <c r="D27" s="691"/>
       <c r="E27" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14907,10 +14907,10 @@
       <c r="B28" s="57">
         <v>1400</v>
       </c>
-      <c r="C28" s="699" t="s">
+      <c r="C28" s="690" t="s">
         <v>517</v>
       </c>
-      <c r="D28" s="700"/>
+      <c r="D28" s="691"/>
       <c r="E28" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14947,10 +14947,10 @@
       <c r="B29" s="57">
         <v>1500</v>
       </c>
-      <c r="C29" s="699" t="s">
+      <c r="C29" s="690" t="s">
         <v>518</v>
       </c>
-      <c r="D29" s="700"/>
+      <c r="D29" s="691"/>
       <c r="E29" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -14984,10 +14984,10 @@
       <c r="B30" s="57">
         <v>1600</v>
       </c>
-      <c r="C30" s="699" t="s">
+      <c r="C30" s="690" t="s">
         <v>519</v>
       </c>
-      <c r="D30" s="700"/>
+      <c r="D30" s="691"/>
       <c r="E30" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15024,10 +15024,10 @@
       <c r="B31" s="57">
         <v>1700</v>
       </c>
-      <c r="C31" s="699" t="s">
+      <c r="C31" s="690" t="s">
         <v>520</v>
       </c>
-      <c r="D31" s="700"/>
+      <c r="D31" s="691"/>
       <c r="E31" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15064,10 +15064,10 @@
       <c r="B32" s="57">
         <v>1800</v>
       </c>
-      <c r="C32" s="699" t="s">
+      <c r="C32" s="690" t="s">
         <v>521</v>
       </c>
-      <c r="D32" s="700"/>
+      <c r="D32" s="691"/>
       <c r="E32" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15104,10 +15104,10 @@
       <c r="B33" s="57">
         <v>1900</v>
       </c>
-      <c r="C33" s="699" t="s">
+      <c r="C33" s="690" t="s">
         <v>522</v>
       </c>
-      <c r="D33" s="700"/>
+      <c r="D33" s="691"/>
       <c r="E33" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15144,10 +15144,10 @@
       <c r="B34" s="57">
         <v>2000</v>
       </c>
-      <c r="C34" s="699" t="s">
+      <c r="C34" s="690" t="s">
         <v>523</v>
       </c>
-      <c r="D34" s="700"/>
+      <c r="D34" s="691"/>
       <c r="E34" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15184,10 +15184,10 @@
       <c r="B35" s="57">
         <v>2400</v>
       </c>
-      <c r="C35" s="699" t="s">
+      <c r="C35" s="690" t="s">
         <v>524</v>
       </c>
-      <c r="D35" s="700"/>
+      <c r="D35" s="691"/>
       <c r="E35" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15224,10 +15224,10 @@
       <c r="B36" s="62">
         <v>2500</v>
       </c>
-      <c r="C36" s="695" t="s">
+      <c r="C36" s="710" t="s">
         <v>525</v>
       </c>
-      <c r="D36" s="696"/>
+      <c r="D36" s="711"/>
       <c r="E36" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15264,10 +15264,10 @@
       <c r="B37" s="57">
         <v>2600</v>
       </c>
-      <c r="C37" s="695" t="s">
+      <c r="C37" s="710" t="s">
         <v>300</v>
       </c>
-      <c r="D37" s="696"/>
+      <c r="D37" s="711"/>
       <c r="E37" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15304,10 +15304,10 @@
       <c r="B38" s="57">
         <v>2700</v>
       </c>
-      <c r="C38" s="699" t="s">
+      <c r="C38" s="690" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="700"/>
+      <c r="D38" s="691"/>
       <c r="E38" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15344,10 +15344,10 @@
       <c r="B39" s="57">
         <v>2800</v>
       </c>
-      <c r="C39" s="699" t="s">
+      <c r="C39" s="690" t="s">
         <v>529</v>
       </c>
-      <c r="D39" s="700"/>
+      <c r="D39" s="691"/>
       <c r="E39" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15384,10 +15384,10 @@
       <c r="B40" s="57">
         <v>3600</v>
       </c>
-      <c r="C40" s="699" t="s">
+      <c r="C40" s="690" t="s">
         <v>530</v>
       </c>
-      <c r="D40" s="700"/>
+      <c r="D40" s="691"/>
       <c r="E40" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15424,10 +15424,10 @@
       <c r="B41" s="57">
         <v>3700</v>
       </c>
-      <c r="C41" s="699" t="s">
+      <c r="C41" s="690" t="s">
         <v>531</v>
       </c>
-      <c r="D41" s="700"/>
+      <c r="D41" s="691"/>
       <c r="E41" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15518,10 +15518,10 @@
       <c r="B43" s="57">
         <v>4100</v>
       </c>
-      <c r="C43" s="699" t="s">
+      <c r="C43" s="690" t="s">
         <v>381</v>
       </c>
-      <c r="D43" s="700"/>
+      <c r="D43" s="691"/>
       <c r="E43" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15559,10 +15559,10 @@
       <c r="B44" s="57">
         <v>4200</v>
       </c>
-      <c r="C44" s="699" t="s">
+      <c r="C44" s="690" t="s">
         <v>382</v>
       </c>
-      <c r="D44" s="700"/>
+      <c r="D44" s="691"/>
       <c r="E44" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15600,10 +15600,10 @@
       <c r="B45" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="C45" s="699" t="s">
+      <c r="C45" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="700"/>
+      <c r="D45" s="691"/>
       <c r="E45" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15641,10 +15641,10 @@
       <c r="B46" s="57">
         <v>4600</v>
       </c>
-      <c r="C46" s="699" t="s">
+      <c r="C46" s="690" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="700"/>
+      <c r="D46" s="691"/>
       <c r="E46" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15681,10 +15681,10 @@
       <c r="B47" s="57">
         <v>4700</v>
       </c>
-      <c r="C47" s="699" t="s">
+      <c r="C47" s="690" t="s">
         <v>1410</v>
       </c>
-      <c r="D47" s="700"/>
+      <c r="D47" s="691"/>
       <c r="E47" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15721,10 +15721,10 @@
       <c r="B48" s="57">
         <v>4800</v>
       </c>
-      <c r="C48" s="774" t="s">
+      <c r="C48" s="706" t="s">
         <v>455</v>
       </c>
-      <c r="D48" s="775"/>
+      <c r="D48" s="707"/>
       <c r="E48" s="202" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -15853,12 +15853,12 @@
       <c r="L53" s="74"/>
     </row>
     <row r="54" spans="1:15" s="46" customFormat="1" ht="44.25" customHeight="1">
-      <c r="B54" s="729" t="e">
+      <c r="B54" s="708" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C54" s="730"/>
-      <c r="D54" s="730"/>
+      <c r="C54" s="709"/>
+      <c r="D54" s="709"/>
       <c r="E54" s="79"/>
       <c r="F54" s="79"/>
       <c r="G54" s="30"/>
@@ -15890,12 +15890,12 @@
       <c r="L55" s="74"/>
     </row>
     <row r="56" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickBot="1">
-      <c r="B56" s="691" t="e">
+      <c r="B56" s="724" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C56" s="692"/>
-      <c r="D56" s="692"/>
+      <c r="C56" s="725"/>
+      <c r="D56" s="725"/>
       <c r="E56" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -15950,12 +15950,12 @@
       <c r="L58" s="74"/>
     </row>
     <row r="59" spans="1:15" s="46" customFormat="1" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B59" s="691" t="e">
+      <c r="B59" s="724" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C59" s="692"/>
-      <c r="D59" s="692"/>
+      <c r="C59" s="725"/>
+      <c r="D59" s="725"/>
       <c r="E59" s="79" t="s">
         <v>505</v>
       </c>
@@ -16026,10 +16026,10 @@
     </row>
     <row r="63" spans="1:15" s="46" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="B63" s="87"/>
-      <c r="C63" s="770" t="s">
+      <c r="C63" s="720" t="s">
         <v>473</v>
       </c>
-      <c r="D63" s="771"/>
+      <c r="D63" s="721"/>
       <c r="E63" s="48" t="s">
         <v>509</v>
       </c>
@@ -16043,16 +16043,16 @@
       <c r="K63" s="169">
         <v>1</v>
       </c>
-      <c r="L63" s="764" t="s">
+      <c r="L63" s="712" t="s">
         <v>1429</v>
       </c>
-      <c r="M63" s="764" t="s">
+      <c r="M63" s="712" t="s">
         <v>1430</v>
       </c>
-      <c r="N63" s="764" t="s">
+      <c r="N63" s="712" t="s">
         <v>1431</v>
       </c>
-      <c r="O63" s="764" t="s">
+      <c r="O63" s="712" t="s">
         <v>1432</v>
       </c>
     </row>
@@ -16060,10 +16060,10 @@
       <c r="B64" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="C64" s="711" t="s">
+      <c r="C64" s="702" t="s">
         <v>707</v>
       </c>
-      <c r="D64" s="767"/>
+      <c r="D64" s="717"/>
       <c r="E64" s="50">
         <v>2017</v>
       </c>
@@ -16085,17 +16085,17 @@
       <c r="K64" s="169">
         <v>1</v>
       </c>
-      <c r="L64" s="772"/>
-      <c r="M64" s="772"/>
-      <c r="N64" s="765"/>
-      <c r="O64" s="765"/>
+      <c r="L64" s="726"/>
+      <c r="M64" s="726"/>
+      <c r="N64" s="713"/>
+      <c r="O64" s="713"/>
     </row>
     <row r="65" spans="1:15" s="46" customFormat="1" ht="21.75" thickBot="1">
       <c r="B65" s="88"/>
-      <c r="C65" s="768" t="s">
+      <c r="C65" s="718" t="s">
         <v>387</v>
       </c>
-      <c r="D65" s="769"/>
+      <c r="D65" s="719"/>
       <c r="E65" s="10" t="s">
         <v>263</v>
       </c>
@@ -16117,10 +16117,10 @@
       <c r="K65" s="169">
         <v>1</v>
       </c>
-      <c r="L65" s="773"/>
-      <c r="M65" s="773"/>
-      <c r="N65" s="766"/>
-      <c r="O65" s="766"/>
+      <c r="L65" s="727"/>
+      <c r="M65" s="727"/>
+      <c r="N65" s="714"/>
+      <c r="O65" s="714"/>
     </row>
     <row r="66" spans="1:15" s="56" customFormat="1" ht="34.5" customHeight="1">
       <c r="A66" s="63">
@@ -16129,10 +16129,10 @@
       <c r="B66" s="54">
         <v>100</v>
       </c>
-      <c r="C66" s="752" t="s">
+      <c r="C66" s="728" t="s">
         <v>388</v>
       </c>
-      <c r="D66" s="732"/>
+      <c r="D66" s="729"/>
       <c r="E66" s="171" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16173,10 +16173,10 @@
       <c r="B67" s="57">
         <v>200</v>
       </c>
-      <c r="C67" s="695" t="s">
+      <c r="C67" s="710" t="s">
         <v>391</v>
       </c>
-      <c r="D67" s="696"/>
+      <c r="D67" s="711"/>
       <c r="E67" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16217,10 +16217,10 @@
       <c r="B68" s="57">
         <v>500</v>
       </c>
-      <c r="C68" s="699" t="s">
+      <c r="C68" s="690" t="s">
         <v>579</v>
       </c>
-      <c r="D68" s="700"/>
+      <c r="D68" s="691"/>
       <c r="E68" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16261,10 +16261,10 @@
       <c r="B69" s="57">
         <v>800</v>
       </c>
-      <c r="C69" s="697" t="s">
+      <c r="C69" s="698" t="s">
         <v>585</v>
       </c>
-      <c r="D69" s="698"/>
+      <c r="D69" s="730"/>
       <c r="E69" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16305,10 +16305,10 @@
       <c r="B70" s="57">
         <v>1000</v>
       </c>
-      <c r="C70" s="695" t="s">
+      <c r="C70" s="710" t="s">
         <v>586</v>
       </c>
-      <c r="D70" s="696"/>
+      <c r="D70" s="711"/>
       <c r="E70" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16349,10 +16349,10 @@
       <c r="B71" s="57">
         <v>1900</v>
       </c>
-      <c r="C71" s="693" t="s">
+      <c r="C71" s="722" t="s">
         <v>456</v>
       </c>
-      <c r="D71" s="694"/>
+      <c r="D71" s="723"/>
       <c r="E71" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16393,10 +16393,10 @@
       <c r="B72" s="57">
         <v>2100</v>
       </c>
-      <c r="C72" s="693" t="s">
+      <c r="C72" s="722" t="s">
         <v>741</v>
       </c>
-      <c r="D72" s="694"/>
+      <c r="D72" s="723"/>
       <c r="E72" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16437,10 +16437,10 @@
       <c r="B73" s="57">
         <v>2200</v>
       </c>
-      <c r="C73" s="693" t="s">
+      <c r="C73" s="722" t="s">
         <v>604</v>
       </c>
-      <c r="D73" s="694"/>
+      <c r="D73" s="723"/>
       <c r="E73" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16481,10 +16481,10 @@
       <c r="B74" s="57">
         <v>2500</v>
       </c>
-      <c r="C74" s="693" t="s">
+      <c r="C74" s="722" t="s">
         <v>606</v>
       </c>
-      <c r="D74" s="694"/>
+      <c r="D74" s="723"/>
       <c r="E74" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16525,10 +16525,10 @@
       <c r="B75" s="57">
         <v>2600</v>
       </c>
-      <c r="C75" s="701" t="s">
+      <c r="C75" s="715" t="s">
         <v>607</v>
       </c>
-      <c r="D75" s="702"/>
+      <c r="D75" s="716"/>
       <c r="E75" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16569,10 +16569,10 @@
       <c r="B76" s="57">
         <v>2700</v>
       </c>
-      <c r="C76" s="701" t="s">
+      <c r="C76" s="715" t="s">
         <v>608</v>
       </c>
-      <c r="D76" s="702"/>
+      <c r="D76" s="716"/>
       <c r="E76" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16613,10 +16613,10 @@
       <c r="B77" s="57">
         <v>2800</v>
       </c>
-      <c r="C77" s="701" t="s">
+      <c r="C77" s="715" t="s">
         <v>1408</v>
       </c>
-      <c r="D77" s="702"/>
+      <c r="D77" s="716"/>
       <c r="E77" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16657,10 +16657,10 @@
       <c r="B78" s="57">
         <v>2900</v>
       </c>
-      <c r="C78" s="693" t="s">
+      <c r="C78" s="722" t="s">
         <v>609</v>
       </c>
-      <c r="D78" s="694"/>
+      <c r="D78" s="723"/>
       <c r="E78" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16745,10 +16745,10 @@
       <c r="B80" s="57">
         <v>3900</v>
       </c>
-      <c r="C80" s="693" t="s">
+      <c r="C80" s="722" t="s">
         <v>618</v>
       </c>
-      <c r="D80" s="694"/>
+      <c r="D80" s="723"/>
       <c r="E80" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16789,10 +16789,10 @@
       <c r="B81" s="57">
         <v>4000</v>
       </c>
-      <c r="C81" s="693" t="s">
+      <c r="C81" s="722" t="s">
         <v>619</v>
       </c>
-      <c r="D81" s="694"/>
+      <c r="D81" s="723"/>
       <c r="E81" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16833,10 +16833,10 @@
       <c r="B82" s="57">
         <v>4100</v>
       </c>
-      <c r="C82" s="693" t="s">
+      <c r="C82" s="722" t="s">
         <v>620</v>
       </c>
-      <c r="D82" s="694"/>
+      <c r="D82" s="723"/>
       <c r="E82" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16877,10 +16877,10 @@
       <c r="B83" s="57">
         <v>4200</v>
       </c>
-      <c r="C83" s="693" t="s">
+      <c r="C83" s="722" t="s">
         <v>621</v>
       </c>
-      <c r="D83" s="694"/>
+      <c r="D83" s="723"/>
       <c r="E83" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16921,10 +16921,10 @@
       <c r="B84" s="57">
         <v>4300</v>
       </c>
-      <c r="C84" s="693" t="s">
+      <c r="C84" s="722" t="s">
         <v>1015</v>
       </c>
-      <c r="D84" s="694"/>
+      <c r="D84" s="723"/>
       <c r="E84" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -16965,10 +16965,10 @@
       <c r="B85" s="57">
         <v>4400</v>
       </c>
-      <c r="C85" s="693" t="s">
+      <c r="C85" s="722" t="s">
         <v>1012</v>
       </c>
-      <c r="D85" s="694"/>
+      <c r="D85" s="723"/>
       <c r="E85" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17009,10 +17009,10 @@
       <c r="B86" s="57">
         <v>4500</v>
       </c>
-      <c r="C86" s="693" t="s">
+      <c r="C86" s="722" t="s">
         <v>1409</v>
       </c>
-      <c r="D86" s="694"/>
+      <c r="D86" s="723"/>
       <c r="E86" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17053,10 +17053,10 @@
       <c r="B87" s="57">
         <v>4600</v>
       </c>
-      <c r="C87" s="701" t="s">
+      <c r="C87" s="715" t="s">
         <v>630</v>
       </c>
-      <c r="D87" s="702"/>
+      <c r="D87" s="716"/>
       <c r="E87" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17097,10 +17097,10 @@
       <c r="B88" s="57">
         <v>4900</v>
       </c>
-      <c r="C88" s="693" t="s">
+      <c r="C88" s="722" t="s">
         <v>460</v>
       </c>
-      <c r="D88" s="694"/>
+      <c r="D88" s="723"/>
       <c r="E88" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17141,10 +17141,10 @@
       <c r="B89" s="96">
         <v>5100</v>
       </c>
-      <c r="C89" s="757" t="s">
+      <c r="C89" s="731" t="s">
         <v>631</v>
       </c>
-      <c r="D89" s="758"/>
+      <c r="D89" s="732"/>
       <c r="E89" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17185,10 +17185,10 @@
       <c r="B90" s="96">
         <v>5200</v>
       </c>
-      <c r="C90" s="757" t="s">
+      <c r="C90" s="731" t="s">
         <v>632</v>
       </c>
-      <c r="D90" s="758"/>
+      <c r="D90" s="732"/>
       <c r="E90" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17229,10 +17229,10 @@
       <c r="B91" s="96">
         <v>5300</v>
       </c>
-      <c r="C91" s="757" t="s">
+      <c r="C91" s="731" t="s">
         <v>191</v>
       </c>
-      <c r="D91" s="758"/>
+      <c r="D91" s="732"/>
       <c r="E91" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17273,10 +17273,10 @@
       <c r="B92" s="96">
         <v>5400</v>
       </c>
-      <c r="C92" s="757" t="s">
+      <c r="C92" s="731" t="s">
         <v>643</v>
       </c>
-      <c r="D92" s="758"/>
+      <c r="D92" s="732"/>
       <c r="E92" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17317,10 +17317,10 @@
       <c r="B93" s="57">
         <v>5500</v>
       </c>
-      <c r="C93" s="693" t="s">
+      <c r="C93" s="722" t="s">
         <v>644</v>
       </c>
-      <c r="D93" s="694"/>
+      <c r="D93" s="723"/>
       <c r="E93" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17361,10 +17361,10 @@
       <c r="B94" s="96">
         <v>5700</v>
       </c>
-      <c r="C94" s="759" t="s">
+      <c r="C94" s="733" t="s">
         <v>649</v>
       </c>
-      <c r="D94" s="760"/>
+      <c r="D94" s="734"/>
       <c r="E94" s="172" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17405,10 +17405,10 @@
       <c r="B95" s="98" t="s">
         <v>708</v>
       </c>
-      <c r="C95" s="761" t="s">
+      <c r="C95" s="735" t="s">
         <v>653</v>
       </c>
-      <c r="D95" s="762"/>
+      <c r="D95" s="736"/>
       <c r="E95" s="176" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17447,10 +17447,10 @@
         <v>825</v>
       </c>
       <c r="B96" s="104"/>
-      <c r="C96" s="763" t="s">
+      <c r="C96" s="737" t="s">
         <v>654</v>
       </c>
-      <c r="D96" s="763"/>
+      <c r="D96" s="737"/>
       <c r="E96" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17516,12 +17516,12 @@
     </row>
     <row r="99" spans="1:11" ht="40.5" customHeight="1">
       <c r="A99" s="70"/>
-      <c r="B99" s="729" t="e">
+      <c r="B99" s="708" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C99" s="730"/>
-      <c r="D99" s="730"/>
+      <c r="C99" s="709"/>
+      <c r="D99" s="709"/>
       <c r="E99" s="79"/>
       <c r="F99" s="79"/>
       <c r="K99" s="167">
@@ -17544,12 +17544,12 @@
     </row>
     <row r="101" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A101" s="70"/>
-      <c r="B101" s="691" t="e">
+      <c r="B101" s="724" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C101" s="692"/>
-      <c r="D101" s="692"/>
+      <c r="C101" s="725"/>
+      <c r="D101" s="725"/>
       <c r="E101" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -17588,12 +17588,12 @@
     </row>
     <row r="104" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A104" s="70"/>
-      <c r="B104" s="691" t="e">
+      <c r="B104" s="724" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C104" s="692"/>
-      <c r="D104" s="692"/>
+      <c r="C104" s="725"/>
+      <c r="D104" s="725"/>
       <c r="E104" s="79" t="s">
         <v>505</v>
       </c>
@@ -17643,10 +17643,10 @@
     <row r="108" spans="1:11" ht="21.75" thickBot="1">
       <c r="A108" s="70"/>
       <c r="B108" s="138"/>
-      <c r="C108" s="743" t="s">
+      <c r="C108" s="747" t="s">
         <v>908</v>
       </c>
-      <c r="D108" s="753"/>
+      <c r="D108" s="748"/>
       <c r="E108" s="48" t="s">
         <v>509</v>
       </c>
@@ -17666,10 +17666,10 @@
       <c r="B109" s="107" t="s">
         <v>474</v>
       </c>
-      <c r="C109" s="754" t="s">
+      <c r="C109" s="749" t="s">
         <v>707</v>
       </c>
-      <c r="D109" s="755"/>
+      <c r="D109" s="750"/>
       <c r="E109" s="50">
         <v>2017</v>
       </c>
@@ -17697,10 +17697,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="740" t="s">
+      <c r="C110" s="751" t="s">
         <v>251</v>
       </c>
-      <c r="D110" s="741"/>
+      <c r="D110" s="705"/>
       <c r="E110" s="10" t="s">
         <v>263</v>
       </c>
@@ -17728,10 +17728,10 @@
         <v>2</v>
       </c>
       <c r="B111" s="14"/>
-      <c r="C111" s="756" t="s">
+      <c r="C111" s="752" t="s">
         <v>463</v>
       </c>
-      <c r="D111" s="741"/>
+      <c r="D111" s="705"/>
       <c r="E111" s="12"/>
       <c r="F111" s="29"/>
       <c r="G111" s="29"/>
@@ -17749,10 +17749,10 @@
       <c r="B112" s="54">
         <v>3000</v>
       </c>
-      <c r="C112" s="736" t="s">
+      <c r="C112" s="753" t="s">
         <v>909</v>
       </c>
-      <c r="D112" s="737"/>
+      <c r="D112" s="754"/>
       <c r="E112" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17789,10 +17789,10 @@
       <c r="B113" s="57">
         <v>3100</v>
       </c>
-      <c r="C113" s="699" t="s">
+      <c r="C113" s="690" t="s">
         <v>464</v>
       </c>
-      <c r="D113" s="700"/>
+      <c r="D113" s="691"/>
       <c r="E113" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17829,10 +17829,10 @@
       <c r="B114" s="110">
         <v>3200</v>
       </c>
-      <c r="C114" s="745" t="s">
+      <c r="C114" s="738" t="s">
         <v>758</v>
       </c>
-      <c r="D114" s="690"/>
+      <c r="D114" s="739"/>
       <c r="E114" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17869,10 +17869,10 @@
       <c r="B115" s="57">
         <v>6000</v>
       </c>
-      <c r="C115" s="752" t="s">
+      <c r="C115" s="728" t="s">
         <v>635</v>
       </c>
-      <c r="D115" s="732"/>
+      <c r="D115" s="729"/>
       <c r="E115" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17909,10 +17909,10 @@
       <c r="B116" s="57">
         <v>6100</v>
       </c>
-      <c r="C116" s="695" t="s">
+      <c r="C116" s="710" t="s">
         <v>636</v>
       </c>
-      <c r="D116" s="696"/>
+      <c r="D116" s="711"/>
       <c r="E116" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17949,10 +17949,10 @@
       <c r="B117" s="57">
         <v>6200</v>
       </c>
-      <c r="C117" s="728" t="s">
+      <c r="C117" s="756" t="s">
         <v>637</v>
       </c>
-      <c r="D117" s="733"/>
+      <c r="D117" s="757"/>
       <c r="E117" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -17989,10 +17989,10 @@
       <c r="B118" s="57">
         <v>6300</v>
       </c>
-      <c r="C118" s="725" t="s">
+      <c r="C118" s="744" t="s">
         <v>638</v>
       </c>
-      <c r="D118" s="702"/>
+      <c r="D118" s="716"/>
       <c r="E118" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18029,10 +18029,10 @@
       <c r="B119" s="57">
         <v>6400</v>
       </c>
-      <c r="C119" s="748" t="s">
+      <c r="C119" s="742" t="s">
         <v>639</v>
       </c>
-      <c r="D119" s="749"/>
+      <c r="D119" s="743"/>
       <c r="E119" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18127,10 +18127,10 @@
       <c r="B121" s="57">
         <v>6600</v>
       </c>
-      <c r="C121" s="725" t="s">
+      <c r="C121" s="744" t="s">
         <v>254</v>
       </c>
-      <c r="D121" s="702"/>
+      <c r="D121" s="716"/>
       <c r="E121" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18167,10 +18167,10 @@
       <c r="B122" s="57">
         <v>6700</v>
       </c>
-      <c r="C122" s="725" t="s">
+      <c r="C122" s="744" t="s">
         <v>687</v>
       </c>
-      <c r="D122" s="702"/>
+      <c r="D122" s="716"/>
       <c r="E122" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18207,10 +18207,10 @@
       <c r="B123" s="57">
         <v>6900</v>
       </c>
-      <c r="C123" s="750" t="s">
+      <c r="C123" s="745" t="s">
         <v>640</v>
       </c>
-      <c r="D123" s="751"/>
+      <c r="D123" s="746"/>
       <c r="E123" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18245,10 +18245,10 @@
         <v>260</v>
       </c>
       <c r="B124" s="71"/>
-      <c r="C124" s="738" t="s">
+      <c r="C124" s="760" t="s">
         <v>252</v>
       </c>
-      <c r="D124" s="739"/>
+      <c r="D124" s="761"/>
       <c r="E124" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18282,10 +18282,10 @@
         <v>261</v>
       </c>
       <c r="B125" s="112"/>
-      <c r="C125" s="740" t="s">
+      <c r="C125" s="751" t="s">
         <v>253</v>
       </c>
-      <c r="D125" s="741"/>
+      <c r="D125" s="705"/>
       <c r="E125" s="113"/>
       <c r="F125" s="170"/>
       <c r="G125" s="170"/>
@@ -18303,10 +18303,10 @@
       <c r="B126" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C126" s="734" t="s">
+      <c r="C126" s="758" t="s">
         <v>899</v>
       </c>
-      <c r="D126" s="735"/>
+      <c r="D126" s="759"/>
       <c r="E126" s="170"/>
       <c r="F126" s="170"/>
       <c r="G126" s="170"/>
@@ -18324,10 +18324,10 @@
       <c r="B127" s="57">
         <v>7400</v>
       </c>
-      <c r="C127" s="736" t="s">
+      <c r="C127" s="753" t="s">
         <v>900</v>
       </c>
-      <c r="D127" s="737"/>
+      <c r="D127" s="754"/>
       <c r="E127" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18364,10 +18364,10 @@
       <c r="B128" s="57">
         <v>7500</v>
       </c>
-      <c r="C128" s="699" t="s">
+      <c r="C128" s="690" t="s">
         <v>710</v>
       </c>
-      <c r="D128" s="700"/>
+      <c r="D128" s="691"/>
       <c r="E128" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18404,10 +18404,10 @@
       <c r="B129" s="57">
         <v>7600</v>
       </c>
-      <c r="C129" s="697" t="s">
+      <c r="C129" s="698" t="s">
         <v>641</v>
       </c>
-      <c r="D129" s="742"/>
+      <c r="D129" s="699"/>
       <c r="E129" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18444,10 +18444,10 @@
       <c r="B130" s="57">
         <v>7700</v>
       </c>
-      <c r="C130" s="697" t="s">
+      <c r="C130" s="698" t="s">
         <v>642</v>
       </c>
-      <c r="D130" s="698"/>
+      <c r="D130" s="730"/>
       <c r="E130" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18484,10 +18484,10 @@
       <c r="B131" s="96">
         <v>7800</v>
       </c>
-      <c r="C131" s="746" t="s">
-        <v>0</v>
-      </c>
-      <c r="D131" s="747"/>
+      <c r="C131" s="740" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="741"/>
       <c r="E131" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18522,10 +18522,10 @@
         <v>315</v>
       </c>
       <c r="B132" s="71"/>
-      <c r="C132" s="738" t="s">
+      <c r="C132" s="760" t="s">
         <v>898</v>
       </c>
-      <c r="D132" s="739"/>
+      <c r="D132" s="761"/>
       <c r="E132" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -18583,12 +18583,12 @@
     </row>
     <row r="136" spans="1:11" ht="42" customHeight="1">
       <c r="A136" s="103"/>
-      <c r="B136" s="729" t="e">
+      <c r="B136" s="708" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C136" s="730"/>
-      <c r="D136" s="730"/>
+      <c r="C136" s="709"/>
+      <c r="D136" s="709"/>
       <c r="E136" s="79"/>
       <c r="F136" s="79"/>
       <c r="K136" s="167">
@@ -18611,12 +18611,12 @@
     </row>
     <row r="138" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A138" s="103"/>
-      <c r="B138" s="691" t="e">
+      <c r="B138" s="724" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C138" s="692"/>
-      <c r="D138" s="692"/>
+      <c r="C138" s="725"/>
+      <c r="D138" s="725"/>
       <c r="E138" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18655,12 +18655,12 @@
     </row>
     <row r="141" spans="1:11" ht="39.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A141" s="103"/>
-      <c r="B141" s="691" t="e">
+      <c r="B141" s="724" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C141" s="692"/>
-      <c r="D141" s="692"/>
+      <c r="C141" s="725"/>
+      <c r="D141" s="725"/>
       <c r="E141" s="79" t="s">
         <v>505</v>
       </c>
@@ -18850,12 +18850,12 @@
     </row>
     <row r="152" spans="1:11" ht="44.25" customHeight="1">
       <c r="A152" s="103"/>
-      <c r="B152" s="729" t="e">
+      <c r="B152" s="708" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C152" s="730"/>
-      <c r="D152" s="730"/>
+      <c r="C152" s="709"/>
+      <c r="D152" s="709"/>
       <c r="E152" s="79"/>
       <c r="F152" s="79"/>
       <c r="K152" s="167">
@@ -18878,12 +18878,12 @@
     </row>
     <row r="154" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A154" s="103"/>
-      <c r="B154" s="691" t="e">
+      <c r="B154" s="724" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C154" s="692"/>
-      <c r="D154" s="692"/>
+      <c r="C154" s="725"/>
+      <c r="D154" s="725"/>
       <c r="E154" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -18922,12 +18922,12 @@
     </row>
     <row r="157" spans="1:11" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A157" s="103"/>
-      <c r="B157" s="691" t="e">
+      <c r="B157" s="724" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C157" s="692"/>
-      <c r="D157" s="692"/>
+      <c r="C157" s="725"/>
+      <c r="D157" s="725"/>
       <c r="E157" s="79" t="s">
         <v>505</v>
       </c>
@@ -18977,10 +18977,10 @@
     <row r="161" spans="1:65" ht="21.75" thickBot="1">
       <c r="A161" s="103"/>
       <c r="B161" s="112"/>
-      <c r="C161" s="743" t="s">
+      <c r="C161" s="747" t="s">
         <v>684</v>
       </c>
-      <c r="D161" s="710"/>
+      <c r="D161" s="703"/>
       <c r="E161" s="48" t="s">
         <v>509</v>
       </c>
@@ -19000,10 +19000,10 @@
       <c r="B162" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="C162" s="711" t="s">
+      <c r="C162" s="702" t="s">
         <v>707</v>
       </c>
-      <c r="D162" s="708"/>
+      <c r="D162" s="701"/>
       <c r="E162" s="50">
         <v>2017</v>
       </c>
@@ -19031,10 +19031,10 @@
         <v>1</v>
       </c>
       <c r="B163" s="139"/>
-      <c r="C163" s="744" t="s">
+      <c r="C163" s="704" t="s">
         <v>685</v>
       </c>
-      <c r="D163" s="741"/>
+      <c r="D163" s="705"/>
       <c r="E163" s="10" t="s">
         <v>263</v>
       </c>
@@ -19064,10 +19064,10 @@
       <c r="B164" s="54">
         <v>7000</v>
       </c>
-      <c r="C164" s="731" t="s">
+      <c r="C164" s="755" t="s">
         <v>902</v>
       </c>
-      <c r="D164" s="732"/>
+      <c r="D164" s="729"/>
       <c r="E164" s="177" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19104,10 +19104,10 @@
       <c r="B165" s="57">
         <v>7100</v>
       </c>
-      <c r="C165" s="693" t="s">
+      <c r="C165" s="722" t="s">
         <v>903</v>
       </c>
-      <c r="D165" s="694"/>
+      <c r="D165" s="723"/>
       <c r="E165" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19144,10 +19144,10 @@
       <c r="B166" s="57">
         <v>7200</v>
       </c>
-      <c r="C166" s="693" t="s">
+      <c r="C166" s="722" t="s">
         <v>1414</v>
       </c>
-      <c r="D166" s="694"/>
+      <c r="D166" s="723"/>
       <c r="E166" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19184,10 +19184,10 @@
       <c r="B167" s="57">
         <v>7300</v>
       </c>
-      <c r="C167" s="701" t="s">
+      <c r="C167" s="715" t="s">
         <v>904</v>
       </c>
-      <c r="D167" s="702"/>
+      <c r="D167" s="716"/>
       <c r="E167" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19224,10 +19224,10 @@
       <c r="B168" s="57">
         <v>7900</v>
       </c>
-      <c r="C168" s="703" t="s">
+      <c r="C168" s="782" t="s">
         <v>905</v>
       </c>
-      <c r="D168" s="704"/>
+      <c r="D168" s="783"/>
       <c r="E168" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19317,10 +19317,10 @@
       <c r="B169" s="57">
         <v>8000</v>
       </c>
-      <c r="C169" s="695" t="s">
+      <c r="C169" s="710" t="s">
         <v>711</v>
       </c>
-      <c r="D169" s="696"/>
+      <c r="D169" s="711"/>
       <c r="E169" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19357,10 +19357,10 @@
       <c r="B170" s="57">
         <v>8100</v>
       </c>
-      <c r="C170" s="697" t="s">
+      <c r="C170" s="698" t="s">
         <v>712</v>
       </c>
-      <c r="D170" s="698"/>
+      <c r="D170" s="730"/>
       <c r="E170" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19397,10 +19397,10 @@
       <c r="B171" s="57">
         <v>8200</v>
       </c>
-      <c r="C171" s="697" t="s">
+      <c r="C171" s="698" t="s">
         <v>101</v>
       </c>
-      <c r="D171" s="698"/>
+      <c r="D171" s="730"/>
       <c r="E171" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19437,10 +19437,10 @@
       <c r="B172" s="57">
         <v>8300</v>
       </c>
-      <c r="C172" s="699" t="s">
+      <c r="C172" s="690" t="s">
         <v>713</v>
       </c>
-      <c r="D172" s="700"/>
+      <c r="D172" s="691"/>
       <c r="E172" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19477,10 +19477,10 @@
       <c r="B173" s="57">
         <v>8500</v>
       </c>
-      <c r="C173" s="695" t="s">
+      <c r="C173" s="710" t="s">
         <v>102</v>
       </c>
-      <c r="D173" s="696"/>
+      <c r="D173" s="711"/>
       <c r="E173" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19517,10 +19517,10 @@
       <c r="B174" s="57">
         <v>8600</v>
       </c>
-      <c r="C174" s="695" t="s">
+      <c r="C174" s="710" t="s">
         <v>103</v>
       </c>
-      <c r="D174" s="696"/>
+      <c r="D174" s="711"/>
       <c r="E174" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19557,10 +19557,10 @@
       <c r="B175" s="57">
         <v>8700</v>
       </c>
-      <c r="C175" s="697" t="s">
+      <c r="C175" s="698" t="s">
         <v>265</v>
       </c>
-      <c r="D175" s="698"/>
+      <c r="D175" s="730"/>
       <c r="E175" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19597,10 +19597,10 @@
       <c r="B176" s="57">
         <v>8800</v>
       </c>
-      <c r="C176" s="697" t="s">
+      <c r="C176" s="698" t="s">
         <v>910</v>
       </c>
-      <c r="D176" s="698"/>
+      <c r="D176" s="730"/>
       <c r="E176" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19637,10 +19637,10 @@
       <c r="B177" s="57">
         <v>8900</v>
       </c>
-      <c r="C177" s="725" t="s">
+      <c r="C177" s="744" t="s">
         <v>759</v>
       </c>
-      <c r="D177" s="702"/>
+      <c r="D177" s="716"/>
       <c r="E177" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19677,10 +19677,10 @@
       <c r="B178" s="57">
         <v>9000</v>
       </c>
-      <c r="C178" s="695" t="s">
+      <c r="C178" s="710" t="s">
         <v>104</v>
       </c>
-      <c r="D178" s="696"/>
+      <c r="D178" s="711"/>
       <c r="E178" s="185" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19717,10 +19717,10 @@
       <c r="B179" s="57">
         <v>9100</v>
       </c>
-      <c r="C179" s="725" t="s">
+      <c r="C179" s="744" t="s">
         <v>911</v>
       </c>
-      <c r="D179" s="728"/>
+      <c r="D179" s="756"/>
       <c r="E179" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19757,10 +19757,10 @@
       <c r="B180" s="57">
         <v>9200</v>
       </c>
-      <c r="C180" s="726" t="s">
+      <c r="C180" s="779" t="s">
         <v>714</v>
       </c>
-      <c r="D180" s="698"/>
+      <c r="D180" s="730"/>
       <c r="E180" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19797,10 +19797,10 @@
       <c r="B181" s="57">
         <v>9300</v>
       </c>
-      <c r="C181" s="695" t="s">
+      <c r="C181" s="710" t="s">
         <v>715</v>
       </c>
-      <c r="D181" s="696"/>
+      <c r="D181" s="711"/>
       <c r="E181" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19837,10 +19837,10 @@
       <c r="B182" s="57">
         <v>9500</v>
       </c>
-      <c r="C182" s="726" t="s">
+      <c r="C182" s="779" t="s">
         <v>716</v>
       </c>
-      <c r="D182" s="727"/>
+      <c r="D182" s="780"/>
       <c r="E182" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19877,10 +19877,10 @@
       <c r="B183" s="57">
         <v>9600</v>
       </c>
-      <c r="C183" s="726" t="s">
+      <c r="C183" s="779" t="s">
         <v>717</v>
       </c>
-      <c r="D183" s="698"/>
+      <c r="D183" s="730"/>
       <c r="E183" s="179" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19917,10 +19917,10 @@
       <c r="B184" s="57">
         <v>9800</v>
       </c>
-      <c r="C184" s="689" t="s">
+      <c r="C184" s="781" t="s">
         <v>465</v>
       </c>
-      <c r="D184" s="690"/>
+      <c r="D184" s="739"/>
       <c r="E184" s="181" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -19955,10 +19955,10 @@
         <v>610</v>
       </c>
       <c r="B185" s="146"/>
-      <c r="C185" s="711" t="s">
+      <c r="C185" s="702" t="s">
         <v>930</v>
       </c>
-      <c r="D185" s="708"/>
+      <c r="D185" s="701"/>
       <c r="E185" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -20021,12 +20021,12 @@
       </c>
     </row>
     <row r="189" spans="1:11" ht="42" customHeight="1">
-      <c r="B189" s="729" t="e">
+      <c r="B189" s="708" t="e">
         <f>$B$7</f>
         <v>#REF!</v>
       </c>
-      <c r="C189" s="730"/>
-      <c r="D189" s="730"/>
+      <c r="C189" s="709"/>
+      <c r="D189" s="709"/>
       <c r="E189" s="79"/>
       <c r="F189" s="79"/>
       <c r="G189" s="56"/>
@@ -20049,12 +20049,12 @@
       </c>
     </row>
     <row r="191" spans="1:11" ht="21.75" thickBot="1">
-      <c r="B191" s="691" t="e">
+      <c r="B191" s="724" t="e">
         <f>$B$9</f>
         <v>#REF!</v>
       </c>
-      <c r="C191" s="692"/>
-      <c r="D191" s="692"/>
+      <c r="C191" s="725"/>
+      <c r="D191" s="725"/>
       <c r="E191" s="82" t="e">
         <f>$E$9</f>
         <v>#REF!</v>
@@ -20093,12 +20093,12 @@
       </c>
     </row>
     <row r="194" spans="2:11" ht="22.5" thickTop="1" thickBot="1">
-      <c r="B194" s="691" t="e">
+      <c r="B194" s="724" t="e">
         <f>$B$12</f>
         <v>#REF!</v>
       </c>
-      <c r="C194" s="692"/>
-      <c r="D194" s="692"/>
+      <c r="C194" s="725"/>
+      <c r="D194" s="725"/>
       <c r="E194" s="79" t="s">
         <v>505</v>
       </c>
@@ -20152,10 +20152,10 @@
       <c r="B198" s="153" t="s">
         <v>474</v>
       </c>
-      <c r="C198" s="707" t="s">
+      <c r="C198" s="764" t="s">
         <v>718</v>
       </c>
-      <c r="D198" s="708"/>
+      <c r="D198" s="701"/>
       <c r="E198" s="48" t="s">
         <v>509</v>
       </c>
@@ -20172,8 +20172,8 @@
     </row>
     <row r="199" spans="2:11" ht="45.75" thickBot="1">
       <c r="B199" s="154"/>
-      <c r="C199" s="709"/>
-      <c r="D199" s="710"/>
+      <c r="C199" s="765"/>
+      <c r="D199" s="703"/>
       <c r="E199" s="50">
         <v>2017</v>
       </c>
@@ -20200,10 +20200,10 @@
       <c r="B200" s="155" t="s">
         <v>719</v>
       </c>
-      <c r="C200" s="723" t="s">
+      <c r="C200" s="777" t="s">
         <v>720</v>
       </c>
-      <c r="D200" s="724"/>
+      <c r="D200" s="778"/>
       <c r="E200" s="187" t="e">
         <f>SUMIF(#REF!,1,#REF!)</f>
         <v>#REF!</v>
@@ -20236,10 +20236,10 @@
       <c r="B201" s="156" t="s">
         <v>721</v>
       </c>
-      <c r="C201" s="716" t="s">
+      <c r="C201" s="770" t="s">
         <v>722</v>
       </c>
-      <c r="D201" s="717"/>
+      <c r="D201" s="771"/>
       <c r="E201" s="188" t="e">
         <f>SUMIF(#REF!,2,#REF!)</f>
         <v>#REF!</v>
@@ -20272,10 +20272,10 @@
       <c r="B202" s="156" t="s">
         <v>723</v>
       </c>
-      <c r="C202" s="716" t="s">
+      <c r="C202" s="770" t="s">
         <v>724</v>
       </c>
-      <c r="D202" s="717"/>
+      <c r="D202" s="771"/>
       <c r="E202" s="188" t="e">
         <f>SUMIF(#REF!,3,#REF!)</f>
         <v>#REF!</v>
@@ -20308,10 +20308,10 @@
       <c r="B203" s="156" t="s">
         <v>725</v>
       </c>
-      <c r="C203" s="719" t="s">
+      <c r="C203" s="773" t="s">
         <v>726</v>
       </c>
-      <c r="D203" s="720"/>
+      <c r="D203" s="774"/>
       <c r="E203" s="188" t="e">
         <f>SUMIF(#REF!,4,#REF!)</f>
         <v>#REF!</v>
@@ -20344,10 +20344,10 @@
       <c r="B204" s="156" t="s">
         <v>727</v>
       </c>
-      <c r="C204" s="721" t="s">
+      <c r="C204" s="775" t="s">
         <v>728</v>
       </c>
-      <c r="D204" s="722"/>
+      <c r="D204" s="776"/>
       <c r="E204" s="188" t="e">
         <f>SUMIF(#REF!,5,#REF!)</f>
         <v>#REF!</v>
@@ -20380,10 +20380,10 @@
       <c r="B205" s="156" t="s">
         <v>729</v>
       </c>
-      <c r="C205" s="718" t="s">
+      <c r="C205" s="772" t="s">
         <v>730</v>
       </c>
-      <c r="D205" s="718"/>
+      <c r="D205" s="772"/>
       <c r="E205" s="188" t="e">
         <f>SUMIF(#REF!,6,#REF!)</f>
         <v>#REF!</v>
@@ -20416,10 +20416,10 @@
       <c r="B206" s="156" t="s">
         <v>731</v>
       </c>
-      <c r="C206" s="712" t="s">
+      <c r="C206" s="766" t="s">
         <v>732</v>
       </c>
-      <c r="D206" s="713"/>
+      <c r="D206" s="767"/>
       <c r="E206" s="188" t="e">
         <f>SUMIF(#REF!,7,#REF!)</f>
         <v>#REF!</v>
@@ -20452,10 +20452,10 @@
       <c r="B207" s="156" t="s">
         <v>733</v>
       </c>
-      <c r="C207" s="712" t="s">
+      <c r="C207" s="766" t="s">
         <v>734</v>
       </c>
-      <c r="D207" s="713"/>
+      <c r="D207" s="767"/>
       <c r="E207" s="188" t="e">
         <f>SUMIF(#REF!,8,#REF!)</f>
         <v>#REF!</v>
@@ -20488,10 +20488,10 @@
       <c r="B208" s="156" t="s">
         <v>735</v>
       </c>
-      <c r="C208" s="714" t="s">
+      <c r="C208" s="768" t="s">
         <v>736</v>
       </c>
-      <c r="D208" s="715"/>
+      <c r="D208" s="769"/>
       <c r="E208" s="189" t="e">
         <f>SUMIF(#REF!,9,#REF!)</f>
         <v>#REF!</v>
@@ -20522,10 +20522,10 @@
     </row>
     <row r="209" spans="2:11" ht="21.75" thickBot="1">
       <c r="B209" s="157"/>
-      <c r="C209" s="705" t="s">
+      <c r="C209" s="762" t="s">
         <v>737</v>
       </c>
-      <c r="D209" s="706"/>
+      <c r="D209" s="763"/>
       <c r="E209" s="158" t="e">
         <f t="shared" ref="E209:J209" si="5">SUM(E200:E208)</f>
         <v>#REF!</v>
@@ -22134,116 +22134,17 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="145">
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="N63:N65"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="O63:O65"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="L63:L65"/>
-    <mergeCell ref="M63:M65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="C164:D164"/>
-    <mergeCell ref="C165:D165"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C161:D161"/>
-    <mergeCell ref="C162:D162"/>
-    <mergeCell ref="C163:D163"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="B136:D136"/>
-    <mergeCell ref="B138:D138"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B152:D152"/>
-    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
     <mergeCell ref="C209:D209"/>
     <mergeCell ref="C198:D198"/>
     <mergeCell ref="C199:D199"/>
@@ -22268,17 +22169,116 @@
     <mergeCell ref="B189:D189"/>
     <mergeCell ref="B194:D194"/>
     <mergeCell ref="C183:D183"/>
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C172:D172"/>
-    <mergeCell ref="C173:D173"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C161:D161"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="C163:D163"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="B152:D152"/>
+    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="N63:N65"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="O63:O65"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="L63:L65"/>
+    <mergeCell ref="M63:M65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
@@ -22331,7 +22331,7 @@
   <dimension ref="A1:Y44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -22481,12 +22481,12 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="209"/>
-      <c r="B7" s="783" t="str">
+      <c r="B7" s="784" t="str">
         <f>VLOOKUP(E8,SMETKA,2,FALSE)</f>
         <v>ОТЧЕТНИ ДАННИ ПО ЕБК ЗА ИЗПЪЛНЕНИЕТО НА БЮДЖЕТА</v>
       </c>
-      <c r="C7" s="784"/>
-      <c r="D7" s="784"/>
+      <c r="C7" s="785"/>
+      <c r="D7" s="785"/>
       <c r="E7" s="337"/>
       <c r="F7" s="337"/>
       <c r="G7" s="337"/>
@@ -22585,11 +22585,11 @@
     </row>
     <row r="13" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="210"/>
-      <c r="B13" s="789" t="s">
-        <v>1510</v>
-      </c>
-      <c r="C13" s="790"/>
-      <c r="D13" s="791"/>
+      <c r="B13" s="790" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C13" s="791"/>
+      <c r="D13" s="792"/>
       <c r="E13" s="338"/>
       <c r="F13" s="353"/>
       <c r="G13" s="326"/>
@@ -22635,9 +22635,9 @@
     </row>
     <row r="16" spans="1:12" s="226" customFormat="1" ht="27" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="792"/>
-      <c r="C16" s="793"/>
-      <c r="D16" s="794"/>
+      <c r="B16" s="793"/>
+      <c r="C16" s="794"/>
+      <c r="D16" s="795"/>
       <c r="E16" s="356"/>
       <c r="F16" s="587"/>
       <c r="G16" s="326"/>
@@ -22651,11 +22651,11 @@
     </row>
     <row r="17" spans="1:25" s="226" customFormat="1">
       <c r="A17" s="210"/>
-      <c r="B17" s="795" t="s">
-        <v>1509</v>
-      </c>
-      <c r="C17" s="795"/>
-      <c r="D17" s="795"/>
+      <c r="B17" s="796" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C17" s="796"/>
+      <c r="D17" s="796"/>
       <c r="E17" s="540"/>
       <c r="F17" s="541"/>
       <c r="G17" s="355"/>
@@ -22815,10 +22815,10 @@
       <c r="B24" s="395">
         <v>100</v>
       </c>
-      <c r="C24" s="786" t="s">
+      <c r="C24" s="787" t="s">
         <v>388</v>
       </c>
-      <c r="D24" s="787"/>
+      <c r="D24" s="788"/>
       <c r="E24" s="241">
         <f>SUMIF($B$43:$B$44,$B24,E$43:E$44)</f>
         <v>0</v>
@@ -22961,7 +22961,7 @@
         <v>551</v>
       </c>
       <c r="D27" s="409" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="E27" s="285">
         <v>0</v>
@@ -22994,7 +22994,7 @@
         <v>560</v>
       </c>
       <c r="D28" s="413" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="E28" s="287">
         <v>0</v>
@@ -23027,7 +23027,7 @@
         <v>580</v>
       </c>
       <c r="D29" s="411" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="E29" s="287">
         <v>0</v>
@@ -23058,7 +23058,7 @@
         <v>590</v>
       </c>
       <c r="D30" s="411" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="E30" s="287">
         <v>0</v>
@@ -23086,10 +23086,10 @@
       <c r="B31" s="395">
         <v>1000</v>
       </c>
-      <c r="C31" s="788" t="s">
+      <c r="C31" s="789" t="s">
         <v>586</v>
       </c>
-      <c r="D31" s="788"/>
+      <c r="D31" s="789"/>
       <c r="E31" s="243">
         <v>0</v>
       </c>
@@ -23233,10 +23233,10 @@
       <c r="B35" s="449" t="s">
         <v>1498</v>
       </c>
-      <c r="C35" s="785" t="s">
-        <v>1499</v>
-      </c>
-      <c r="D35" s="785"/>
+      <c r="C35" s="786" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D35" s="786"/>
       <c r="E35" s="243">
         <v>0</v>
       </c>
@@ -23265,10 +23265,10 @@
       </c>
       <c r="B36" s="402"/>
       <c r="C36" s="403" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="D36" s="404" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="E36" s="287">
         <v>0</v>
@@ -23298,10 +23298,10 @@
       </c>
       <c r="B37" s="396"/>
       <c r="C37" s="419" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D37" s="420" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="E37" s="296">
         <v>0</v>
@@ -23331,7 +23331,7 @@
       </c>
       <c r="B38" s="402"/>
       <c r="C38" s="683" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D38" s="684" t="s">
         <v>191</v>
@@ -23339,7 +23339,7 @@
       <c r="E38" s="685">
         <v>0</v>
       </c>
-      <c r="F38" s="815">
+      <c r="F38" s="689">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -23729,12 +23729,12 @@
         <v>3</v>
       </c>
       <c r="H14" s="328"/>
-      <c r="I14" s="801">
+      <c r="I14" s="800">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J14" s="802"/>
-      <c r="K14" s="802"/>
+      <c r="J14" s="801"/>
+      <c r="K14" s="801"/>
       <c r="L14" s="346"/>
       <c r="M14" s="346"/>
       <c r="N14" s="347"/>
@@ -23778,12 +23778,12 @@
         <v>5</v>
       </c>
       <c r="H16" s="328"/>
-      <c r="I16" s="803">
+      <c r="I16" s="802">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J16" s="804"/>
-      <c r="K16" s="805"/>
+      <c r="J16" s="803"/>
+      <c r="K16" s="804"/>
       <c r="L16" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -23850,12 +23850,12 @@
         <v>8</v>
       </c>
       <c r="H19" s="328"/>
-      <c r="I19" s="806">
+      <c r="I19" s="805">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J19" s="807"/>
-      <c r="K19" s="808"/>
+      <c r="J19" s="806"/>
+      <c r="K19" s="807"/>
       <c r="L19" s="356" t="s">
         <v>934</v>
       </c>
@@ -24150,10 +24150,10 @@
       <c r="I30" s="395">
         <v>100</v>
       </c>
-      <c r="J30" s="786" t="s">
+      <c r="J30" s="787" t="s">
         <v>388</v>
       </c>
-      <c r="K30" s="787"/>
+      <c r="K30" s="788"/>
       <c r="L30" s="241">
         <f t="shared" ref="L30:Q30" si="0">SUM(L31:L32)</f>
         <v>0</v>
@@ -24246,10 +24246,10 @@
       <c r="I33" s="395">
         <v>200</v>
       </c>
-      <c r="J33" s="788" t="s">
+      <c r="J33" s="789" t="s">
         <v>391</v>
       </c>
-      <c r="K33" s="788"/>
+      <c r="K33" s="789"/>
       <c r="L33" s="241">
         <f t="shared" ref="L33:Q33" si="2">SUM(L34:L38)</f>
         <v>0</v>
@@ -24423,10 +24423,10 @@
       <c r="I39" s="395">
         <v>500</v>
       </c>
-      <c r="J39" s="814" t="s">
+      <c r="J39" s="798" t="s">
         <v>579</v>
       </c>
-      <c r="K39" s="814"/>
+      <c r="K39" s="798"/>
       <c r="L39" s="241">
         <f t="shared" ref="L39:Q39" si="3">SUM(L40:L46)</f>
         <v>0</v>
@@ -24695,10 +24695,10 @@
       <c r="I47" s="395">
         <v>800</v>
       </c>
-      <c r="J47" s="810" t="s">
+      <c r="J47" s="809" t="s">
         <v>698</v>
       </c>
-      <c r="K47" s="811"/>
+      <c r="K47" s="810"/>
       <c r="L47" s="567"/>
       <c r="M47" s="244">
         <f t="shared" si="4"/>
@@ -24722,10 +24722,10 @@
       <c r="I48" s="395">
         <v>1000</v>
       </c>
-      <c r="J48" s="788" t="s">
+      <c r="J48" s="789" t="s">
         <v>586</v>
       </c>
-      <c r="K48" s="788"/>
+      <c r="K48" s="789"/>
       <c r="L48" s="243">
         <f t="shared" ref="L48:Q48" si="5">SUM(L49:L65)</f>
         <v>0</v>
@@ -25241,10 +25241,10 @@
       <c r="I66" s="395">
         <v>1900</v>
       </c>
-      <c r="J66" s="796" t="s">
+      <c r="J66" s="797" t="s">
         <v>456</v>
       </c>
-      <c r="K66" s="796"/>
+      <c r="K66" s="797"/>
       <c r="L66" s="243">
         <f t="shared" ref="L66:Q66" si="7">SUM(L67:L69)</f>
         <v>0</v>
@@ -25368,10 +25368,10 @@
       <c r="I70" s="395">
         <v>2100</v>
       </c>
-      <c r="J70" s="796" t="s">
+      <c r="J70" s="797" t="s">
         <v>741</v>
       </c>
-      <c r="K70" s="796"/>
+      <c r="K70" s="797"/>
       <c r="L70" s="243">
         <f t="shared" ref="L70:Q70" si="8">SUM(L71:L75)</f>
         <v>0</v>
@@ -25554,10 +25554,10 @@
       <c r="I76" s="395">
         <v>2200</v>
       </c>
-      <c r="J76" s="796" t="s">
+      <c r="J76" s="797" t="s">
         <v>604</v>
       </c>
-      <c r="K76" s="796"/>
+      <c r="K76" s="797"/>
       <c r="L76" s="243">
         <f t="shared" ref="L76:Q76" si="9">SUM(L77:L78)</f>
         <v>0</v>
@@ -25650,10 +25650,10 @@
       <c r="I79" s="395">
         <v>2500</v>
       </c>
-      <c r="J79" s="796" t="s">
+      <c r="J79" s="797" t="s">
         <v>606</v>
       </c>
-      <c r="K79" s="812"/>
+      <c r="K79" s="811"/>
       <c r="L79" s="567"/>
       <c r="M79" s="244">
         <f t="shared" si="10"/>
@@ -25677,10 +25677,10 @@
       <c r="I80" s="395">
         <v>2600</v>
       </c>
-      <c r="J80" s="813" t="s">
+      <c r="J80" s="799" t="s">
         <v>607</v>
       </c>
-      <c r="K80" s="787"/>
+      <c r="K80" s="788"/>
       <c r="L80" s="567"/>
       <c r="M80" s="244">
         <f t="shared" si="10"/>
@@ -25704,10 +25704,10 @@
       <c r="I81" s="395">
         <v>2700</v>
       </c>
-      <c r="J81" s="813" t="s">
+      <c r="J81" s="799" t="s">
         <v>608</v>
       </c>
-      <c r="K81" s="787"/>
+      <c r="K81" s="788"/>
       <c r="L81" s="567"/>
       <c r="M81" s="244">
         <f t="shared" si="10"/>
@@ -25731,10 +25731,10 @@
       <c r="I82" s="395">
         <v>2800</v>
       </c>
-      <c r="J82" s="813" t="s">
+      <c r="J82" s="799" t="s">
         <v>1011</v>
       </c>
-      <c r="K82" s="787"/>
+      <c r="K82" s="788"/>
       <c r="L82" s="567"/>
       <c r="M82" s="244">
         <f t="shared" si="10"/>
@@ -25758,10 +25758,10 @@
       <c r="I83" s="395">
         <v>2900</v>
       </c>
-      <c r="J83" s="796" t="s">
+      <c r="J83" s="797" t="s">
         <v>609</v>
       </c>
-      <c r="K83" s="796"/>
+      <c r="K83" s="797"/>
       <c r="L83" s="243">
         <f t="shared" ref="L83:Q83" si="11">SUM(L84:L91)</f>
         <v>0</v>
@@ -26213,10 +26213,10 @@
       <c r="I98" s="395">
         <v>3900</v>
       </c>
-      <c r="J98" s="796" t="s">
+      <c r="J98" s="797" t="s">
         <v>618</v>
       </c>
-      <c r="K98" s="796"/>
+      <c r="K98" s="797"/>
       <c r="L98" s="567"/>
       <c r="M98" s="244">
         <f t="shared" si="14"/>
@@ -26240,10 +26240,10 @@
       <c r="I99" s="395">
         <v>4000</v>
       </c>
-      <c r="J99" s="796" t="s">
+      <c r="J99" s="797" t="s">
         <v>619</v>
       </c>
-      <c r="K99" s="796"/>
+      <c r="K99" s="797"/>
       <c r="L99" s="567"/>
       <c r="M99" s="244">
         <f t="shared" si="14"/>
@@ -26267,10 +26267,10 @@
       <c r="I100" s="395">
         <v>4100</v>
       </c>
-      <c r="J100" s="796" t="s">
+      <c r="J100" s="797" t="s">
         <v>620</v>
       </c>
-      <c r="K100" s="796"/>
+      <c r="K100" s="797"/>
       <c r="L100" s="567"/>
       <c r="M100" s="244">
         <f t="shared" si="14"/>
@@ -26294,10 +26294,10 @@
       <c r="I101" s="395">
         <v>4200</v>
       </c>
-      <c r="J101" s="796" t="s">
+      <c r="J101" s="797" t="s">
         <v>621</v>
       </c>
-      <c r="K101" s="796"/>
+      <c r="K101" s="797"/>
       <c r="L101" s="243">
         <f t="shared" ref="L101:Q101" si="16">SUM(L102:L107)</f>
         <v>0</v>
@@ -26498,10 +26498,10 @@
       <c r="I108" s="395">
         <v>4300</v>
       </c>
-      <c r="J108" s="796" t="s">
+      <c r="J108" s="797" t="s">
         <v>1015</v>
       </c>
-      <c r="K108" s="796"/>
+      <c r="K108" s="797"/>
       <c r="L108" s="243">
         <f t="shared" ref="L108:Q108" si="18">SUM(L109:L111)</f>
         <v>0</v>
@@ -26621,10 +26621,10 @@
       <c r="I112" s="395">
         <v>4400</v>
       </c>
-      <c r="J112" s="796" t="s">
+      <c r="J112" s="797" t="s">
         <v>1012</v>
       </c>
-      <c r="K112" s="796"/>
+      <c r="K112" s="797"/>
       <c r="L112" s="567"/>
       <c r="M112" s="244">
         <f t="shared" si="19"/>
@@ -26648,10 +26648,10 @@
       <c r="I113" s="395">
         <v>4500</v>
       </c>
-      <c r="J113" s="796" t="s">
+      <c r="J113" s="797" t="s">
         <v>1013</v>
       </c>
-      <c r="K113" s="796"/>
+      <c r="K113" s="797"/>
       <c r="L113" s="567"/>
       <c r="M113" s="244">
         <f t="shared" si="19"/>
@@ -26675,10 +26675,10 @@
       <c r="I114" s="395">
         <v>4600</v>
       </c>
-      <c r="J114" s="813" t="s">
+      <c r="J114" s="799" t="s">
         <v>630</v>
       </c>
-      <c r="K114" s="787"/>
+      <c r="K114" s="788"/>
       <c r="L114" s="567"/>
       <c r="M114" s="244">
         <f t="shared" si="19"/>
@@ -26702,10 +26702,10 @@
       <c r="I115" s="395">
         <v>4900</v>
       </c>
-      <c r="J115" s="796" t="s">
+      <c r="J115" s="797" t="s">
         <v>460</v>
       </c>
-      <c r="K115" s="796"/>
+      <c r="K115" s="797"/>
       <c r="L115" s="243">
         <f t="shared" ref="L115:Q115" si="20">+L116+L117</f>
         <v>0</v>
@@ -26798,10 +26798,10 @@
       <c r="I118" s="449">
         <v>5100</v>
       </c>
-      <c r="J118" s="785" t="s">
+      <c r="J118" s="786" t="s">
         <v>631</v>
       </c>
-      <c r="K118" s="785"/>
+      <c r="K118" s="786"/>
       <c r="L118" s="567"/>
       <c r="M118" s="244">
         <f>N118+O118+P118+Q118</f>
@@ -26825,10 +26825,10 @@
       <c r="I119" s="449">
         <v>5200</v>
       </c>
-      <c r="J119" s="785" t="s">
+      <c r="J119" s="786" t="s">
         <v>632</v>
       </c>
-      <c r="K119" s="785"/>
+      <c r="K119" s="786"/>
       <c r="L119" s="243">
         <f t="shared" ref="L119:Q119" si="21">SUM(L120:L126)</f>
         <v>0</v>
@@ -27056,10 +27056,10 @@
       <c r="I127" s="449">
         <v>5300</v>
       </c>
-      <c r="J127" s="785" t="s">
+      <c r="J127" s="786" t="s">
         <v>191</v>
       </c>
-      <c r="K127" s="785"/>
+      <c r="K127" s="786"/>
       <c r="L127" s="243">
         <f t="shared" ref="L127:Q127" si="23">SUM(L128:L129)</f>
         <v>0</v>
@@ -27152,10 +27152,10 @@
       <c r="I130" s="449">
         <v>5400</v>
       </c>
-      <c r="J130" s="785" t="s">
+      <c r="J130" s="786" t="s">
         <v>643</v>
       </c>
-      <c r="K130" s="785"/>
+      <c r="K130" s="786"/>
       <c r="L130" s="567"/>
       <c r="M130" s="244">
         <f>N130+O130+P130+Q130</f>
@@ -27179,10 +27179,10 @@
       <c r="I131" s="395">
         <v>5500</v>
       </c>
-      <c r="J131" s="796" t="s">
+      <c r="J131" s="797" t="s">
         <v>644</v>
       </c>
-      <c r="K131" s="796"/>
+      <c r="K131" s="797"/>
       <c r="L131" s="243">
         <f t="shared" ref="L131:Q131" si="24">SUM(L132:L135)</f>
         <v>0</v>
@@ -27329,10 +27329,10 @@
       <c r="I136" s="449">
         <v>5700</v>
       </c>
-      <c r="J136" s="797" t="s">
+      <c r="J136" s="812" t="s">
         <v>943</v>
       </c>
-      <c r="K136" s="798"/>
+      <c r="K136" s="813"/>
       <c r="L136" s="243">
         <f t="shared" ref="L136:Q136" si="25">SUM(L137:L139)</f>
         <v>0</v>
@@ -27472,10 +27472,10 @@
       <c r="I141" s="464">
         <v>98</v>
       </c>
-      <c r="J141" s="799" t="s">
+      <c r="J141" s="814" t="s">
         <v>653</v>
       </c>
-      <c r="K141" s="800"/>
+      <c r="K141" s="815"/>
       <c r="L141" s="573"/>
       <c r="M141" s="324">
         <f>N141+O141+P141+Q141</f>
@@ -27671,12 +27671,12 @@
         <v>138</v>
       </c>
       <c r="H149" s="328"/>
-      <c r="I149" s="801">
+      <c r="I149" s="800">
         <f>$B$7</f>
         <v>0</v>
       </c>
-      <c r="J149" s="802"/>
-      <c r="K149" s="802"/>
+      <c r="J149" s="801"/>
+      <c r="K149" s="801"/>
       <c r="L149" s="326"/>
       <c r="M149" s="326"/>
       <c r="N149" s="326"/>
@@ -27718,12 +27718,12 @@
         <v>140</v>
       </c>
       <c r="H151" s="328"/>
-      <c r="I151" s="803">
+      <c r="I151" s="802">
         <f>$B$9</f>
         <v>0</v>
       </c>
-      <c r="J151" s="804"/>
-      <c r="K151" s="805"/>
+      <c r="J151" s="803"/>
+      <c r="K151" s="804"/>
       <c r="L151" s="338">
         <f>$E$9</f>
         <v>0</v>
@@ -27790,12 +27790,12 @@
         <v>143</v>
       </c>
       <c r="H154" s="328"/>
-      <c r="I154" s="806">
+      <c r="I154" s="805">
         <f>$B$12</f>
         <v>0</v>
       </c>
-      <c r="J154" s="807"/>
-      <c r="K154" s="808"/>
+      <c r="J154" s="806"/>
+      <c r="K154" s="807"/>
       <c r="L154" s="356" t="s">
         <v>934</v>
       </c>
@@ -28593,11 +28593,11 @@
         <v>175</v>
       </c>
       <c r="H186" s="328"/>
-      <c r="I186" s="809" t="s">
+      <c r="I186" s="808" t="s">
         <v>249</v>
       </c>
-      <c r="J186" s="809"/>
-      <c r="K186" s="809"/>
+      <c r="J186" s="808"/>
+      <c r="K186" s="808"/>
       <c r="L186" s="327"/>
       <c r="M186" s="327"/>
       <c r="N186" s="327"/>
@@ -29939,21 +29939,11 @@
   </sheetData>
   <sheetProtection password="81B0" sheet="1"/>
   <mergeCells count="36">
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J141:K141"/>
     <mergeCell ref="I149:K149"/>
     <mergeCell ref="I151:K151"/>
     <mergeCell ref="I154:K154"/>
@@ -29970,11 +29960,21 @@
     <mergeCell ref="J99:K99"/>
     <mergeCell ref="J100:K100"/>
     <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L156:M156">

</xml_diff>